<commit_message>
Add card-level output to DR spreadsheets
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
-    <sheet name="Parcel Detail" sheetId="2" r:id="rId1"/>
+    <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
+    <sheet name="Card Detail" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>PIN</t>
   </si>
@@ -180,6 +181,36 @@
   </si>
   <si>
     <t>Run ID (condo):</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Contains only PINs with multiple cards</t>
+  </si>
+  <si>
+    <t>Card % Total (By Sqft)</t>
+  </si>
+  <si>
+    <t>Card Initial FMV</t>
+  </si>
+  <si>
+    <t>Card Final FMV</t>
+  </si>
+  <si>
+    <t># Beds</t>
+  </si>
+  <si>
+    <t>Ext. Wall</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
+    <t>Total        Bld. S. F.</t>
+  </si>
+  <si>
+    <t>Townhome Complex/Condo Building ID</t>
   </si>
 </sst>
 </file>
@@ -736,7 +767,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF1048576"/>
+  <dimension ref="A1:BG1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
@@ -751,39 +782,39 @@
     <col min="2" max="2" width="12.125" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="13.875" customWidth="1"/>
-    <col min="5" max="5" width="14.375" customWidth="1"/>
-    <col min="6" max="6" width="8.875" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
-    <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="10" customWidth="1"/>
-    <col min="12" max="12" width="10.875" style="10" customWidth="1"/>
-    <col min="13" max="13" width="10.625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.625" style="17" customWidth="1"/>
-    <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
-    <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
-    <col min="19" max="19" width="11" style="10"/>
-    <col min="20" max="20" width="10.875" style="10" customWidth="1"/>
-    <col min="21" max="21" width="11.125" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
-    <col min="23" max="23" width="11" style="12"/>
-    <col min="24" max="24" width="11" style="11"/>
-    <col min="25" max="25" width="10.375" customWidth="1"/>
-    <col min="26" max="26" width="13" style="10" customWidth="1"/>
-    <col min="27" max="28" width="13" style="18" customWidth="1"/>
-    <col min="29" max="29" width="13" style="10" customWidth="1"/>
-    <col min="30" max="30" width="13" style="18" customWidth="1"/>
-    <col min="34" max="34" width="11" style="13"/>
-    <col min="43" max="43" width="14" customWidth="1"/>
-    <col min="44" max="44" width="12.375" customWidth="1"/>
-    <col min="45" max="45" width="11.875" customWidth="1"/>
-    <col min="46" max="46" width="10.875" customWidth="1"/>
-    <col min="47" max="47" width="11.5" customWidth="1"/>
-    <col min="48" max="48" width="11" customWidth="1"/>
+    <col min="5" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="8.875" customWidth="1"/>
+    <col min="8" max="8" width="15.375" customWidth="1"/>
+    <col min="9" max="9" width="13.875" style="11" customWidth="1"/>
+    <col min="10" max="11" width="11.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" style="10" customWidth="1"/>
+    <col min="13" max="13" width="10.875" style="10" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="9.125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="13.625" style="17" customWidth="1"/>
+    <col min="17" max="18" width="11.625" style="10" customWidth="1"/>
+    <col min="19" max="19" width="13.625" style="10" customWidth="1"/>
+    <col min="20" max="20" width="11" style="10"/>
+    <col min="21" max="21" width="10.875" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.125" style="10" customWidth="1"/>
+    <col min="23" max="23" width="11.625" style="11" customWidth="1"/>
+    <col min="24" max="24" width="11" style="12"/>
+    <col min="25" max="25" width="11" style="11"/>
+    <col min="26" max="26" width="10.375" customWidth="1"/>
+    <col min="27" max="27" width="13" style="10" customWidth="1"/>
+    <col min="28" max="29" width="13" style="18" customWidth="1"/>
+    <col min="30" max="30" width="13" style="10" customWidth="1"/>
+    <col min="31" max="31" width="13" style="18" customWidth="1"/>
+    <col min="35" max="35" width="11" style="13"/>
+    <col min="44" max="44" width="14" customWidth="1"/>
+    <col min="45" max="45" width="12.375" customWidth="1"/>
+    <col min="46" max="46" width="11.875" customWidth="1"/>
+    <col min="47" max="47" width="10.875" customWidth="1"/>
+    <col min="48" max="48" width="11.5" customWidth="1"/>
+    <col min="49" max="49" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:59" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -842,8 +873,9 @@
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
-    </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="BG1" s="5"/>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -852,7 +884,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2"/>
+      <c r="I2" s="1"/>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -868,14 +900,15 @@
       <c r="V2"/>
       <c r="W2"/>
       <c r="X2"/>
-      <c r="Z2"/>
+      <c r="Y2"/>
       <c r="AA2"/>
       <c r="AB2"/>
       <c r="AC2"/>
       <c r="AD2"/>
-      <c r="AH2"/>
-    </row>
-    <row r="3" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE2"/>
+      <c r="AI2"/>
+    </row>
+    <row r="3" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>47</v>
       </c>
@@ -889,7 +922,7 @@
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
-      <c r="L3"/>
+      <c r="L3" s="16"/>
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
@@ -902,14 +935,15 @@
       <c r="V3"/>
       <c r="W3"/>
       <c r="X3"/>
-      <c r="Z3"/>
+      <c r="Y3"/>
       <c r="AA3"/>
       <c r="AB3"/>
       <c r="AC3"/>
       <c r="AD3"/>
-      <c r="AH3"/>
-    </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="AE3"/>
+      <c r="AI3"/>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>48</v>
       </c>
@@ -920,7 +954,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4"/>
+      <c r="I4" s="1"/>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -936,16 +970,16 @@
       <c r="V4"/>
       <c r="W4"/>
       <c r="X4"/>
-      <c r="Z4"/>
+      <c r="Y4"/>
       <c r="AA4"/>
       <c r="AB4"/>
       <c r="AC4"/>
       <c r="AD4"/>
-      <c r="AH4"/>
-    </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="AE4"/>
+      <c r="AI4"/>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
@@ -962,41 +996,41 @@
       <c r="V5"/>
       <c r="W5"/>
       <c r="X5"/>
-      <c r="Z5"/>
+      <c r="Y5"/>
       <c r="AA5"/>
       <c r="AB5"/>
       <c r="AC5"/>
       <c r="AD5"/>
-      <c r="AH5"/>
-    </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="H6"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20"/>
+      <c r="AE5"/>
+      <c r="AI5"/>
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="I6"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="24"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="23"/>
       <c r="Q6" s="24"/>
       <c r="R6" s="24"/>
       <c r="S6" s="24"/>
       <c r="T6" s="24"/>
       <c r="U6" s="24"/>
-      <c r="V6" s="25"/>
-      <c r="W6"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="25"/>
       <c r="X6"/>
-      <c r="Z6"/>
+      <c r="Y6"/>
       <c r="AA6"/>
       <c r="AB6"/>
       <c r="AC6"/>
       <c r="AD6"/>
-      <c r="AH6"/>
-      <c r="AI6" s="22" t="s">
+      <c r="AE6"/>
+      <c r="AI6"/>
+      <c r="AJ6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="AJ6" s="22"/>
       <c r="AK6" s="22"/>
       <c r="AL6" s="22"/>
       <c r="AM6" s="22"/>
@@ -1010,8 +1044,9 @@
       <c r="AU6" s="22"/>
       <c r="AV6" s="22"/>
       <c r="AW6" s="22"/>
-    </row>
-    <row r="7" spans="1:58" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="AX6" s="22"/>
+    </row>
+    <row r="7" spans="1:59" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1028,318 +1063,614 @@
         <v>16</v>
       </c>
       <c r="F7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="I7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="N7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="O7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="P7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="Q7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="R7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="S7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="T7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="U7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="V7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="V7" s="7" t="s">
+      <c r="W7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="X7" s="4" t="s">
+      <c r="Y7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Z7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Z7" s="4" t="s">
+      <c r="AA7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AA7" s="3" t="s">
+      <c r="AB7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AB7" s="2" t="s">
+      <c r="AC7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC7" s="4" t="s">
+      <c r="AD7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AD7" s="3" t="s">
+      <c r="AE7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AE7" s="2" t="s">
+      <c r="AF7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AF7" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="AG7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AH7" s="4" t="s">
+      <c r="AI7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AI7" s="8" t="s">
+      <c r="AJ7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AJ7" s="8" t="s">
+      <c r="AK7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AK7" s="8" t="s">
+      <c r="AL7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AL7" s="8" t="s">
+      <c r="AM7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AM7" s="8" t="s">
+      <c r="AN7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AN7" s="8" t="s">
+      <c r="AO7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AO7" s="9" t="s">
+      <c r="AP7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AP7" s="8" t="s">
+      <c r="AQ7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AQ7" s="9" t="s">
+      <c r="AR7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AR7" s="9" t="s">
+      <c r="AS7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AS7" s="9" t="s">
+      <c r="AT7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AT7" s="9" t="s">
+      <c r="AU7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AU7" s="9" t="s">
+      <c r="AV7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AV7" s="9" t="s">
+      <c r="AW7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AW7" s="9" t="s">
+      <c r="AX7" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="1048520" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048575" s="13"/>
-    </row>
-    <row r="1048576" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048576" s="13"/>
+    <row r="1048520" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048575" s="13"/>
+    </row>
+    <row r="1048576" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048576" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="AI6:AW6"/>
-    <mergeCell ref="O6:V6"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="AJ6:AX6"/>
+    <mergeCell ref="P6:W6"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W1048573"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="11.875" style="17" customWidth="1"/>
+    <col min="6" max="7" width="14.625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="9.25" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="15.75" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="11" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="N2"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1048517" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048517" s="13"/>
+    </row>
+    <row r="1048518" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048518" s="13"/>
+    </row>
+    <row r="1048519" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048573" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Minor formatting tweaks for DR spreadsheets
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -385,7 +385,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -423,6 +423,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -442,12 +451,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -773,13 +776,13 @@
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="13.875" customWidth="1"/>
     <col min="5" max="6" width="14.375" customWidth="1"/>
@@ -816,15 +819,15 @@
   <sheetData>
     <row r="1" spans="1:59" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -909,13 +912,12 @@
       <c r="AI2"/>
     </row>
     <row r="3" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="B3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
@@ -944,13 +946,12 @@
       <c r="AI3"/>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="B4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1006,20 +1007,20 @@
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="I6"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="25"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="28"/>
       <c r="X6"/>
       <c r="Y6"/>
       <c r="AA6"/>
@@ -1028,23 +1029,23 @@
       <c r="AD6"/>
       <c r="AE6"/>
       <c r="AI6"/>
-      <c r="AJ6" s="22" t="s">
+      <c r="AJ6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="AK6" s="22"/>
-      <c r="AL6" s="22"/>
-      <c r="AM6" s="22"/>
-      <c r="AN6" s="22"/>
-      <c r="AO6" s="22"/>
-      <c r="AP6" s="22"/>
-      <c r="AQ6" s="22"/>
-      <c r="AR6" s="22"/>
-      <c r="AS6" s="22"/>
-      <c r="AT6" s="22"/>
-      <c r="AU6" s="22"/>
-      <c r="AV6" s="22"/>
-      <c r="AW6" s="22"/>
-      <c r="AX6" s="22"/>
+      <c r="AK6" s="25"/>
+      <c r="AL6" s="25"/>
+      <c r="AM6" s="25"/>
+      <c r="AN6" s="25"/>
+      <c r="AO6" s="25"/>
+      <c r="AP6" s="25"/>
+      <c r="AQ6" s="25"/>
+      <c r="AR6" s="25"/>
+      <c r="AS6" s="25"/>
+      <c r="AT6" s="25"/>
+      <c r="AU6" s="25"/>
+      <c r="AV6" s="25"/>
+      <c r="AW6" s="25"/>
+      <c r="AX6" s="25"/>
     </row>
     <row r="7" spans="1:59" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1370,12 +1371,13 @@
       <c r="AG1048576" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="B1:J1"/>
     <mergeCell ref="J6:O6"/>
     <mergeCell ref="AJ6:AX6"/>
     <mergeCell ref="P6:W6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1390,7 +1392,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1409,18 +1411,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="B1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1446,9 +1447,9 @@
       <c r="N2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="N3"/>
     </row>
     <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
@@ -1667,8 +1668,9 @@
       <c r="L1048573" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Move condo DR export to condo model repo
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>PIN</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Proration Error</t>
   </si>
   <si>
-    <t>Condo Fixed Unit</t>
-  </si>
-  <si>
-    <t>Condo Garage</t>
-  </si>
-  <si>
     <t>Street Address</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>Building</t>
   </si>
   <si>
-    <t>Tieback Percent Ass./Ownership</t>
-  </si>
-  <si>
     <t>Lnd. S. F.</t>
   </si>
   <si>
@@ -180,9 +171,6 @@
     <t>Run ID (res):</t>
   </si>
   <si>
-    <t>Run ID (condo):</t>
-  </si>
-  <si>
     <t>Card</t>
   </si>
   <si>
@@ -210,7 +198,10 @@
     <t>Total        Bld. S. F.</t>
   </si>
   <si>
-    <t>Townhome Complex/Condo Building ID</t>
+    <t>Townhome Complex ID</t>
+  </si>
+  <si>
+    <t>Tieback (Proration) Rate</t>
   </si>
 </sst>
 </file>
@@ -385,7 +376,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -424,9 +415,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -770,13 +758,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG1048576"/>
+  <dimension ref="A1:BE1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -814,20 +802,19 @@
     <col min="46" max="46" width="11.875" customWidth="1"/>
     <col min="47" max="47" width="10.875" customWidth="1"/>
     <col min="48" max="48" width="11.5" customWidth="1"/>
-    <col min="49" max="49" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:57" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -875,10 +862,8 @@
       <c r="BC1" s="5"/>
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
-      <c r="BF1" s="5"/>
-      <c r="BG1" s="5"/>
-    </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -911,9 +896,9 @@
       <c r="AE2"/>
       <c r="AI2"/>
     </row>
-    <row r="3" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -945,17 +930,9 @@
       <c r="AE3"/>
       <c r="AI3"/>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -979,23 +956,22 @@
       <c r="AE4"/>
       <c r="AI4"/>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
-      <c r="W5"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="27"/>
       <c r="X5"/>
       <c r="Y5"/>
       <c r="AA5"/>
@@ -1004,200 +980,170 @@
       <c r="AD5"/>
       <c r="AE5"/>
       <c r="AI5"/>
-    </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="I6"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="28"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-      <c r="AE6"/>
-      <c r="AI6"/>
-      <c r="AJ6" s="25" t="s">
+      <c r="AJ5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AK6" s="25"/>
-      <c r="AL6" s="25"/>
-      <c r="AM6" s="25"/>
-      <c r="AN6" s="25"/>
-      <c r="AO6" s="25"/>
-      <c r="AP6" s="25"/>
-      <c r="AQ6" s="25"/>
-      <c r="AR6" s="25"/>
-      <c r="AS6" s="25"/>
-      <c r="AT6" s="25"/>
-      <c r="AU6" s="25"/>
-      <c r="AV6" s="25"/>
-      <c r="AW6" s="25"/>
-      <c r="AX6" s="25"/>
-    </row>
-    <row r="7" spans="1:59" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="AK5" s="24"/>
+      <c r="AL5" s="24"/>
+      <c r="AM5" s="24"/>
+      <c r="AN5" s="24"/>
+      <c r="AO5" s="24"/>
+      <c r="AP5" s="24"/>
+      <c r="AQ5" s="24"/>
+      <c r="AR5" s="24"/>
+      <c r="AS5" s="24"/>
+      <c r="AT5" s="24"/>
+      <c r="AU5" s="24"/>
+      <c r="AV5" s="24"/>
+    </row>
+    <row r="6" spans="1:57" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="Q6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="U6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="15" t="s">
+      <c r="V6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AS6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AK7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AN7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AQ7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AR7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AS7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AU7" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="AW7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="AX7" s="9" t="s">
-        <v>14</v>
-      </c>
+    </row>
+    <row r="1048519" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG1048519" s="13"/>
     </row>
     <row r="1048520" spans="33:33" x14ac:dyDescent="0.25">
       <c r="AG1048520" s="13"/>
@@ -1367,17 +1313,13 @@
     <row r="1048575" spans="33:33" x14ac:dyDescent="0.25">
       <c r="AG1048575" s="13"/>
     </row>
-    <row r="1048576" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048576" s="13"/>
-    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
     <mergeCell ref="B1:J1"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="AJ6:AX6"/>
-    <mergeCell ref="P6:W6"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="AJ5:AV5"/>
+    <mergeCell ref="P5:W5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1392,7 +1334,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1411,17 +1353,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="B1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1447,9 +1389,9 @@
       <c r="N2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
       <c r="N3"/>
     </row>
     <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
@@ -1457,34 +1399,34 @@
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="K4" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>8</v>
@@ -1493,7 +1435,7 @@
         <v>7</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="1048517" spans="12:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add comp PINs and scores to desk review spreadsheet
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F82121-034B-433D-AF88-1110A03F5B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
     <sheet name="Card Detail" sheetId="4" r:id="rId2"/>
+    <sheet name="Comp Detail" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +29,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t>PIN</t>
   </si>
@@ -202,19 +206,43 @@
   </si>
   <si>
     <t>Tieback (Proration) Rate</t>
+  </si>
+  <si>
+    <t>Comp 1</t>
+  </si>
+  <si>
+    <t>Comp 2</t>
+  </si>
+  <si>
+    <t>Overall comp score</t>
+  </si>
+  <si>
+    <t>Detail view for comparable sales</t>
+  </si>
+  <si>
+    <t>Sale price</t>
+  </si>
+  <si>
+    <t>Sale date</t>
+  </si>
+  <si>
+    <t>Comp 1 score</t>
+  </si>
+  <si>
+    <t>Comp 2 score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,6 +276,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -370,11 +406,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -388,7 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -398,38 +435,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="37" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -442,9 +479,10 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
@@ -757,14 +795,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE1048575"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BJ1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="AG7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -782,7 +820,7 @@
     <col min="13" max="13" width="10.875" style="10" customWidth="1"/>
     <col min="14" max="14" width="10.625" style="10" customWidth="1"/>
     <col min="15" max="15" width="9.125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="13.625" style="17" customWidth="1"/>
+    <col min="16" max="16" width="13.625" style="15" customWidth="1"/>
     <col min="17" max="18" width="11.625" style="10" customWidth="1"/>
     <col min="19" max="19" width="13.625" style="10" customWidth="1"/>
     <col min="20" max="20" width="11" style="10"/>
@@ -793,18 +831,22 @@
     <col min="25" max="25" width="11" style="11"/>
     <col min="26" max="26" width="10.375" customWidth="1"/>
     <col min="27" max="27" width="13" style="10" customWidth="1"/>
-    <col min="28" max="29" width="13" style="18" customWidth="1"/>
+    <col min="28" max="29" width="13" style="16" customWidth="1"/>
     <col min="30" max="30" width="13" style="10" customWidth="1"/>
-    <col min="31" max="31" width="13" style="18" customWidth="1"/>
-    <col min="35" max="35" width="11" style="13"/>
-    <col min="44" max="44" width="14" customWidth="1"/>
-    <col min="45" max="45" width="12.375" customWidth="1"/>
-    <col min="46" max="46" width="11.875" customWidth="1"/>
-    <col min="47" max="47" width="10.875" customWidth="1"/>
-    <col min="48" max="48" width="11.5" customWidth="1"/>
+    <col min="31" max="31" width="13" style="16" customWidth="1"/>
+    <col min="35" max="36" width="11" style="13"/>
+    <col min="37" max="37" width="15.625" style="13" customWidth="1"/>
+    <col min="38" max="38" width="11" style="13"/>
+    <col min="39" max="39" width="15.625" style="13" customWidth="1"/>
+    <col min="40" max="40" width="11" style="13"/>
+    <col min="49" max="49" width="14" customWidth="1"/>
+    <col min="50" max="50" width="12.375" customWidth="1"/>
+    <col min="51" max="51" width="11.875" customWidth="1"/>
+    <col min="52" max="52" width="10.875" customWidth="1"/>
+    <col min="53" max="53" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:62" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -862,8 +904,13 @@
       <c r="BC1" s="5"/>
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
-    </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
+      <c r="BJ1" s="5"/>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -895,21 +942,26 @@
       <c r="AD2"/>
       <c r="AE2"/>
       <c r="AI2"/>
-    </row>
-    <row r="3" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+    </row>
+    <row r="3" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
@@ -929,8 +981,13 @@
       <c r="AD3"/>
       <c r="AE3"/>
       <c r="AI3"/>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
+      <c r="AM3"/>
+      <c r="AN3"/>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -955,8 +1012,13 @@
       <c r="AD4"/>
       <c r="AE4"/>
       <c r="AI4"/>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AJ4"/>
+      <c r="AK4"/>
+      <c r="AL4"/>
+      <c r="AM4"/>
+      <c r="AN4"/>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="I5"/>
       <c r="J5" s="21"/>
       <c r="K5" s="22"/>
@@ -980,14 +1042,14 @@
       <c r="AD5"/>
       <c r="AE5"/>
       <c r="AI5"/>
-      <c r="AJ5" s="24" t="s">
+      <c r="AJ5"/>
+      <c r="AK5"/>
+      <c r="AL5"/>
+      <c r="AM5"/>
+      <c r="AN5"/>
+      <c r="AO5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AK5" s="24"/>
-      <c r="AL5" s="24"/>
-      <c r="AM5" s="24"/>
-      <c r="AN5" s="24"/>
-      <c r="AO5" s="24"/>
       <c r="AP5" s="24"/>
       <c r="AQ5" s="24"/>
       <c r="AR5" s="24"/>
@@ -995,8 +1057,13 @@
       <c r="AT5" s="24"/>
       <c r="AU5" s="24"/>
       <c r="AV5" s="24"/>
-    </row>
-    <row r="6" spans="1:57" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="AW5" s="24"/>
+      <c r="AX5" s="24"/>
+      <c r="AY5" s="24"/>
+      <c r="AZ5" s="24"/>
+      <c r="BA5" s="24"/>
+    </row>
+    <row r="6" spans="1:62" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1088,7 @@
       <c r="H6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="14" t="s">
         <v>55</v>
       </c>
       <c r="J6" s="6" t="s">
@@ -1045,7 +1112,7 @@
       <c r="P6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="R6" s="6" t="s">
@@ -1099,48 +1166,71 @@
       <c r="AH6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AI6" s="4" t="s">
+      <c r="AI6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="8" t="s">
+      <c r="AJ6" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AK6" s="8" t="s">
+      <c r="AP6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AL6" s="8" t="s">
+      <c r="AQ6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AM6" s="8" t="s">
+      <c r="AR6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AN6" s="8" t="s">
+      <c r="AS6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AO6" s="8" t="s">
+      <c r="AT6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AP6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AQ6" s="8" t="s">
+      <c r="AV6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AR6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AS6" s="9" t="s">
+      <c r="AX6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AT6" s="9" t="s">
+      <c r="AY6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AZ6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AV6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="AK8" s="18"/>
+      <c r="AL8" s="18"/>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="AK9" s="18"/>
+      <c r="AL9" s="18"/>
     </row>
     <row r="1048519" spans="33:33" x14ac:dyDescent="0.25">
       <c r="AG1048519" s="13"/>
@@ -1318,7 +1408,7 @@
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AJ5:AV5"/>
+    <mergeCell ref="AO5:BA5"/>
     <mergeCell ref="P5:W5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1327,14 +1417,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W1048573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1343,7 +1433,7 @@
     <col min="2" max="2" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="9.875" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="11.875" style="15" customWidth="1"/>
     <col min="6" max="7" width="14.625" style="10" customWidth="1"/>
     <col min="9" max="9" width="9.25" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
@@ -1410,10 +1500,10 @@
       <c r="E4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="9" t="s">
         <v>49</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -1617,4 +1707,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up comps sheet and prep for sales val outlier flags in desk review workbook
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F82121-034B-433D-AF88-1110A03F5B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F91BE3D-8B7B-4A01-A1F2-CAA27344AFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32025" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
     <sheet name="Card Detail" sheetId="4" r:id="rId2"/>
-    <sheet name="Comp Detail" sheetId="5" r:id="rId3"/>
+    <sheet name="Sales" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +37,114 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean Cochrane</author>
+  </authors>
+  <commentList>
+    <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jean Cochrane:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm. If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AL6" authorId="0" shapeId="0" xr:uid="{0878E9D8-A2FA-4E71-98AD-3CB2F004A791}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jean Cochrane:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column represents the average similarity score for all of the comparable parcels we extracted for this property based on the model structure. (The first two comps are shown in subsequent columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AM6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jean Cochrane:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jean Cochrane:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column represents the similarity score for this comparable sale, which we can interpret as the percent confidence that the model has that the parcel sold in this sale is comparable to the target parcel.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
     <t>PIN</t>
   </si>
@@ -208,12 +314,6 @@
     <t>Tieback (Proration) Rate</t>
   </si>
   <si>
-    <t>Comp 1</t>
-  </si>
-  <si>
-    <t>Comp 2</t>
-  </si>
-  <si>
     <t>Overall comp score</t>
   </si>
   <si>
@@ -230,6 +330,18 @@
   </si>
   <si>
     <t>Comp 2 score</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 2</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 1</t>
+  </si>
+  <si>
+    <t>Comp 1 PIN</t>
+  </si>
+  <si>
+    <t>Comp 2 PIN</t>
   </si>
 </sst>
 </file>
@@ -242,7 +354,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -287,6 +399,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -795,14 +920,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ1048575"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BL1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="AG7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="AJ6" sqref="AJ6"/>
+      <selection pane="bottomRight" activeCell="AO13" sqref="AO13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -830,23 +955,23 @@
     <col min="24" max="24" width="11" style="12"/>
     <col min="25" max="25" width="11" style="11"/>
     <col min="26" max="26" width="10.375" customWidth="1"/>
-    <col min="27" max="27" width="13" style="10" customWidth="1"/>
-    <col min="28" max="29" width="13" style="16" customWidth="1"/>
-    <col min="30" max="30" width="13" style="10" customWidth="1"/>
-    <col min="31" max="31" width="13" style="16" customWidth="1"/>
-    <col min="35" max="36" width="11" style="13"/>
-    <col min="37" max="37" width="15.625" style="13" customWidth="1"/>
-    <col min="38" max="38" width="11" style="13"/>
+    <col min="27" max="28" width="13" style="10" customWidth="1"/>
+    <col min="29" max="30" width="13" style="16" customWidth="1"/>
+    <col min="31" max="32" width="13" style="10" customWidth="1"/>
+    <col min="33" max="33" width="13" style="16" customWidth="1"/>
+    <col min="37" max="38" width="11" style="13"/>
     <col min="39" max="39" width="15.625" style="13" customWidth="1"/>
     <col min="40" max="40" width="11" style="13"/>
-    <col min="49" max="49" width="14" customWidth="1"/>
-    <col min="50" max="50" width="12.375" customWidth="1"/>
-    <col min="51" max="51" width="11.875" customWidth="1"/>
-    <col min="52" max="52" width="10.875" customWidth="1"/>
-    <col min="53" max="53" width="11.5" customWidth="1"/>
+    <col min="41" max="41" width="15.625" style="13" customWidth="1"/>
+    <col min="42" max="42" width="11" style="13"/>
+    <col min="51" max="51" width="14" customWidth="1"/>
+    <col min="52" max="52" width="12.375" customWidth="1"/>
+    <col min="53" max="53" width="11.875" customWidth="1"/>
+    <col min="54" max="54" width="10.875" customWidth="1"/>
+    <col min="55" max="55" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -909,8 +1034,10 @@
       <c r="BH1" s="5"/>
       <c r="BI1" s="5"/>
       <c r="BJ1" s="5"/>
-    </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="5"/>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -941,14 +1068,16 @@
       <c r="AC2"/>
       <c r="AD2"/>
       <c r="AE2"/>
-      <c r="AI2"/>
-      <c r="AJ2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
       <c r="AK2"/>
       <c r="AL2"/>
       <c r="AM2"/>
       <c r="AN2"/>
-    </row>
-    <row r="3" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO2"/>
+      <c r="AP2"/>
+    </row>
+    <row r="3" spans="1:64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>44</v>
       </c>
@@ -980,14 +1109,16 @@
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3"/>
-      <c r="AI3"/>
-      <c r="AJ3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
       <c r="AK3"/>
       <c r="AL3"/>
       <c r="AM3"/>
       <c r="AN3"/>
-    </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="AO3"/>
+      <c r="AP3"/>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1011,14 +1142,16 @@
       <c r="AC4"/>
       <c r="AD4"/>
       <c r="AE4"/>
-      <c r="AI4"/>
-      <c r="AJ4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
       <c r="AK4"/>
       <c r="AL4"/>
       <c r="AM4"/>
       <c r="AN4"/>
-    </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="AO4"/>
+      <c r="AP4"/>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="I5"/>
       <c r="J5" s="21"/>
       <c r="K5" s="22"/>
@@ -1041,17 +1174,17 @@
       <c r="AC5"/>
       <c r="AD5"/>
       <c r="AE5"/>
-      <c r="AI5"/>
-      <c r="AJ5"/>
+      <c r="AF5"/>
+      <c r="AG5"/>
       <c r="AK5"/>
       <c r="AL5"/>
       <c r="AM5"/>
       <c r="AN5"/>
-      <c r="AO5" s="24" t="s">
+      <c r="AO5"/>
+      <c r="AP5"/>
+      <c r="AQ5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AP5" s="24"/>
-      <c r="AQ5" s="24"/>
       <c r="AR5" s="24"/>
       <c r="AS5" s="24"/>
       <c r="AT5" s="24"/>
@@ -1062,8 +1195,10 @@
       <c r="AY5" s="24"/>
       <c r="AZ5" s="24"/>
       <c r="BA5" s="24"/>
-    </row>
-    <row r="6" spans="1:62" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="BB5" s="24"/>
+      <c r="BC5" s="24"/>
+    </row>
+    <row r="6" spans="1:64" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1142,277 +1277,284 @@
       <c r="Z6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AA6" s="4" t="s">
+      <c r="AA6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AB6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AD6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AD6" s="4" t="s">
+      <c r="AE6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AH6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AI6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AJ6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AI6" s="3" t="s">
+      <c r="AK6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="AK6" s="8" t="s">
+      <c r="AL6" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AL6" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="AM6" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AN6" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="AN6" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="AO6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AP6" s="8" t="s">
+      <c r="AR6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AQ6" s="8" t="s">
+      <c r="AS6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AR6" s="8" t="s">
+      <c r="AT6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AS6" s="8" t="s">
+      <c r="AU6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AT6" s="8" t="s">
+      <c r="AV6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AV6" s="8" t="s">
+      <c r="AX6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AW6" s="9" t="s">
+      <c r="AY6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AX6" s="9" t="s">
+      <c r="AZ6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AY6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AZ6" s="9" t="s">
+      <c r="BB6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BC6" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="AK8" s="18"/>
-      <c r="AL8" s="18"/>
-    </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="AK9" s="18"/>
-      <c r="AL9" s="18"/>
-    </row>
-    <row r="1048519" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048575" s="13"/>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="18"/>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AM9" s="18"/>
+      <c r="AN9" s="18"/>
+    </row>
+    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AO5:BA5"/>
+    <mergeCell ref="AQ5:BC5"/>
     <mergeCell ref="P5:W5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1715,17 +1857,22 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="3" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="24.375" customWidth="1"/>
+    <col min="9" max="10" width="15.625" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="13" max="13" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
@@ -1737,10 +1884,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Query and display sale outlier information in the desk review workbook
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F91BE3D-8B7B-4A01-A1F2-CAA27344AFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE02853-6D9A-4243-BA0E-8DA5BD5268CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32025" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32385" yWindow="735" windowWidth="21600" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -924,7 +924,7 @@
   <dimension ref="A1:BL1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="AG7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="bottomRight" activeCell="AO13" sqref="AO13"/>
@@ -955,9 +955,11 @@
     <col min="24" max="24" width="11" style="12"/>
     <col min="25" max="25" width="11" style="11"/>
     <col min="26" max="26" width="10.375" customWidth="1"/>
-    <col min="27" max="28" width="13" style="10" customWidth="1"/>
+    <col min="27" max="27" width="13" style="10" customWidth="1"/>
+    <col min="28" max="28" width="18.625" style="10" customWidth="1"/>
     <col min="29" max="30" width="13" style="16" customWidth="1"/>
-    <col min="31" max="32" width="13" style="10" customWidth="1"/>
+    <col min="31" max="31" width="13" style="10" customWidth="1"/>
+    <col min="32" max="32" width="18.625" style="10" customWidth="1"/>
     <col min="33" max="33" width="13" style="16" customWidth="1"/>
     <col min="37" max="38" width="11" style="13"/>
     <col min="39" max="39" width="15.625" style="13" customWidth="1"/>
@@ -1856,8 +1858,10 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L7" sqref="L7"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Standardize formatting of new column names in desk review workbook
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE02853-6D9A-4243-BA0E-8DA5BD5268CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FF3C63-03B4-410B-A6CB-6F8639D11974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32385" yWindow="735" windowWidth="21600" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -314,9 +314,6 @@
     <t>Tieback (Proration) Rate</t>
   </si>
   <si>
-    <t>Overall comp score</t>
-  </si>
-  <si>
     <t>Detail view for comparable sales</t>
   </si>
   <si>
@@ -326,22 +323,25 @@
     <t>Sale date</t>
   </si>
   <si>
-    <t>Comp 1 score</t>
-  </si>
-  <si>
-    <t>Comp 2 score</t>
-  </si>
-  <si>
     <t>Non-Arm's-Length Sale Flag 2</t>
   </si>
   <si>
     <t>Non-Arm's-Length Sale Flag 1</t>
   </si>
   <si>
-    <t>Comp 1 PIN</t>
-  </si>
-  <si>
-    <t>Comp 2 PIN</t>
+    <t>Overall Comp. Score</t>
+  </si>
+  <si>
+    <t>Comp. 1 PIN</t>
+  </si>
+  <si>
+    <t>Comp. 1 Score</t>
+  </si>
+  <si>
+    <t>Comp. 2 PIN</t>
+  </si>
+  <si>
+    <t>Comp. 2 Score</t>
   </si>
 </sst>
 </file>
@@ -927,7 +927,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="AO13" sqref="AO13"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1283,7 @@
         <v>21</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AC6" s="3" t="s">
         <v>22</v>
@@ -1295,7 +1295,7 @@
         <v>24</v>
       </c>
       <c r="AF6" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AG6" s="3" t="s">
         <v>25</v>
@@ -1313,19 +1313,19 @@
         <v>40</v>
       </c>
       <c r="AL6" s="17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="AM6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AN6" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO6" s="8" t="s">
+      <c r="AP6" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="AP6" s="14" t="s">
-        <v>61</v>
       </c>
       <c r="AQ6" s="8" t="s">
         <v>26</v>
@@ -1876,7 +1876,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
@@ -1888,10 +1888,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Tweak export stage following Dan's review
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FF3C63-03B4-410B-A6CB-6F8639D11974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897A2092-31C1-4E99-B2C2-EC0737924189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
     <sheet name="Card Detail" sheetId="4" r:id="rId2"/>
-    <sheet name="Sales" sheetId="5" r:id="rId3"/>
+    <sheet name="Comparables" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>PIN</t>
   </si>
@@ -342,6 +342,18 @@
   </si>
   <si>
     <t>Comp. 2 Score</t>
+  </si>
+  <si>
+    <t>Comparables</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Characteristics</t>
+  </si>
+  <si>
+    <t>Change in value</t>
   </si>
 </sst>
 </file>
@@ -414,7 +426,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,8 +445,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -530,6 +566,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -538,7 +585,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -576,6 +623,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="37" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -601,6 +651,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -924,10 +992,10 @@
   <dimension ref="A1:BL1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -935,7 +1003,7 @@
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="38.875" customWidth="1"/>
     <col min="5" max="6" width="14.375" customWidth="1"/>
     <col min="7" max="7" width="8.875" customWidth="1"/>
     <col min="8" max="8" width="15.375" customWidth="1"/>
@@ -975,15 +1043,15 @@
   <sheetData>
     <row r="1" spans="1:64" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1083,9 +1151,9 @@
       <c r="B3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1146,7 +1214,10 @@
       <c r="AE4"/>
       <c r="AF4"/>
       <c r="AG4"/>
-      <c r="AK4"/>
+      <c r="AH4" s="31"/>
+      <c r="AI4" s="31"/>
+      <c r="AJ4" s="31"/>
+      <c r="AK4" s="31"/>
       <c r="AL4"/>
       <c r="AM4"/>
       <c r="AN4"/>
@@ -1155,50 +1226,62 @@
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="27"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-      <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5"/>
-      <c r="AD5"/>
-      <c r="AE5"/>
-      <c r="AF5"/>
-      <c r="AG5"/>
-      <c r="AK5"/>
-      <c r="AL5"/>
-      <c r="AM5"/>
-      <c r="AN5"/>
-      <c r="AO5"/>
-      <c r="AP5"/>
-      <c r="AQ5" s="24" t="s">
+      <c r="J5" s="22"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA5" s="30"/>
+      <c r="AB5" s="30"/>
+      <c r="AC5" s="30"/>
+      <c r="AD5" s="30"/>
+      <c r="AE5" s="30"/>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="30"/>
+      <c r="AH5" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI5" s="33"/>
+      <c r="AJ5" s="33"/>
+      <c r="AK5" s="33"/>
+      <c r="AL5" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM5" s="29"/>
+      <c r="AN5" s="29"/>
+      <c r="AO5" s="29"/>
+      <c r="AP5" s="29"/>
+      <c r="AQ5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="AR5" s="24"/>
-      <c r="AS5" s="24"/>
-      <c r="AT5" s="24"/>
-      <c r="AU5" s="24"/>
-      <c r="AV5" s="24"/>
-      <c r="AW5" s="24"/>
-      <c r="AX5" s="24"/>
-      <c r="AY5" s="24"/>
-      <c r="AZ5" s="24"/>
-      <c r="BA5" s="24"/>
-      <c r="BB5" s="24"/>
-      <c r="BC5" s="24"/>
+      <c r="AR5" s="25"/>
+      <c r="AS5" s="25"/>
+      <c r="AT5" s="25"/>
+      <c r="AU5" s="25"/>
+      <c r="AV5" s="25"/>
+      <c r="AW5" s="25"/>
+      <c r="AX5" s="25"/>
+      <c r="AY5" s="25"/>
+      <c r="AZ5" s="25"/>
+      <c r="BA5" s="25"/>
+      <c r="BB5" s="25"/>
+      <c r="BC5" s="25"/>
     </row>
     <row r="6" spans="1:64" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1300,16 +1383,16 @@
       <c r="AG6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AH6" s="2" t="s">
+      <c r="AH6" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="AI6" s="3" t="s">
+      <c r="AI6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AJ6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AK6" s="3" t="s">
+      <c r="AK6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="AL6" s="17" t="s">
@@ -1547,12 +1630,17 @@
       <c r="AI1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
     <mergeCell ref="AQ5:BC5"/>
     <mergeCell ref="P5:W5"/>
+    <mergeCell ref="AL5:AP5"/>
+    <mergeCell ref="Z5:AG5"/>
+    <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="AH5:AK5"/>
+    <mergeCell ref="X5:Y5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1587,17 +1675,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1623,9 +1711,9 @@
       <c r="N2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="N3"/>
     </row>
     <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
@@ -1875,13 +1963,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">

</xml_diff>

<commit_message>
Add comps and sales val indicators to desk review workbook (#199)
* Fixup export stage to reflect new data model

* Add comp PINs and scores to desk review spreadsheet

* WIP add comps sheet to desk review workbook

* Clean up comps sheet and prep for sales val outlier flags in desk review workbook

* Query and display sale outlier information in the desk review workbook

* Standardize formatting of new column names in desk review workbook

* Appease pre-commit

* Add comments to new desk review workbook code

* Tweak export stage following Dan's review

* Add comment to outlier inclusion in assess stage
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897A2092-31C1-4E99-B2C2-EC0737924189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
     <sheet name="Card Detail" sheetId="4" r:id="rId2"/>
+    <sheet name="Comparables" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,14 +29,122 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean Cochrane</author>
+  </authors>
+  <commentList>
+    <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jean Cochrane:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm. If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AL6" authorId="0" shapeId="0" xr:uid="{0878E9D8-A2FA-4E71-98AD-3CB2F004A791}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jean Cochrane:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column represents the average similarity score for all of the comparable parcels we extracted for this property based on the model structure. (The first two comps are shown in subsequent columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AM6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jean Cochrane:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jean Cochrane:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column represents the similarity score for this comparable sale, which we can interpret as the percent confidence that the model has that the parcel sold in this sale is comparable to the target parcel.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>PIN</t>
   </si>
@@ -202,19 +312,61 @@
   </si>
   <si>
     <t>Tieback (Proration) Rate</t>
+  </si>
+  <si>
+    <t>Detail view for comparable sales</t>
+  </si>
+  <si>
+    <t>Sale price</t>
+  </si>
+  <si>
+    <t>Sale date</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 2</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 1</t>
+  </si>
+  <si>
+    <t>Overall Comp. Score</t>
+  </si>
+  <si>
+    <t>Comp. 1 PIN</t>
+  </si>
+  <si>
+    <t>Comp. 1 Score</t>
+  </si>
+  <si>
+    <t>Comp. 2 PIN</t>
+  </si>
+  <si>
+    <t>Comp. 2 Score</t>
+  </si>
+  <si>
+    <t>Comparables</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Characteristics</t>
+  </si>
+  <si>
+    <t>Change in value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,8 +404,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,8 +445,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -369,14 +566,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -388,7 +597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -398,38 +607,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="37" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -441,10 +653,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
@@ -757,14 +988,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE1048575"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BL1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -772,7 +1003,7 @@
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="38.875" customWidth="1"/>
     <col min="5" max="6" width="14.375" customWidth="1"/>
     <col min="7" max="7" width="8.875" customWidth="1"/>
     <col min="8" max="8" width="15.375" customWidth="1"/>
@@ -782,7 +1013,7 @@
     <col min="13" max="13" width="10.875" style="10" customWidth="1"/>
     <col min="14" max="14" width="10.625" style="10" customWidth="1"/>
     <col min="15" max="15" width="9.125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="13.625" style="17" customWidth="1"/>
+    <col min="16" max="16" width="13.625" style="15" customWidth="1"/>
     <col min="17" max="18" width="11.625" style="10" customWidth="1"/>
     <col min="19" max="19" width="13.625" style="10" customWidth="1"/>
     <col min="20" max="20" width="11" style="10"/>
@@ -793,28 +1024,34 @@
     <col min="25" max="25" width="11" style="11"/>
     <col min="26" max="26" width="10.375" customWidth="1"/>
     <col min="27" max="27" width="13" style="10" customWidth="1"/>
-    <col min="28" max="29" width="13" style="18" customWidth="1"/>
-    <col min="30" max="30" width="13" style="10" customWidth="1"/>
-    <col min="31" max="31" width="13" style="18" customWidth="1"/>
-    <col min="35" max="35" width="11" style="13"/>
-    <col min="44" max="44" width="14" customWidth="1"/>
-    <col min="45" max="45" width="12.375" customWidth="1"/>
-    <col min="46" max="46" width="11.875" customWidth="1"/>
-    <col min="47" max="47" width="10.875" customWidth="1"/>
-    <col min="48" max="48" width="11.5" customWidth="1"/>
+    <col min="28" max="28" width="18.625" style="10" customWidth="1"/>
+    <col min="29" max="30" width="13" style="16" customWidth="1"/>
+    <col min="31" max="31" width="13" style="10" customWidth="1"/>
+    <col min="32" max="32" width="18.625" style="10" customWidth="1"/>
+    <col min="33" max="33" width="13" style="16" customWidth="1"/>
+    <col min="37" max="38" width="11" style="13"/>
+    <col min="39" max="39" width="15.625" style="13" customWidth="1"/>
+    <col min="40" max="40" width="11" style="13"/>
+    <col min="41" max="41" width="15.625" style="13" customWidth="1"/>
+    <col min="42" max="42" width="11" style="13"/>
+    <col min="51" max="51" width="14" customWidth="1"/>
+    <col min="52" max="52" width="12.375" customWidth="1"/>
+    <col min="53" max="53" width="11.875" customWidth="1"/>
+    <col min="54" max="54" width="10.875" customWidth="1"/>
+    <col min="55" max="55" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -862,8 +1099,15 @@
       <c r="BC1" s="5"/>
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
-    </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
+      <c r="BJ1" s="5"/>
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="5"/>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -894,22 +1138,29 @@
       <c r="AC2"/>
       <c r="AD2"/>
       <c r="AE2"/>
-      <c r="AI2"/>
-    </row>
-    <row r="3" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+    </row>
+    <row r="3" spans="1:64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
@@ -928,9 +1179,16 @@
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3"/>
-      <c r="AI3"/>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
+      <c r="AM3"/>
+      <c r="AN3"/>
+      <c r="AO3"/>
+      <c r="AP3"/>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -954,49 +1212,78 @@
       <c r="AC4"/>
       <c r="AD4"/>
       <c r="AE4"/>
-      <c r="AI4"/>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AH4" s="31"/>
+      <c r="AI4" s="31"/>
+      <c r="AJ4" s="31"/>
+      <c r="AK4" s="31"/>
+      <c r="AL4"/>
+      <c r="AM4"/>
+      <c r="AN4"/>
+      <c r="AO4"/>
+      <c r="AP4"/>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="27"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-      <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5"/>
-      <c r="AD5"/>
-      <c r="AE5"/>
-      <c r="AI5"/>
-      <c r="AJ5" s="24" t="s">
+      <c r="J5" s="22"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA5" s="30"/>
+      <c r="AB5" s="30"/>
+      <c r="AC5" s="30"/>
+      <c r="AD5" s="30"/>
+      <c r="AE5" s="30"/>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="30"/>
+      <c r="AH5" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI5" s="33"/>
+      <c r="AJ5" s="33"/>
+      <c r="AK5" s="33"/>
+      <c r="AL5" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM5" s="29"/>
+      <c r="AN5" s="29"/>
+      <c r="AO5" s="29"/>
+      <c r="AP5" s="29"/>
+      <c r="AQ5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="AK5" s="24"/>
-      <c r="AL5" s="24"/>
-      <c r="AM5" s="24"/>
-      <c r="AN5" s="24"/>
-      <c r="AO5" s="24"/>
-      <c r="AP5" s="24"/>
-      <c r="AQ5" s="24"/>
-      <c r="AR5" s="24"/>
-      <c r="AS5" s="24"/>
-      <c r="AT5" s="24"/>
-      <c r="AU5" s="24"/>
-      <c r="AV5" s="24"/>
-    </row>
-    <row r="6" spans="1:57" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="AR5" s="25"/>
+      <c r="AS5" s="25"/>
+      <c r="AT5" s="25"/>
+      <c r="AU5" s="25"/>
+      <c r="AV5" s="25"/>
+      <c r="AW5" s="25"/>
+      <c r="AX5" s="25"/>
+      <c r="AY5" s="25"/>
+      <c r="AZ5" s="25"/>
+      <c r="BA5" s="25"/>
+      <c r="BB5" s="25"/>
+      <c r="BC5" s="25"/>
+    </row>
+    <row r="6" spans="1:64" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1308,7 @@
       <c r="H6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="14" t="s">
         <v>55</v>
       </c>
       <c r="J6" s="6" t="s">
@@ -1045,7 +1332,7 @@
       <c r="P6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="R6" s="6" t="s">
@@ -1075,266 +1362,301 @@
       <c r="Z6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AA6" s="4" t="s">
+      <c r="AA6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AB6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AD6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AD6" s="4" t="s">
+      <c r="AE6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AH6" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AI6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AJ6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AI6" s="4" t="s">
+      <c r="AK6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="8" t="s">
+      <c r="AL6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP6" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AK6" s="8" t="s">
+      <c r="AR6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AL6" s="8" t="s">
+      <c r="AS6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AM6" s="8" t="s">
+      <c r="AT6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AN6" s="8" t="s">
+      <c r="AU6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AO6" s="8" t="s">
+      <c r="AV6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AP6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AQ6" s="8" t="s">
+      <c r="AX6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AR6" s="9" t="s">
+      <c r="AY6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AS6" s="9" t="s">
+      <c r="AZ6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AT6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="BB6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AV6" s="9" t="s">
+      <c r="BC6" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="1048519" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="33:33" x14ac:dyDescent="0.25">
-      <c r="AG1048575" s="13"/>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="18"/>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AM9" s="18"/>
+      <c r="AN9" s="18"/>
+    </row>
+    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AJ5:AV5"/>
+    <mergeCell ref="AQ5:BC5"/>
     <mergeCell ref="P5:W5"/>
+    <mergeCell ref="AL5:AP5"/>
+    <mergeCell ref="Z5:AG5"/>
+    <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="AH5:AK5"/>
+    <mergeCell ref="X5:Y5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W1048573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1343,7 +1665,7 @@
     <col min="2" max="2" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="9.875" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="11.875" style="15" customWidth="1"/>
     <col min="6" max="7" width="14.625" style="10" customWidth="1"/>
     <col min="9" max="9" width="9.25" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
@@ -1353,17 +1675,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1389,9 +1711,9 @@
       <c r="N2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="N3"/>
     </row>
     <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
@@ -1410,10 +1732,10 @@
       <c r="E4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="9" t="s">
         <v>49</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -1617,4 +1939,83 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="3" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="24.375" customWidth="1"/>
+    <col min="9" max="10" width="15.625" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="13" max="13" width="11.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+    </row>
+    <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add numbers of units to desk review output
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27321"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897A2092-31C1-4E99-B2C2-EC0737924189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{897A2092-31C1-4E99-B2C2-EC0737924189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6D96D48-2A34-4C5C-976E-A22FDC2D12B3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Card Detail" sheetId="4" r:id="rId2"/>
     <sheet name="Comparables" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,6 +41,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jean Cochrane</author>
+    <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
     <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
@@ -67,7 +68,19 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL6" authorId="0" shapeId="0" xr:uid="{0878E9D8-A2FA-4E71-98AD-3CB2F004A791}">
+    <comment ref="AL6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
+      <text>
+        <t>Jean Cochrane (Assessor):
+The number of apartments in a property. Only present for class 211 and class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+      </text>
+    </comment>
+    <comment ref="AM6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
+      <text>
+        <t>Jean Cochrane (Assessor):
+The number of commercial units in a property. Only present for class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+      </text>
+    </comment>
+    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{0878E9D8-A2FA-4E71-98AD-3CB2F004A791}">
       <text>
         <r>
           <rPr>
@@ -91,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
       <text>
         <r>
           <rPr>
@@ -115,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
       <text>
         <r>
           <rPr>
@@ -143,8 +156,48 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean Cochrane (Assessor)</author>
+  </authors>
+  <commentList>
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
+      <text>
+        <t>Jean Cochrane (Assessor):
+The number of apartments in a card. Only present for class 211 and 212 parcels.</t>
+      </text>
+    </comment>
+    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
+      <text>
+        <t>Jean Cochrane (Assessor):
+The number of commercial units in a card. Only present for class 212 parcels.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+  <si>
+    <t>Run ID (res):</t>
+  </si>
+  <si>
+    <t>Change in value</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Characteristics</t>
+  </si>
+  <si>
+    <t>Comparables</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
   <si>
     <t>PIN</t>
   </si>
@@ -152,168 +205,189 @@
     <t>Class</t>
   </si>
   <si>
+    <t>Nbhd.</t>
+  </si>
+  <si>
+    <t>Street Address</t>
+  </si>
+  <si>
+    <t>Municipality</t>
+  </si>
+  <si>
+    <t>Townhome Complex ID</t>
+  </si>
+  <si>
+    <t>PIN Num. Cards</t>
+  </si>
+  <si>
+    <t>Tieback Key PIN</t>
+  </si>
+  <si>
+    <t>Tieback (Proration) Rate</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Lnd. Rate    S. F.</t>
+  </si>
+  <si>
+    <t>Bld. Rate    S. F.</t>
+  </si>
+  <si>
+    <t>Lnd. % of Total</t>
+  </si>
+  <si>
+    <t>Before Rounding</t>
+  </si>
+  <si>
+    <t>Lnd. Rate Original</t>
+  </si>
+  <si>
+    <t>Lnd. Rate     Effective</t>
+  </si>
+  <si>
+    <t>Bld. Rate     S. F.</t>
+  </si>
+  <si>
+    <t>Lnd. % of Tot.</t>
+  </si>
+  <si>
     <t>YoY ∆ $</t>
   </si>
   <si>
     <t>YoY ∆ %</t>
   </si>
   <si>
-    <t>Land</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Lnd. % of Tot.</t>
+    <t>Sale Date 1</t>
+  </si>
+  <si>
+    <t>Sale Amount 1</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 1</t>
+  </si>
+  <si>
+    <t>Sale Doc. 1</t>
+  </si>
+  <si>
+    <t>Sale Date 2</t>
+  </si>
+  <si>
+    <t>Sale Amount 2</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 2</t>
+  </si>
+  <si>
+    <t>Sale Doc. 2</t>
+  </si>
+  <si>
+    <t>Year Built</t>
+  </si>
+  <si>
+    <t>Total        Bld. S. F.</t>
   </si>
   <si>
     <t>Stories</t>
   </si>
   <si>
+    <t>Lnd. S. F.</t>
+  </si>
+  <si>
+    <t># Res. Units</t>
+  </si>
+  <si>
+    <t># Comm. Units</t>
+  </si>
+  <si>
+    <t>Overall Comp. Score</t>
+  </si>
+  <si>
+    <t>Comp. 1 PIN</t>
+  </si>
+  <si>
+    <t>Comp. 1 Score</t>
+  </si>
+  <si>
+    <t>Comp. 2 PIN</t>
+  </si>
+  <si>
+    <t>Comp. 2 Score</t>
+  </si>
+  <si>
+    <t>Is Prorated</t>
+  </si>
+  <si>
+    <t>Proration Error</t>
+  </si>
+  <si>
+    <t>Multi-Card</t>
+  </si>
+  <si>
+    <t>Multi-Land</t>
+  </si>
+  <si>
+    <t>Lnd. &gt;= 95% in Town</t>
+  </si>
+  <si>
+    <t>Bld. &gt;= 95% in Town</t>
+  </si>
+  <si>
+    <t>Land Value Capped</t>
+  </si>
+  <si>
+    <t># Expired 288s</t>
+  </si>
+  <si>
+    <t>Value Unchanged</t>
+  </si>
+  <si>
+    <t>Post-Modeling Change</t>
+  </si>
+  <si>
+    <t>YoY Change &gt;= 50%</t>
+  </si>
+  <si>
+    <t>YoY Change &lt;= -5%</t>
+  </si>
+  <si>
+    <t>Critical Char. Missing</t>
+  </si>
+  <si>
+    <t>Contains only PINs with multiple cards</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Card % Total (By Sqft)</t>
+  </si>
+  <si>
+    <t>Card Initial FMV</t>
+  </si>
+  <si>
+    <t>Card Final FMV</t>
+  </si>
+  <si>
+    <t># Beds</t>
+  </si>
+  <si>
+    <t>Ext. Wall</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
     <t>Bld. S. F.</t>
   </si>
   <si>
-    <t>Lnd. % of Total</t>
-  </si>
-  <si>
-    <t>Bld. Rate     S. F.</t>
-  </si>
-  <si>
-    <t>Flags</t>
-  </si>
-  <si>
-    <t>Proration Error</t>
-  </si>
-  <si>
-    <t>Street Address</t>
-  </si>
-  <si>
-    <t>Municipality</t>
-  </si>
-  <si>
-    <t>Before Rounding</t>
-  </si>
-  <si>
-    <t>Tieback Key PIN</t>
-  </si>
-  <si>
-    <t>PIN Num. Cards</t>
-  </si>
-  <si>
-    <t>Lnd. Rate Original</t>
-  </si>
-  <si>
-    <t>Lnd. Rate     Effective</t>
-  </si>
-  <si>
-    <t>Sale Date 1</t>
-  </si>
-  <si>
-    <t>Sale Amount 1</t>
-  </si>
-  <si>
-    <t>Sale Doc. 1</t>
-  </si>
-  <si>
-    <t>Sale Date 2</t>
-  </si>
-  <si>
-    <t>Sale Amount 2</t>
-  </si>
-  <si>
-    <t>Sale Doc. 2</t>
-  </si>
-  <si>
-    <t>Is Prorated</t>
-  </si>
-  <si>
-    <t>Multi-Land</t>
-  </si>
-  <si>
-    <t>Multi-Card</t>
-  </si>
-  <si>
-    <t>Lnd. &gt;= 95% in Town</t>
-  </si>
-  <si>
-    <t>Bld. &gt;= 95% in Town</t>
-  </si>
-  <si>
-    <t>Land Value Capped</t>
-  </si>
-  <si>
-    <t># Expired 288s</t>
-  </si>
-  <si>
-    <t>Value Unchanged</t>
-  </si>
-  <si>
-    <t>Post-Modeling Change</t>
-  </si>
-  <si>
-    <t>YoY Change &gt;= 50%</t>
-  </si>
-  <si>
-    <t>YoY Change &lt;= -5%</t>
-  </si>
-  <si>
-    <t>Lnd. Rate    S. F.</t>
-  </si>
-  <si>
-    <t>Bld. Rate    S. F.</t>
-  </si>
-  <si>
-    <t>Building</t>
-  </si>
-  <si>
-    <t>Lnd. S. F.</t>
-  </si>
-  <si>
-    <t>Year Built</t>
-  </si>
-  <si>
-    <t>Critical Char. Missing</t>
-  </si>
-  <si>
-    <t>Nbhd.</t>
-  </si>
-  <si>
-    <t>Run ID (res):</t>
-  </si>
-  <si>
-    <t>Card</t>
-  </si>
-  <si>
-    <t>Contains only PINs with multiple cards</t>
-  </si>
-  <si>
-    <t>Card % Total (By Sqft)</t>
-  </si>
-  <si>
-    <t>Card Initial FMV</t>
-  </si>
-  <si>
-    <t>Card Final FMV</t>
-  </si>
-  <si>
-    <t># Beds</t>
-  </si>
-  <si>
-    <t>Ext. Wall</t>
-  </si>
-  <si>
-    <t>Heat</t>
-  </si>
-  <si>
-    <t>Total        Bld. S. F.</t>
-  </si>
-  <si>
-    <t>Townhome Complex ID</t>
-  </si>
-  <si>
-    <t>Tieback (Proration) Rate</t>
-  </si>
-  <si>
     <t>Detail view for comparable sales</t>
   </si>
   <si>
@@ -321,39 +395,6 @@
   </si>
   <si>
     <t>Sale date</t>
-  </si>
-  <si>
-    <t>Non-Arm's-Length Sale Flag 2</t>
-  </si>
-  <si>
-    <t>Non-Arm's-Length Sale Flag 1</t>
-  </si>
-  <si>
-    <t>Overall Comp. Score</t>
-  </si>
-  <si>
-    <t>Comp. 1 PIN</t>
-  </si>
-  <si>
-    <t>Comp. 1 Score</t>
-  </si>
-  <si>
-    <t>Comp. 2 PIN</t>
-  </si>
-  <si>
-    <t>Comp. 2 Score</t>
-  </si>
-  <si>
-    <t>Comparables</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Characteristics</t>
-  </si>
-  <si>
-    <t>Change in value</t>
   </si>
 </sst>
 </file>
@@ -366,7 +407,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -470,7 +511,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -577,6 +618,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -585,7 +646,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -627,6 +688,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -659,17 +729,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -989,16 +1062,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL1048575"/>
+  <dimension ref="A1:BN1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="AF7" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AM19" sqref="AM19"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1029,29 +1102,29 @@
     <col min="31" max="31" width="13" style="10" customWidth="1"/>
     <col min="32" max="32" width="18.625" style="10" customWidth="1"/>
     <col min="33" max="33" width="13" style="16" customWidth="1"/>
-    <col min="37" max="38" width="11" style="13"/>
-    <col min="39" max="39" width="15.625" style="13" customWidth="1"/>
-    <col min="40" max="40" width="11" style="13"/>
+    <col min="37" max="40" width="11" style="13"/>
     <col min="41" max="41" width="15.625" style="13" customWidth="1"/>
     <col min="42" max="42" width="11" style="13"/>
-    <col min="51" max="51" width="14" customWidth="1"/>
-    <col min="52" max="52" width="12.375" customWidth="1"/>
-    <col min="53" max="53" width="11.875" customWidth="1"/>
-    <col min="54" max="54" width="10.875" customWidth="1"/>
-    <col min="55" max="55" width="11.5" customWidth="1"/>
+    <col min="43" max="43" width="15.625" style="13" customWidth="1"/>
+    <col min="44" max="44" width="11" style="13"/>
+    <col min="53" max="53" width="14" customWidth="1"/>
+    <col min="54" max="54" width="12.375" customWidth="1"/>
+    <col min="55" max="55" width="11.875" customWidth="1"/>
+    <col min="56" max="56" width="10.875" customWidth="1"/>
+    <col min="57" max="57" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:66" ht="21">
       <c r="A1" s="5"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1106,8 +1179,10 @@
       <c r="BJ1" s="5"/>
       <c r="BK1" s="5"/>
       <c r="BL1" s="5"/>
-    </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM1" s="5"/>
+      <c r="BN1" s="5"/>
+    </row>
+    <row r="2" spans="1:66">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1146,14 +1221,16 @@
       <c r="AN2"/>
       <c r="AO2"/>
       <c r="AP2"/>
-    </row>
-    <row r="3" spans="1:64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AQ2"/>
+      <c r="AR2"/>
+    </row>
+    <row r="3" spans="1:66" ht="15.75" customHeight="1">
       <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1187,8 +1264,10 @@
       <c r="AN3"/>
       <c r="AO3"/>
       <c r="AP3"/>
-    </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AQ3"/>
+      <c r="AR3"/>
+    </row>
+    <row r="4" spans="1:66">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1214,431 +1293,440 @@
       <c r="AE4"/>
       <c r="AF4"/>
       <c r="AG4"/>
-      <c r="AH4" s="31"/>
-      <c r="AI4" s="31"/>
-      <c r="AJ4" s="31"/>
-      <c r="AK4" s="31"/>
-      <c r="AL4"/>
-      <c r="AM4"/>
+      <c r="AH4" s="20"/>
+      <c r="AI4" s="20"/>
+      <c r="AJ4" s="20"/>
+      <c r="AK4" s="20"/>
+      <c r="AL4" s="20"/>
+      <c r="AM4" s="20"/>
       <c r="AN4"/>
       <c r="AO4"/>
       <c r="AP4"/>
-    </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AQ4"/>
+      <c r="AR4"/>
+    </row>
+    <row r="5" spans="1:66">
       <c r="I5"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="28"/>
-      <c r="X5" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA5" s="30"/>
-      <c r="AB5" s="30"/>
-      <c r="AC5" s="30"/>
-      <c r="AD5" s="30"/>
-      <c r="AE5" s="30"/>
-      <c r="AF5" s="30"/>
-      <c r="AG5" s="30"/>
-      <c r="AH5" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI5" s="33"/>
-      <c r="AJ5" s="33"/>
-      <c r="AK5" s="33"/>
-      <c r="AL5" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM5" s="29"/>
-      <c r="AN5" s="29"/>
-      <c r="AO5" s="29"/>
-      <c r="AP5" s="29"/>
-      <c r="AQ5" s="25" t="s">
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="36"/>
+      <c r="Z5" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="33"/>
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="33"/>
+      <c r="AD5" s="33"/>
+      <c r="AE5" s="33"/>
+      <c r="AF5" s="33"/>
+      <c r="AG5" s="33"/>
+      <c r="AH5" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI5" s="34"/>
+      <c r="AJ5" s="34"/>
+      <c r="AK5" s="34"/>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="21"/>
+      <c r="AN5" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO5" s="32"/>
+      <c r="AP5" s="32"/>
+      <c r="AQ5" s="32"/>
+      <c r="AR5" s="32"/>
+      <c r="AS5" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="28"/>
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="28"/>
+      <c r="AX5" s="28"/>
+      <c r="AY5" s="28"/>
+      <c r="AZ5" s="28"/>
+      <c r="BA5" s="28"/>
+      <c r="BB5" s="28"/>
+      <c r="BC5" s="28"/>
+      <c r="BD5" s="28"/>
+      <c r="BE5" s="28"/>
+    </row>
+    <row r="6" spans="1:66" ht="32.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AR5" s="25"/>
-      <c r="AS5" s="25"/>
-      <c r="AT5" s="25"/>
-      <c r="AU5" s="25"/>
-      <c r="AV5" s="25"/>
-      <c r="AW5" s="25"/>
-      <c r="AX5" s="25"/>
-      <c r="AY5" s="25"/>
-      <c r="AZ5" s="25"/>
-      <c r="BA5" s="25"/>
-      <c r="BB5" s="25"/>
-      <c r="BC5" s="25"/>
-    </row>
-    <row r="6" spans="1:64" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="G6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL6" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM6" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="AP6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AV6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="14" t="s">
+      <c r="BA6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF6" s="4" t="s">
+      <c r="BB6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="BD6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AG6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH6" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AQ6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="AR6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="AU6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AV6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="AW6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AX6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AY6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AZ6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="BA6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="BB6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="BC6" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="AM8" s="18"/>
-      <c r="AN8" s="18"/>
-    </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="AM9" s="18"/>
-      <c r="AN9" s="18"/>
-    </row>
-    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:66">
+      <c r="AO8" s="18"/>
+      <c r="AP8" s="18"/>
+    </row>
+    <row r="9" spans="1:66">
+      <c r="AO9" s="18"/>
+      <c r="AP9" s="18"/>
+    </row>
+    <row r="1048519" spans="35:35">
       <c r="AI1048519" s="13"/>
     </row>
-    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="35:35">
       <c r="AI1048520" s="13"/>
     </row>
-    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="35:35">
       <c r="AI1048521" s="13"/>
     </row>
-    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="35:35">
       <c r="AI1048522" s="13"/>
     </row>
-    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="35:35">
       <c r="AI1048523" s="13"/>
     </row>
-    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="35:35">
       <c r="AI1048524" s="13"/>
     </row>
-    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="35:35">
       <c r="AI1048525" s="13"/>
     </row>
-    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="35:35">
       <c r="AI1048526" s="13"/>
     </row>
-    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="35:35">
       <c r="AI1048527" s="13"/>
     </row>
-    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="35:35">
       <c r="AI1048528" s="13"/>
     </row>
-    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="35:35">
       <c r="AI1048529" s="13"/>
     </row>
-    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="35:35">
       <c r="AI1048530" s="13"/>
     </row>
-    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="35:35">
       <c r="AI1048531" s="13"/>
     </row>
-    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="35:35">
       <c r="AI1048532" s="13"/>
     </row>
-    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="35:35">
       <c r="AI1048533" s="13"/>
     </row>
-    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="35:35">
       <c r="AI1048534" s="13"/>
     </row>
-    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="35:35">
       <c r="AI1048535" s="13"/>
     </row>
-    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="35:35">
       <c r="AI1048536" s="13"/>
     </row>
-    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="35:35">
       <c r="AI1048537" s="13"/>
     </row>
-    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="35:35">
       <c r="AI1048538" s="13"/>
     </row>
-    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="35:35">
       <c r="AI1048539" s="13"/>
     </row>
-    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="35:35">
       <c r="AI1048540" s="13"/>
     </row>
-    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="35:35">
       <c r="AI1048541" s="13"/>
     </row>
-    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="35:35">
       <c r="AI1048542" s="13"/>
     </row>
-    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="35:35">
       <c r="AI1048543" s="13"/>
     </row>
-    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="35:35">
       <c r="AI1048544" s="13"/>
     </row>
-    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="35:35">
       <c r="AI1048545" s="13"/>
     </row>
-    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="35:35">
       <c r="AI1048546" s="13"/>
     </row>
-    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="35:35">
       <c r="AI1048547" s="13"/>
     </row>
-    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="35:35">
       <c r="AI1048548" s="13"/>
     </row>
-    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="35:35">
       <c r="AI1048549" s="13"/>
     </row>
-    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="35:35">
       <c r="AI1048550" s="13"/>
     </row>
-    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="35:35">
       <c r="AI1048551" s="13"/>
     </row>
-    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="35:35">
       <c r="AI1048552" s="13"/>
     </row>
-    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="35:35">
       <c r="AI1048553" s="13"/>
     </row>
-    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="35:35">
       <c r="AI1048554" s="13"/>
     </row>
-    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="35:35">
       <c r="AI1048555" s="13"/>
     </row>
-    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="35:35">
       <c r="AI1048556" s="13"/>
     </row>
-    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="35:35">
       <c r="AI1048557" s="13"/>
     </row>
-    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="35:35">
       <c r="AI1048558" s="13"/>
     </row>
-    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="35:35">
       <c r="AI1048559" s="13"/>
     </row>
-    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="35:35">
       <c r="AI1048560" s="13"/>
     </row>
-    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="35:35">
       <c r="AI1048561" s="13"/>
     </row>
-    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="35:35">
       <c r="AI1048562" s="13"/>
     </row>
-    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="35:35">
       <c r="AI1048563" s="13"/>
     </row>
-    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="35:35">
       <c r="AI1048564" s="13"/>
     </row>
-    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="35:35">
       <c r="AI1048565" s="13"/>
     </row>
-    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="35:35">
       <c r="AI1048566" s="13"/>
     </row>
-    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="35:35">
       <c r="AI1048567" s="13"/>
     </row>
-    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="35:35">
       <c r="AI1048568" s="13"/>
     </row>
-    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="35:35">
       <c r="AI1048569" s="13"/>
     </row>
-    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="35:35">
       <c r="AI1048570" s="13"/>
     </row>
-    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="35:35">
       <c r="AI1048571" s="13"/>
     </row>
-    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="35:35">
       <c r="AI1048572" s="13"/>
     </row>
-    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="35:35">
       <c r="AI1048573" s="13"/>
     </row>
-    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048574" spans="35:35">
       <c r="AI1048574" s="13"/>
     </row>
-    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048575" spans="35:35">
       <c r="AI1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AQ5:BC5"/>
+    <mergeCell ref="AS5:BE5"/>
     <mergeCell ref="P5:W5"/>
-    <mergeCell ref="AL5:AP5"/>
+    <mergeCell ref="AN5:AR5"/>
     <mergeCell ref="Z5:AG5"/>
-    <mergeCell ref="AH4:AK4"/>
     <mergeCell ref="AH5:AK5"/>
     <mergeCell ref="X5:Y5"/>
   </mergeCells>
@@ -1649,17 +1737,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W1048573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
@@ -1674,18 +1762,18 @@
     <col min="14" max="14" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+    <row r="1" spans="1:23" ht="21">
+      <c r="B1" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1700,7 +1788,7 @@
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1710,225 +1798,231 @@
       <c r="G2"/>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
+    <row r="3" spans="1:23">
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="32.25">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="1048517" spans="12:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1048517" spans="12:12">
       <c r="L1048517" s="13"/>
     </row>
-    <row r="1048518" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048518" spans="12:12">
       <c r="L1048518" s="13"/>
     </row>
-    <row r="1048519" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="12:12">
       <c r="L1048519" s="13"/>
     </row>
-    <row r="1048520" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="12:12">
       <c r="L1048520" s="13"/>
     </row>
-    <row r="1048521" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="12:12">
       <c r="L1048521" s="13"/>
     </row>
-    <row r="1048522" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="12:12">
       <c r="L1048522" s="13"/>
     </row>
-    <row r="1048523" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="12:12">
       <c r="L1048523" s="13"/>
     </row>
-    <row r="1048524" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="12:12">
       <c r="L1048524" s="13"/>
     </row>
-    <row r="1048525" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="12:12">
       <c r="L1048525" s="13"/>
     </row>
-    <row r="1048526" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="12:12">
       <c r="L1048526" s="13"/>
     </row>
-    <row r="1048527" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="12:12">
       <c r="L1048527" s="13"/>
     </row>
-    <row r="1048528" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="12:12">
       <c r="L1048528" s="13"/>
     </row>
-    <row r="1048529" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="12:12">
       <c r="L1048529" s="13"/>
     </row>
-    <row r="1048530" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="12:12">
       <c r="L1048530" s="13"/>
     </row>
-    <row r="1048531" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="12:12">
       <c r="L1048531" s="13"/>
     </row>
-    <row r="1048532" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="12:12">
       <c r="L1048532" s="13"/>
     </row>
-    <row r="1048533" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="12:12">
       <c r="L1048533" s="13"/>
     </row>
-    <row r="1048534" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="12:12">
       <c r="L1048534" s="13"/>
     </row>
-    <row r="1048535" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="12:12">
       <c r="L1048535" s="13"/>
     </row>
-    <row r="1048536" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="12:12">
       <c r="L1048536" s="13"/>
     </row>
-    <row r="1048537" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="12:12">
       <c r="L1048537" s="13"/>
     </row>
-    <row r="1048538" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="12:12">
       <c r="L1048538" s="13"/>
     </row>
-    <row r="1048539" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="12:12">
       <c r="L1048539" s="13"/>
     </row>
-    <row r="1048540" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="12:12">
       <c r="L1048540" s="13"/>
     </row>
-    <row r="1048541" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="12:12">
       <c r="L1048541" s="13"/>
     </row>
-    <row r="1048542" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="12:12">
       <c r="L1048542" s="13"/>
     </row>
-    <row r="1048543" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="12:12">
       <c r="L1048543" s="13"/>
     </row>
-    <row r="1048544" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="12:12">
       <c r="L1048544" s="13"/>
     </row>
-    <row r="1048545" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="12:12">
       <c r="L1048545" s="13"/>
     </row>
-    <row r="1048546" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="12:12">
       <c r="L1048546" s="13"/>
     </row>
-    <row r="1048547" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="12:12">
       <c r="L1048547" s="13"/>
     </row>
-    <row r="1048548" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="12:12">
       <c r="L1048548" s="13"/>
     </row>
-    <row r="1048549" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="12:12">
       <c r="L1048549" s="13"/>
     </row>
-    <row r="1048550" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="12:12">
       <c r="L1048550" s="13"/>
     </row>
-    <row r="1048551" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="12:12">
       <c r="L1048551" s="13"/>
     </row>
-    <row r="1048552" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="12:12">
       <c r="L1048552" s="13"/>
     </row>
-    <row r="1048553" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="12:12">
       <c r="L1048553" s="13"/>
     </row>
-    <row r="1048554" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="12:12">
       <c r="L1048554" s="13"/>
     </row>
-    <row r="1048555" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="12:12">
       <c r="L1048555" s="13"/>
     </row>
-    <row r="1048556" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="12:12">
       <c r="L1048556" s="13"/>
     </row>
-    <row r="1048557" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="12:12">
       <c r="L1048557" s="13"/>
     </row>
-    <row r="1048558" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="12:12">
       <c r="L1048558" s="13"/>
     </row>
-    <row r="1048559" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="12:12">
       <c r="L1048559" s="13"/>
     </row>
-    <row r="1048560" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="12:12">
       <c r="L1048560" s="13"/>
     </row>
-    <row r="1048561" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="12:12">
       <c r="L1048561" s="13"/>
     </row>
-    <row r="1048562" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="12:12">
       <c r="L1048562" s="13"/>
     </row>
-    <row r="1048563" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="12:12">
       <c r="L1048563" s="13"/>
     </row>
-    <row r="1048564" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="12:12">
       <c r="L1048564" s="13"/>
     </row>
-    <row r="1048565" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="12:12">
       <c r="L1048565" s="13"/>
     </row>
-    <row r="1048566" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="12:12">
       <c r="L1048566" s="13"/>
     </row>
-    <row r="1048567" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="12:12">
       <c r="L1048567" s="13"/>
     </row>
-    <row r="1048568" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="12:12">
       <c r="L1048568" s="13"/>
     </row>
-    <row r="1048569" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="12:12">
       <c r="L1048569" s="13"/>
     </row>
-    <row r="1048570" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="12:12">
       <c r="L1048570" s="13"/>
     </row>
-    <row r="1048571" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="12:12">
       <c r="L1048571" s="13"/>
     </row>
-    <row r="1048572" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="12:12">
       <c r="L1048572" s="13"/>
     </row>
-    <row r="1048573" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="12:12">
       <c r="L1048573" s="13"/>
     </row>
   </sheetData>
@@ -1938,6 +2032,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1946,13 +2041,13 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="3" width="11.625" customWidth="1"/>
@@ -1962,54 +2057,54 @@
     <col min="13" max="13" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="21" customHeight="1">
+      <c r="B1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add columns representing number of units to the desk review workbook (#206)
* Add numbers of units to desk review output

* Make sure that unit numbers are only and always present for 211s and 212s

---------

Co-authored-by: Dan Snow <31494343+dfsnow@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27321"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897A2092-31C1-4E99-B2C2-EC0737924189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{897A2092-31C1-4E99-B2C2-EC0737924189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6D96D48-2A34-4C5C-976E-A22FDC2D12B3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Card Detail" sheetId="4" r:id="rId2"/>
     <sheet name="Comparables" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,6 +41,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jean Cochrane</author>
+    <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
     <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
@@ -67,7 +68,19 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL6" authorId="0" shapeId="0" xr:uid="{0878E9D8-A2FA-4E71-98AD-3CB2F004A791}">
+    <comment ref="AL6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
+      <text>
+        <t>Jean Cochrane (Assessor):
+The number of apartments in a property. Only present for class 211 and class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+      </text>
+    </comment>
+    <comment ref="AM6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
+      <text>
+        <t>Jean Cochrane (Assessor):
+The number of commercial units in a property. Only present for class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+      </text>
+    </comment>
+    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{0878E9D8-A2FA-4E71-98AD-3CB2F004A791}">
       <text>
         <r>
           <rPr>
@@ -91,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
       <text>
         <r>
           <rPr>
@@ -115,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
       <text>
         <r>
           <rPr>
@@ -143,8 +156,48 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean Cochrane (Assessor)</author>
+  </authors>
+  <commentList>
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
+      <text>
+        <t>Jean Cochrane (Assessor):
+The number of apartments in a card. Only present for class 211 and 212 parcels.</t>
+      </text>
+    </comment>
+    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
+      <text>
+        <t>Jean Cochrane (Assessor):
+The number of commercial units in a card. Only present for class 212 parcels.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+  <si>
+    <t>Run ID (res):</t>
+  </si>
+  <si>
+    <t>Change in value</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Characteristics</t>
+  </si>
+  <si>
+    <t>Comparables</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
   <si>
     <t>PIN</t>
   </si>
@@ -152,168 +205,189 @@
     <t>Class</t>
   </si>
   <si>
+    <t>Nbhd.</t>
+  </si>
+  <si>
+    <t>Street Address</t>
+  </si>
+  <si>
+    <t>Municipality</t>
+  </si>
+  <si>
+    <t>Townhome Complex ID</t>
+  </si>
+  <si>
+    <t>PIN Num. Cards</t>
+  </si>
+  <si>
+    <t>Tieback Key PIN</t>
+  </si>
+  <si>
+    <t>Tieback (Proration) Rate</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Lnd. Rate    S. F.</t>
+  </si>
+  <si>
+    <t>Bld. Rate    S. F.</t>
+  </si>
+  <si>
+    <t>Lnd. % of Total</t>
+  </si>
+  <si>
+    <t>Before Rounding</t>
+  </si>
+  <si>
+    <t>Lnd. Rate Original</t>
+  </si>
+  <si>
+    <t>Lnd. Rate     Effective</t>
+  </si>
+  <si>
+    <t>Bld. Rate     S. F.</t>
+  </si>
+  <si>
+    <t>Lnd. % of Tot.</t>
+  </si>
+  <si>
     <t>YoY ∆ $</t>
   </si>
   <si>
     <t>YoY ∆ %</t>
   </si>
   <si>
-    <t>Land</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Lnd. % of Tot.</t>
+    <t>Sale Date 1</t>
+  </si>
+  <si>
+    <t>Sale Amount 1</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 1</t>
+  </si>
+  <si>
+    <t>Sale Doc. 1</t>
+  </si>
+  <si>
+    <t>Sale Date 2</t>
+  </si>
+  <si>
+    <t>Sale Amount 2</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 2</t>
+  </si>
+  <si>
+    <t>Sale Doc. 2</t>
+  </si>
+  <si>
+    <t>Year Built</t>
+  </si>
+  <si>
+    <t>Total        Bld. S. F.</t>
   </si>
   <si>
     <t>Stories</t>
   </si>
   <si>
+    <t>Lnd. S. F.</t>
+  </si>
+  <si>
+    <t># Res. Units</t>
+  </si>
+  <si>
+    <t># Comm. Units</t>
+  </si>
+  <si>
+    <t>Overall Comp. Score</t>
+  </si>
+  <si>
+    <t>Comp. 1 PIN</t>
+  </si>
+  <si>
+    <t>Comp. 1 Score</t>
+  </si>
+  <si>
+    <t>Comp. 2 PIN</t>
+  </si>
+  <si>
+    <t>Comp. 2 Score</t>
+  </si>
+  <si>
+    <t>Is Prorated</t>
+  </si>
+  <si>
+    <t>Proration Error</t>
+  </si>
+  <si>
+    <t>Multi-Card</t>
+  </si>
+  <si>
+    <t>Multi-Land</t>
+  </si>
+  <si>
+    <t>Lnd. &gt;= 95% in Town</t>
+  </si>
+  <si>
+    <t>Bld. &gt;= 95% in Town</t>
+  </si>
+  <si>
+    <t>Land Value Capped</t>
+  </si>
+  <si>
+    <t># Expired 288s</t>
+  </si>
+  <si>
+    <t>Value Unchanged</t>
+  </si>
+  <si>
+    <t>Post-Modeling Change</t>
+  </si>
+  <si>
+    <t>YoY Change &gt;= 50%</t>
+  </si>
+  <si>
+    <t>YoY Change &lt;= -5%</t>
+  </si>
+  <si>
+    <t>Critical Char. Missing</t>
+  </si>
+  <si>
+    <t>Contains only PINs with multiple cards</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Card % Total (By Sqft)</t>
+  </si>
+  <si>
+    <t>Card Initial FMV</t>
+  </si>
+  <si>
+    <t>Card Final FMV</t>
+  </si>
+  <si>
+    <t># Beds</t>
+  </si>
+  <si>
+    <t>Ext. Wall</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
     <t>Bld. S. F.</t>
   </si>
   <si>
-    <t>Lnd. % of Total</t>
-  </si>
-  <si>
-    <t>Bld. Rate     S. F.</t>
-  </si>
-  <si>
-    <t>Flags</t>
-  </si>
-  <si>
-    <t>Proration Error</t>
-  </si>
-  <si>
-    <t>Street Address</t>
-  </si>
-  <si>
-    <t>Municipality</t>
-  </si>
-  <si>
-    <t>Before Rounding</t>
-  </si>
-  <si>
-    <t>Tieback Key PIN</t>
-  </si>
-  <si>
-    <t>PIN Num. Cards</t>
-  </si>
-  <si>
-    <t>Lnd. Rate Original</t>
-  </si>
-  <si>
-    <t>Lnd. Rate     Effective</t>
-  </si>
-  <si>
-    <t>Sale Date 1</t>
-  </si>
-  <si>
-    <t>Sale Amount 1</t>
-  </si>
-  <si>
-    <t>Sale Doc. 1</t>
-  </si>
-  <si>
-    <t>Sale Date 2</t>
-  </si>
-  <si>
-    <t>Sale Amount 2</t>
-  </si>
-  <si>
-    <t>Sale Doc. 2</t>
-  </si>
-  <si>
-    <t>Is Prorated</t>
-  </si>
-  <si>
-    <t>Multi-Land</t>
-  </si>
-  <si>
-    <t>Multi-Card</t>
-  </si>
-  <si>
-    <t>Lnd. &gt;= 95% in Town</t>
-  </si>
-  <si>
-    <t>Bld. &gt;= 95% in Town</t>
-  </si>
-  <si>
-    <t>Land Value Capped</t>
-  </si>
-  <si>
-    <t># Expired 288s</t>
-  </si>
-  <si>
-    <t>Value Unchanged</t>
-  </si>
-  <si>
-    <t>Post-Modeling Change</t>
-  </si>
-  <si>
-    <t>YoY Change &gt;= 50%</t>
-  </si>
-  <si>
-    <t>YoY Change &lt;= -5%</t>
-  </si>
-  <si>
-    <t>Lnd. Rate    S. F.</t>
-  </si>
-  <si>
-    <t>Bld. Rate    S. F.</t>
-  </si>
-  <si>
-    <t>Building</t>
-  </si>
-  <si>
-    <t>Lnd. S. F.</t>
-  </si>
-  <si>
-    <t>Year Built</t>
-  </si>
-  <si>
-    <t>Critical Char. Missing</t>
-  </si>
-  <si>
-    <t>Nbhd.</t>
-  </si>
-  <si>
-    <t>Run ID (res):</t>
-  </si>
-  <si>
-    <t>Card</t>
-  </si>
-  <si>
-    <t>Contains only PINs with multiple cards</t>
-  </si>
-  <si>
-    <t>Card % Total (By Sqft)</t>
-  </si>
-  <si>
-    <t>Card Initial FMV</t>
-  </si>
-  <si>
-    <t>Card Final FMV</t>
-  </si>
-  <si>
-    <t># Beds</t>
-  </si>
-  <si>
-    <t>Ext. Wall</t>
-  </si>
-  <si>
-    <t>Heat</t>
-  </si>
-  <si>
-    <t>Total        Bld. S. F.</t>
-  </si>
-  <si>
-    <t>Townhome Complex ID</t>
-  </si>
-  <si>
-    <t>Tieback (Proration) Rate</t>
-  </si>
-  <si>
     <t>Detail view for comparable sales</t>
   </si>
   <si>
@@ -321,39 +395,6 @@
   </si>
   <si>
     <t>Sale date</t>
-  </si>
-  <si>
-    <t>Non-Arm's-Length Sale Flag 2</t>
-  </si>
-  <si>
-    <t>Non-Arm's-Length Sale Flag 1</t>
-  </si>
-  <si>
-    <t>Overall Comp. Score</t>
-  </si>
-  <si>
-    <t>Comp. 1 PIN</t>
-  </si>
-  <si>
-    <t>Comp. 1 Score</t>
-  </si>
-  <si>
-    <t>Comp. 2 PIN</t>
-  </si>
-  <si>
-    <t>Comp. 2 Score</t>
-  </si>
-  <si>
-    <t>Comparables</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Characteristics</t>
-  </si>
-  <si>
-    <t>Change in value</t>
   </si>
 </sst>
 </file>
@@ -366,7 +407,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -470,7 +511,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -577,6 +618,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -585,7 +646,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -627,6 +688,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -659,17 +729,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -989,16 +1062,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL1048575"/>
+  <dimension ref="A1:BN1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="AF7" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AM19" sqref="AM19"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1029,29 +1102,29 @@
     <col min="31" max="31" width="13" style="10" customWidth="1"/>
     <col min="32" max="32" width="18.625" style="10" customWidth="1"/>
     <col min="33" max="33" width="13" style="16" customWidth="1"/>
-    <col min="37" max="38" width="11" style="13"/>
-    <col min="39" max="39" width="15.625" style="13" customWidth="1"/>
-    <col min="40" max="40" width="11" style="13"/>
+    <col min="37" max="40" width="11" style="13"/>
     <col min="41" max="41" width="15.625" style="13" customWidth="1"/>
     <col min="42" max="42" width="11" style="13"/>
-    <col min="51" max="51" width="14" customWidth="1"/>
-    <col min="52" max="52" width="12.375" customWidth="1"/>
-    <col min="53" max="53" width="11.875" customWidth="1"/>
-    <col min="54" max="54" width="10.875" customWidth="1"/>
-    <col min="55" max="55" width="11.5" customWidth="1"/>
+    <col min="43" max="43" width="15.625" style="13" customWidth="1"/>
+    <col min="44" max="44" width="11" style="13"/>
+    <col min="53" max="53" width="14" customWidth="1"/>
+    <col min="54" max="54" width="12.375" customWidth="1"/>
+    <col min="55" max="55" width="11.875" customWidth="1"/>
+    <col min="56" max="56" width="10.875" customWidth="1"/>
+    <col min="57" max="57" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:66" ht="21">
       <c r="A1" s="5"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1106,8 +1179,10 @@
       <c r="BJ1" s="5"/>
       <c r="BK1" s="5"/>
       <c r="BL1" s="5"/>
-    </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM1" s="5"/>
+      <c r="BN1" s="5"/>
+    </row>
+    <row r="2" spans="1:66">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1146,14 +1221,16 @@
       <c r="AN2"/>
       <c r="AO2"/>
       <c r="AP2"/>
-    </row>
-    <row r="3" spans="1:64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AQ2"/>
+      <c r="AR2"/>
+    </row>
+    <row r="3" spans="1:66" ht="15.75" customHeight="1">
       <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1187,8 +1264,10 @@
       <c r="AN3"/>
       <c r="AO3"/>
       <c r="AP3"/>
-    </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AQ3"/>
+      <c r="AR3"/>
+    </row>
+    <row r="4" spans="1:66">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1214,431 +1293,440 @@
       <c r="AE4"/>
       <c r="AF4"/>
       <c r="AG4"/>
-      <c r="AH4" s="31"/>
-      <c r="AI4" s="31"/>
-      <c r="AJ4" s="31"/>
-      <c r="AK4" s="31"/>
-      <c r="AL4"/>
-      <c r="AM4"/>
+      <c r="AH4" s="20"/>
+      <c r="AI4" s="20"/>
+      <c r="AJ4" s="20"/>
+      <c r="AK4" s="20"/>
+      <c r="AL4" s="20"/>
+      <c r="AM4" s="20"/>
       <c r="AN4"/>
       <c r="AO4"/>
       <c r="AP4"/>
-    </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AQ4"/>
+      <c r="AR4"/>
+    </row>
+    <row r="5" spans="1:66">
       <c r="I5"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="28"/>
-      <c r="X5" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA5" s="30"/>
-      <c r="AB5" s="30"/>
-      <c r="AC5" s="30"/>
-      <c r="AD5" s="30"/>
-      <c r="AE5" s="30"/>
-      <c r="AF5" s="30"/>
-      <c r="AG5" s="30"/>
-      <c r="AH5" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI5" s="33"/>
-      <c r="AJ5" s="33"/>
-      <c r="AK5" s="33"/>
-      <c r="AL5" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM5" s="29"/>
-      <c r="AN5" s="29"/>
-      <c r="AO5" s="29"/>
-      <c r="AP5" s="29"/>
-      <c r="AQ5" s="25" t="s">
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="36"/>
+      <c r="Z5" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="33"/>
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="33"/>
+      <c r="AD5" s="33"/>
+      <c r="AE5" s="33"/>
+      <c r="AF5" s="33"/>
+      <c r="AG5" s="33"/>
+      <c r="AH5" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI5" s="34"/>
+      <c r="AJ5" s="34"/>
+      <c r="AK5" s="34"/>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="21"/>
+      <c r="AN5" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO5" s="32"/>
+      <c r="AP5" s="32"/>
+      <c r="AQ5" s="32"/>
+      <c r="AR5" s="32"/>
+      <c r="AS5" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="28"/>
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="28"/>
+      <c r="AX5" s="28"/>
+      <c r="AY5" s="28"/>
+      <c r="AZ5" s="28"/>
+      <c r="BA5" s="28"/>
+      <c r="BB5" s="28"/>
+      <c r="BC5" s="28"/>
+      <c r="BD5" s="28"/>
+      <c r="BE5" s="28"/>
+    </row>
+    <row r="6" spans="1:66" ht="32.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AR5" s="25"/>
-      <c r="AS5" s="25"/>
-      <c r="AT5" s="25"/>
-      <c r="AU5" s="25"/>
-      <c r="AV5" s="25"/>
-      <c r="AW5" s="25"/>
-      <c r="AX5" s="25"/>
-      <c r="AY5" s="25"/>
-      <c r="AZ5" s="25"/>
-      <c r="BA5" s="25"/>
-      <c r="BB5" s="25"/>
-      <c r="BC5" s="25"/>
-    </row>
-    <row r="6" spans="1:64" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="G6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL6" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM6" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="AP6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AV6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="14" t="s">
+      <c r="BA6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF6" s="4" t="s">
+      <c r="BB6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="BD6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AG6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH6" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AQ6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="AR6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="AU6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AV6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="AW6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AX6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AY6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AZ6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="BA6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="BB6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="BC6" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="AM8" s="18"/>
-      <c r="AN8" s="18"/>
-    </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="AM9" s="18"/>
-      <c r="AN9" s="18"/>
-    </row>
-    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:66">
+      <c r="AO8" s="18"/>
+      <c r="AP8" s="18"/>
+    </row>
+    <row r="9" spans="1:66">
+      <c r="AO9" s="18"/>
+      <c r="AP9" s="18"/>
+    </row>
+    <row r="1048519" spans="35:35">
       <c r="AI1048519" s="13"/>
     </row>
-    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="35:35">
       <c r="AI1048520" s="13"/>
     </row>
-    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="35:35">
       <c r="AI1048521" s="13"/>
     </row>
-    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="35:35">
       <c r="AI1048522" s="13"/>
     </row>
-    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="35:35">
       <c r="AI1048523" s="13"/>
     </row>
-    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="35:35">
       <c r="AI1048524" s="13"/>
     </row>
-    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="35:35">
       <c r="AI1048525" s="13"/>
     </row>
-    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="35:35">
       <c r="AI1048526" s="13"/>
     </row>
-    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="35:35">
       <c r="AI1048527" s="13"/>
     </row>
-    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="35:35">
       <c r="AI1048528" s="13"/>
     </row>
-    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="35:35">
       <c r="AI1048529" s="13"/>
     </row>
-    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="35:35">
       <c r="AI1048530" s="13"/>
     </row>
-    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="35:35">
       <c r="AI1048531" s="13"/>
     </row>
-    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="35:35">
       <c r="AI1048532" s="13"/>
     </row>
-    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="35:35">
       <c r="AI1048533" s="13"/>
     </row>
-    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="35:35">
       <c r="AI1048534" s="13"/>
     </row>
-    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="35:35">
       <c r="AI1048535" s="13"/>
     </row>
-    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="35:35">
       <c r="AI1048536" s="13"/>
     </row>
-    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="35:35">
       <c r="AI1048537" s="13"/>
     </row>
-    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="35:35">
       <c r="AI1048538" s="13"/>
     </row>
-    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="35:35">
       <c r="AI1048539" s="13"/>
     </row>
-    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="35:35">
       <c r="AI1048540" s="13"/>
     </row>
-    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="35:35">
       <c r="AI1048541" s="13"/>
     </row>
-    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="35:35">
       <c r="AI1048542" s="13"/>
     </row>
-    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="35:35">
       <c r="AI1048543" s="13"/>
     </row>
-    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="35:35">
       <c r="AI1048544" s="13"/>
     </row>
-    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="35:35">
       <c r="AI1048545" s="13"/>
     </row>
-    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="35:35">
       <c r="AI1048546" s="13"/>
     </row>
-    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="35:35">
       <c r="AI1048547" s="13"/>
     </row>
-    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="35:35">
       <c r="AI1048548" s="13"/>
     </row>
-    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="35:35">
       <c r="AI1048549" s="13"/>
     </row>
-    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="35:35">
       <c r="AI1048550" s="13"/>
     </row>
-    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="35:35">
       <c r="AI1048551" s="13"/>
     </row>
-    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="35:35">
       <c r="AI1048552" s="13"/>
     </row>
-    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="35:35">
       <c r="AI1048553" s="13"/>
     </row>
-    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="35:35">
       <c r="AI1048554" s="13"/>
     </row>
-    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="35:35">
       <c r="AI1048555" s="13"/>
     </row>
-    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="35:35">
       <c r="AI1048556" s="13"/>
     </row>
-    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="35:35">
       <c r="AI1048557" s="13"/>
     </row>
-    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="35:35">
       <c r="AI1048558" s="13"/>
     </row>
-    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="35:35">
       <c r="AI1048559" s="13"/>
     </row>
-    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="35:35">
       <c r="AI1048560" s="13"/>
     </row>
-    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="35:35">
       <c r="AI1048561" s="13"/>
     </row>
-    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="35:35">
       <c r="AI1048562" s="13"/>
     </row>
-    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="35:35">
       <c r="AI1048563" s="13"/>
     </row>
-    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="35:35">
       <c r="AI1048564" s="13"/>
     </row>
-    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="35:35">
       <c r="AI1048565" s="13"/>
     </row>
-    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="35:35">
       <c r="AI1048566" s="13"/>
     </row>
-    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="35:35">
       <c r="AI1048567" s="13"/>
     </row>
-    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="35:35">
       <c r="AI1048568" s="13"/>
     </row>
-    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="35:35">
       <c r="AI1048569" s="13"/>
     </row>
-    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="35:35">
       <c r="AI1048570" s="13"/>
     </row>
-    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="35:35">
       <c r="AI1048571" s="13"/>
     </row>
-    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="35:35">
       <c r="AI1048572" s="13"/>
     </row>
-    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="35:35">
       <c r="AI1048573" s="13"/>
     </row>
-    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048574" spans="35:35">
       <c r="AI1048574" s="13"/>
     </row>
-    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
+    <row r="1048575" spans="35:35">
       <c r="AI1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AQ5:BC5"/>
+    <mergeCell ref="AS5:BE5"/>
     <mergeCell ref="P5:W5"/>
-    <mergeCell ref="AL5:AP5"/>
+    <mergeCell ref="AN5:AR5"/>
     <mergeCell ref="Z5:AG5"/>
-    <mergeCell ref="AH4:AK4"/>
     <mergeCell ref="AH5:AK5"/>
     <mergeCell ref="X5:Y5"/>
   </mergeCells>
@@ -1649,17 +1737,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W1048573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
@@ -1674,18 +1762,18 @@
     <col min="14" max="14" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+    <row r="1" spans="1:23" ht="21">
+      <c r="B1" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1700,7 +1788,7 @@
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1710,225 +1798,231 @@
       <c r="G2"/>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
+    <row r="3" spans="1:23">
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="32.25">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="1048517" spans="12:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1048517" spans="12:12">
       <c r="L1048517" s="13"/>
     </row>
-    <row r="1048518" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048518" spans="12:12">
       <c r="L1048518" s="13"/>
     </row>
-    <row r="1048519" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="12:12">
       <c r="L1048519" s="13"/>
     </row>
-    <row r="1048520" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="12:12">
       <c r="L1048520" s="13"/>
     </row>
-    <row r="1048521" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="12:12">
       <c r="L1048521" s="13"/>
     </row>
-    <row r="1048522" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="12:12">
       <c r="L1048522" s="13"/>
     </row>
-    <row r="1048523" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="12:12">
       <c r="L1048523" s="13"/>
     </row>
-    <row r="1048524" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="12:12">
       <c r="L1048524" s="13"/>
     </row>
-    <row r="1048525" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="12:12">
       <c r="L1048525" s="13"/>
     </row>
-    <row r="1048526" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="12:12">
       <c r="L1048526" s="13"/>
     </row>
-    <row r="1048527" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="12:12">
       <c r="L1048527" s="13"/>
     </row>
-    <row r="1048528" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="12:12">
       <c r="L1048528" s="13"/>
     </row>
-    <row r="1048529" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="12:12">
       <c r="L1048529" s="13"/>
     </row>
-    <row r="1048530" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="12:12">
       <c r="L1048530" s="13"/>
     </row>
-    <row r="1048531" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="12:12">
       <c r="L1048531" s="13"/>
     </row>
-    <row r="1048532" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="12:12">
       <c r="L1048532" s="13"/>
     </row>
-    <row r="1048533" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="12:12">
       <c r="L1048533" s="13"/>
     </row>
-    <row r="1048534" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="12:12">
       <c r="L1048534" s="13"/>
     </row>
-    <row r="1048535" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="12:12">
       <c r="L1048535" s="13"/>
     </row>
-    <row r="1048536" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="12:12">
       <c r="L1048536" s="13"/>
     </row>
-    <row r="1048537" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="12:12">
       <c r="L1048537" s="13"/>
     </row>
-    <row r="1048538" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="12:12">
       <c r="L1048538" s="13"/>
     </row>
-    <row r="1048539" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="12:12">
       <c r="L1048539" s="13"/>
     </row>
-    <row r="1048540" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="12:12">
       <c r="L1048540" s="13"/>
     </row>
-    <row r="1048541" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="12:12">
       <c r="L1048541" s="13"/>
     </row>
-    <row r="1048542" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="12:12">
       <c r="L1048542" s="13"/>
     </row>
-    <row r="1048543" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="12:12">
       <c r="L1048543" s="13"/>
     </row>
-    <row r="1048544" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="12:12">
       <c r="L1048544" s="13"/>
     </row>
-    <row r="1048545" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="12:12">
       <c r="L1048545" s="13"/>
     </row>
-    <row r="1048546" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="12:12">
       <c r="L1048546" s="13"/>
     </row>
-    <row r="1048547" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="12:12">
       <c r="L1048547" s="13"/>
     </row>
-    <row r="1048548" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="12:12">
       <c r="L1048548" s="13"/>
     </row>
-    <row r="1048549" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="12:12">
       <c r="L1048549" s="13"/>
     </row>
-    <row r="1048550" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="12:12">
       <c r="L1048550" s="13"/>
     </row>
-    <row r="1048551" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="12:12">
       <c r="L1048551" s="13"/>
     </row>
-    <row r="1048552" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="12:12">
       <c r="L1048552" s="13"/>
     </row>
-    <row r="1048553" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="12:12">
       <c r="L1048553" s="13"/>
     </row>
-    <row r="1048554" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="12:12">
       <c r="L1048554" s="13"/>
     </row>
-    <row r="1048555" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="12:12">
       <c r="L1048555" s="13"/>
     </row>
-    <row r="1048556" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="12:12">
       <c r="L1048556" s="13"/>
     </row>
-    <row r="1048557" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="12:12">
       <c r="L1048557" s="13"/>
     </row>
-    <row r="1048558" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="12:12">
       <c r="L1048558" s="13"/>
     </row>
-    <row r="1048559" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="12:12">
       <c r="L1048559" s="13"/>
     </row>
-    <row r="1048560" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="12:12">
       <c r="L1048560" s="13"/>
     </row>
-    <row r="1048561" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="12:12">
       <c r="L1048561" s="13"/>
     </row>
-    <row r="1048562" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="12:12">
       <c r="L1048562" s="13"/>
     </row>
-    <row r="1048563" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="12:12">
       <c r="L1048563" s="13"/>
     </row>
-    <row r="1048564" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="12:12">
       <c r="L1048564" s="13"/>
     </row>
-    <row r="1048565" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="12:12">
       <c r="L1048565" s="13"/>
     </row>
-    <row r="1048566" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="12:12">
       <c r="L1048566" s="13"/>
     </row>
-    <row r="1048567" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="12:12">
       <c r="L1048567" s="13"/>
     </row>
-    <row r="1048568" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="12:12">
       <c r="L1048568" s="13"/>
     </row>
-    <row r="1048569" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="12:12">
       <c r="L1048569" s="13"/>
     </row>
-    <row r="1048570" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="12:12">
       <c r="L1048570" s="13"/>
     </row>
-    <row r="1048571" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="12:12">
       <c r="L1048571" s="13"/>
     </row>
-    <row r="1048572" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="12:12">
       <c r="L1048572" s="13"/>
     </row>
-    <row r="1048573" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="12:12">
       <c r="L1048573" s="13"/>
     </row>
   </sheetData>
@@ -1938,6 +2032,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1946,13 +2041,13 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="3" width="11.625" customWidth="1"/>
@@ -1962,54 +2057,54 @@
     <col min="13" max="13" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="21" customHeight="1">
+      <c r="B1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update DR template notes and headings
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27321"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{897A2092-31C1-4E99-B2C2-EC0737924189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6D96D48-2A34-4C5C-976E-A22FDC2D12B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518B7432-B237-4DFB-B6D2-C536D5B9FFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,59 +48,55 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Jean Cochrane:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm. If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
+          <t>This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm.
+If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
         </r>
       </text>
     </comment>
     <comment ref="AL6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
       <text>
-        <t>Jean Cochrane (Assessor):
-The number of apartments in a property. Only present for class 211 and class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The number of apartments in a property. Only present for class 211 and class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+        </r>
       </text>
     </comment>
     <comment ref="AM6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
       <text>
-        <t>Jean Cochrane (Assessor):
-The number of commercial units in a property. Only present for class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The number of commercial units in a property. Only present for class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+        </r>
       </text>
     </comment>
     <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{0878E9D8-A2FA-4E71-98AD-3CB2F004A791}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Jean Cochrane:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This column represents the average similarity score for all of the comparable parcels we extracted for this property based on the model structure. (The first two comps are shown in subsequent columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
+          <t>This column represents the average similarity score for all of the comparable parcels we extracted for this property based on the model structure. (The first two comps are shown in subsequent columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
         </r>
       </text>
     </comment>
@@ -108,23 +104,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Jean Cochrane:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
+          <t>This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
         </r>
       </text>
     </comment>
@@ -132,23 +118,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Jean Cochrane:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This column represents the similarity score for this comparable sale, which we can interpret as the percent confidence that the model has that the parcel sold in this sale is comparable to the target parcel.</t>
+          <t>This column represents the similarity score for this comparable sale, which we can interpret as the percent confidence that the model has that the parcel sold in this sale is comparable to the target parcel.</t>
         </r>
       </text>
     </comment>
@@ -164,14 +140,30 @@
   <commentList>
     <comment ref="O4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
       <text>
-        <t>Jean Cochrane (Assessor):
-The number of apartments in a card. Only present for class 211 and 212 parcels.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The number of apartments in a card. Only present for class 211 and 212 parcels.</t>
+        </r>
       </text>
     </comment>
     <comment ref="P4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
       <text>
-        <t>Jean Cochrane (Assessor):
-The number of commercial units in a card. Only present for class 212 parcels.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The number of commercial units in a card. Only present for class 212 parcels.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -179,17 +171,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
   <si>
     <t>Run ID (res):</t>
   </si>
   <si>
-    <t>Change in value</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
     <t>Characteristics</t>
   </si>
   <si>
@@ -391,10 +377,25 @@
     <t>Detail view for comparable sales</t>
   </si>
   <si>
-    <t>Sale price</t>
-  </si>
-  <si>
-    <t>Sale date</t>
+    <t>PIN Information</t>
+  </si>
+  <si>
+    <t>Change In Value</t>
+  </si>
+  <si>
+    <t>Card Information</t>
+  </si>
+  <si>
+    <t>Card Characteristics</t>
+  </si>
+  <si>
+    <t>Sale Price</t>
+  </si>
+  <si>
+    <t>Sale Date</t>
+  </si>
+  <si>
+    <t>Sales Information</t>
   </si>
 </sst>
 </file>
@@ -407,7 +408,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -419,13 +420,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -461,13 +455,28 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,8 +519,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9CCFC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -620,33 +635,22 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -658,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -683,66 +687,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="37" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="37" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -754,6 +785,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF9CCFC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1065,13 +1101,13 @@
   <dimension ref="A1:BN1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="AF7" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AM19" sqref="AM19"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1114,17 +1150,17 @@
     <col min="57" max="57" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="21">
+    <row r="1" spans="1:66" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1182,7 +1218,7 @@
       <c r="BM1" s="5"/>
       <c r="BN1" s="5"/>
     </row>
-    <row r="2" spans="1:66">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1224,13 +1260,13 @@
       <c r="AQ2"/>
       <c r="AR2"/>
     </row>
-    <row r="3" spans="1:66" ht="15.75" customHeight="1">
+    <row r="3" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1267,7 +1303,7 @@
       <c r="AQ3"/>
       <c r="AR3"/>
     </row>
-    <row r="4" spans="1:66">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1305,421 +1341,430 @@
       <c r="AQ4"/>
       <c r="AR4"/>
     </row>
-    <row r="5" spans="1:66">
-      <c r="I5"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="30"/>
-      <c r="V5" s="30"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="35" t="s">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="B5" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="42"/>
+      <c r="X5" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA5" s="38"/>
+      <c r="AB5" s="38"/>
+      <c r="AC5" s="38"/>
+      <c r="AD5" s="38"/>
+      <c r="AE5" s="38"/>
+      <c r="AF5" s="38"/>
+      <c r="AG5" s="39"/>
+      <c r="AH5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="Y5" s="36"/>
-      <c r="Z5" s="33" t="s">
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="35"/>
+      <c r="AL5" s="35"/>
+      <c r="AM5" s="36"/>
+      <c r="AN5" s="31" t="s">
         <v>2</v>
-      </c>
-      <c r="AA5" s="33"/>
-      <c r="AB5" s="33"/>
-      <c r="AC5" s="33"/>
-      <c r="AD5" s="33"/>
-      <c r="AE5" s="33"/>
-      <c r="AF5" s="33"/>
-      <c r="AG5" s="33"/>
-      <c r="AH5" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI5" s="34"/>
-      <c r="AJ5" s="34"/>
-      <c r="AK5" s="34"/>
-      <c r="AL5" s="21"/>
-      <c r="AM5" s="21"/>
-      <c r="AN5" s="32" t="s">
-        <v>4</v>
       </c>
       <c r="AO5" s="32"/>
       <c r="AP5" s="32"/>
       <c r="AQ5" s="32"/>
-      <c r="AR5" s="32"/>
+      <c r="AR5" s="33"/>
       <c r="AS5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT5" s="29"/>
+      <c r="AU5" s="29"/>
+      <c r="AV5" s="29"/>
+      <c r="AW5" s="29"/>
+      <c r="AX5" s="29"/>
+      <c r="AY5" s="29"/>
+      <c r="AZ5" s="29"/>
+      <c r="BA5" s="29"/>
+      <c r="BB5" s="29"/>
+      <c r="BC5" s="29"/>
+      <c r="BD5" s="29"/>
+      <c r="BE5" s="30"/>
+    </row>
+    <row r="6" spans="1:66" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AT5" s="28"/>
-      <c r="AU5" s="28"/>
-      <c r="AV5" s="28"/>
-      <c r="AW5" s="28"/>
-      <c r="AX5" s="28"/>
-      <c r="AY5" s="28"/>
-      <c r="AZ5" s="28"/>
-      <c r="BA5" s="28"/>
-      <c r="BB5" s="28"/>
-      <c r="BC5" s="28"/>
-      <c r="BD5" s="28"/>
-      <c r="BE5" s="28"/>
-    </row>
-    <row r="6" spans="1:66" ht="32.25">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="I6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="J6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="K6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="O6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="P6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="Q6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="U6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="T6" s="6" t="s">
+      <c r="V6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="W6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="X6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="W6" s="7" t="s">
+      <c r="Y6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="Z6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="AA6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AB6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AC6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AD6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AE6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AF6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AG6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AF6" s="4" t="s">
+      <c r="AH6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AI6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AH6" s="19" t="s">
+      <c r="AJ6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AI6" s="6" t="s">
+      <c r="AK6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AJ6" s="6" t="s">
+      <c r="AL6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AK6" s="6" t="s">
+      <c r="AM6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AL6" s="22" t="s">
+      <c r="AN6" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AM6" s="22" t="s">
+      <c r="AO6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AN6" s="17" t="s">
+      <c r="AP6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AO6" s="8" t="s">
+      <c r="AQ6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AP6" s="8" t="s">
+      <c r="AR6" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AQ6" s="8" t="s">
+      <c r="AS6" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="AR6" s="14" t="s">
+      <c r="AT6" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="AS6" s="8" t="s">
+      <c r="AU6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AT6" s="8" t="s">
+      <c r="AV6" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="AU6" s="8" t="s">
+      <c r="AW6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="AV6" s="8" t="s">
+      <c r="AX6" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="AW6" s="8" t="s">
+      <c r="AY6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AX6" s="8" t="s">
+      <c r="AZ6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AY6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AZ6" s="8" t="s">
+      <c r="BB6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BC6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="BD6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE6" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:66">
+    </row>
+    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="AO8" s="18"/>
       <c r="AP8" s="18"/>
     </row>
-    <row r="9" spans="1:66">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
       <c r="AO9" s="18"/>
       <c r="AP9" s="18"/>
     </row>
-    <row r="1048519" spans="35:35">
+    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048519" s="13"/>
     </row>
-    <row r="1048520" spans="35:35">
+    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048520" s="13"/>
     </row>
-    <row r="1048521" spans="35:35">
+    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048521" s="13"/>
     </row>
-    <row r="1048522" spans="35:35">
+    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048522" s="13"/>
     </row>
-    <row r="1048523" spans="35:35">
+    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048523" s="13"/>
     </row>
-    <row r="1048524" spans="35:35">
+    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048524" s="13"/>
     </row>
-    <row r="1048525" spans="35:35">
+    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048525" s="13"/>
     </row>
-    <row r="1048526" spans="35:35">
+    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048526" s="13"/>
     </row>
-    <row r="1048527" spans="35:35">
+    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048527" s="13"/>
     </row>
-    <row r="1048528" spans="35:35">
+    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048528" s="13"/>
     </row>
-    <row r="1048529" spans="35:35">
+    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048529" s="13"/>
     </row>
-    <row r="1048530" spans="35:35">
+    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048530" s="13"/>
     </row>
-    <row r="1048531" spans="35:35">
+    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048531" s="13"/>
     </row>
-    <row r="1048532" spans="35:35">
+    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048532" s="13"/>
     </row>
-    <row r="1048533" spans="35:35">
+    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048533" s="13"/>
     </row>
-    <row r="1048534" spans="35:35">
+    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048534" s="13"/>
     </row>
-    <row r="1048535" spans="35:35">
+    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048535" s="13"/>
     </row>
-    <row r="1048536" spans="35:35">
+    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048536" s="13"/>
     </row>
-    <row r="1048537" spans="35:35">
+    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048537" s="13"/>
     </row>
-    <row r="1048538" spans="35:35">
+    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048538" s="13"/>
     </row>
-    <row r="1048539" spans="35:35">
+    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048539" s="13"/>
     </row>
-    <row r="1048540" spans="35:35">
+    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048540" s="13"/>
     </row>
-    <row r="1048541" spans="35:35">
+    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048541" s="13"/>
     </row>
-    <row r="1048542" spans="35:35">
+    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048542" s="13"/>
     </row>
-    <row r="1048543" spans="35:35">
+    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048543" s="13"/>
     </row>
-    <row r="1048544" spans="35:35">
+    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048544" s="13"/>
     </row>
-    <row r="1048545" spans="35:35">
+    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048545" s="13"/>
     </row>
-    <row r="1048546" spans="35:35">
+    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048546" s="13"/>
     </row>
-    <row r="1048547" spans="35:35">
+    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048547" s="13"/>
     </row>
-    <row r="1048548" spans="35:35">
+    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048548" s="13"/>
     </row>
-    <row r="1048549" spans="35:35">
+    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048549" s="13"/>
     </row>
-    <row r="1048550" spans="35:35">
+    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048550" s="13"/>
     </row>
-    <row r="1048551" spans="35:35">
+    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048551" s="13"/>
     </row>
-    <row r="1048552" spans="35:35">
+    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048552" s="13"/>
     </row>
-    <row r="1048553" spans="35:35">
+    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048553" s="13"/>
     </row>
-    <row r="1048554" spans="35:35">
+    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048554" s="13"/>
     </row>
-    <row r="1048555" spans="35:35">
+    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048555" s="13"/>
     </row>
-    <row r="1048556" spans="35:35">
+    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048556" s="13"/>
     </row>
-    <row r="1048557" spans="35:35">
+    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048557" s="13"/>
     </row>
-    <row r="1048558" spans="35:35">
+    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048558" s="13"/>
     </row>
-    <row r="1048559" spans="35:35">
+    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048559" s="13"/>
     </row>
-    <row r="1048560" spans="35:35">
+    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048560" s="13"/>
     </row>
-    <row r="1048561" spans="35:35">
+    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048561" s="13"/>
     </row>
-    <row r="1048562" spans="35:35">
+    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048562" s="13"/>
     </row>
-    <row r="1048563" spans="35:35">
+    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048563" s="13"/>
     </row>
-    <row r="1048564" spans="35:35">
+    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048564" s="13"/>
     </row>
-    <row r="1048565" spans="35:35">
+    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048565" s="13"/>
     </row>
-    <row r="1048566" spans="35:35">
+    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048566" s="13"/>
     </row>
-    <row r="1048567" spans="35:35">
+    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048567" s="13"/>
     </row>
-    <row r="1048568" spans="35:35">
+    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048568" s="13"/>
     </row>
-    <row r="1048569" spans="35:35">
+    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048569" s="13"/>
     </row>
-    <row r="1048570" spans="35:35">
+    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048570" s="13"/>
     </row>
-    <row r="1048571" spans="35:35">
+    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048571" s="13"/>
     </row>
-    <row r="1048572" spans="35:35">
+    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048572" s="13"/>
     </row>
-    <row r="1048573" spans="35:35">
+    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048573" s="13"/>
     </row>
-    <row r="1048574" spans="35:35">
+    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048574" s="13"/>
     </row>
-    <row r="1048575" spans="35:35">
+    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
@@ -1727,8 +1772,9 @@
     <mergeCell ref="P5:W5"/>
     <mergeCell ref="AN5:AR5"/>
     <mergeCell ref="Z5:AG5"/>
-    <mergeCell ref="AH5:AK5"/>
     <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="AH5:AM5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1742,12 +1788,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
@@ -1762,18 +1808,18 @@
     <col min="14" max="14" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21">
-      <c r="B1" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1788,7 +1834,7 @@
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1798,237 +1844,254 @@
       <c r="G2"/>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:23">
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="N3"/>
-    </row>
-    <row r="4" spans="1:23" ht="32.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="36"/>
+    </row>
+    <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="E4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="G4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="H4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="J4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="K4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="P4" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" s="38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="1048517" spans="12:12">
+    </row>
+    <row r="1048517" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048517" s="13"/>
     </row>
-    <row r="1048518" spans="12:12">
+    <row r="1048518" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048518" s="13"/>
     </row>
-    <row r="1048519" spans="12:12">
+    <row r="1048519" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048519" s="13"/>
     </row>
-    <row r="1048520" spans="12:12">
+    <row r="1048520" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048520" s="13"/>
     </row>
-    <row r="1048521" spans="12:12">
+    <row r="1048521" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048521" s="13"/>
     </row>
-    <row r="1048522" spans="12:12">
+    <row r="1048522" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048522" s="13"/>
     </row>
-    <row r="1048523" spans="12:12">
+    <row r="1048523" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048523" s="13"/>
     </row>
-    <row r="1048524" spans="12:12">
+    <row r="1048524" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048524" s="13"/>
     </row>
-    <row r="1048525" spans="12:12">
+    <row r="1048525" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048525" s="13"/>
     </row>
-    <row r="1048526" spans="12:12">
+    <row r="1048526" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048526" s="13"/>
     </row>
-    <row r="1048527" spans="12:12">
+    <row r="1048527" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048527" s="13"/>
     </row>
-    <row r="1048528" spans="12:12">
+    <row r="1048528" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048528" s="13"/>
     </row>
-    <row r="1048529" spans="12:12">
+    <row r="1048529" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048529" s="13"/>
     </row>
-    <row r="1048530" spans="12:12">
+    <row r="1048530" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048530" s="13"/>
     </row>
-    <row r="1048531" spans="12:12">
+    <row r="1048531" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048531" s="13"/>
     </row>
-    <row r="1048532" spans="12:12">
+    <row r="1048532" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048532" s="13"/>
     </row>
-    <row r="1048533" spans="12:12">
+    <row r="1048533" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048533" s="13"/>
     </row>
-    <row r="1048534" spans="12:12">
+    <row r="1048534" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048534" s="13"/>
     </row>
-    <row r="1048535" spans="12:12">
+    <row r="1048535" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048535" s="13"/>
     </row>
-    <row r="1048536" spans="12:12">
+    <row r="1048536" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048536" s="13"/>
     </row>
-    <row r="1048537" spans="12:12">
+    <row r="1048537" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048537" s="13"/>
     </row>
-    <row r="1048538" spans="12:12">
+    <row r="1048538" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048538" s="13"/>
     </row>
-    <row r="1048539" spans="12:12">
+    <row r="1048539" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048539" s="13"/>
     </row>
-    <row r="1048540" spans="12:12">
+    <row r="1048540" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048540" s="13"/>
     </row>
-    <row r="1048541" spans="12:12">
+    <row r="1048541" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048541" s="13"/>
     </row>
-    <row r="1048542" spans="12:12">
+    <row r="1048542" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048542" s="13"/>
     </row>
-    <row r="1048543" spans="12:12">
+    <row r="1048543" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048543" s="13"/>
     </row>
-    <row r="1048544" spans="12:12">
+    <row r="1048544" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048544" s="13"/>
     </row>
-    <row r="1048545" spans="12:12">
+    <row r="1048545" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048545" s="13"/>
     </row>
-    <row r="1048546" spans="12:12">
+    <row r="1048546" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048546" s="13"/>
     </row>
-    <row r="1048547" spans="12:12">
+    <row r="1048547" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048547" s="13"/>
     </row>
-    <row r="1048548" spans="12:12">
+    <row r="1048548" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048548" s="13"/>
     </row>
-    <row r="1048549" spans="12:12">
+    <row r="1048549" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048549" s="13"/>
     </row>
-    <row r="1048550" spans="12:12">
+    <row r="1048550" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048550" s="13"/>
     </row>
-    <row r="1048551" spans="12:12">
+    <row r="1048551" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048551" s="13"/>
     </row>
-    <row r="1048552" spans="12:12">
+    <row r="1048552" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048552" s="13"/>
     </row>
-    <row r="1048553" spans="12:12">
+    <row r="1048553" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048553" s="13"/>
     </row>
-    <row r="1048554" spans="12:12">
+    <row r="1048554" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048554" s="13"/>
     </row>
-    <row r="1048555" spans="12:12">
+    <row r="1048555" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048555" s="13"/>
     </row>
-    <row r="1048556" spans="12:12">
+    <row r="1048556" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048556" s="13"/>
     </row>
-    <row r="1048557" spans="12:12">
+    <row r="1048557" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048557" s="13"/>
     </row>
-    <row r="1048558" spans="12:12">
+    <row r="1048558" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048558" s="13"/>
     </row>
-    <row r="1048559" spans="12:12">
+    <row r="1048559" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048559" s="13"/>
     </row>
-    <row r="1048560" spans="12:12">
+    <row r="1048560" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048560" s="13"/>
     </row>
-    <row r="1048561" spans="12:12">
+    <row r="1048561" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048561" s="13"/>
     </row>
-    <row r="1048562" spans="12:12">
+    <row r="1048562" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048562" s="13"/>
     </row>
-    <row r="1048563" spans="12:12">
+    <row r="1048563" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048563" s="13"/>
     </row>
-    <row r="1048564" spans="12:12">
+    <row r="1048564" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048564" s="13"/>
     </row>
-    <row r="1048565" spans="12:12">
+    <row r="1048565" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048565" s="13"/>
     </row>
-    <row r="1048566" spans="12:12">
+    <row r="1048566" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048566" s="13"/>
     </row>
-    <row r="1048567" spans="12:12">
+    <row r="1048567" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048567" s="13"/>
     </row>
-    <row r="1048568" spans="12:12">
+    <row r="1048568" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048568" s="13"/>
     </row>
-    <row r="1048569" spans="12:12">
+    <row r="1048569" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048569" s="13"/>
     </row>
-    <row r="1048570" spans="12:12">
+    <row r="1048570" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048570" s="13"/>
     </row>
-    <row r="1048571" spans="12:12">
+    <row r="1048571" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048571" s="13"/>
     </row>
-    <row r="1048572" spans="12:12">
+    <row r="1048572" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048572" s="13"/>
     </row>
-    <row r="1048573" spans="12:12">
+    <row r="1048573" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048573" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2041,75 +2104,99 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="3" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="24.375" customWidth="1"/>
+    <col min="6" max="6" width="26.625" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
     <col min="9" max="10" width="15.625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="13" max="13" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1">
-      <c r="B1" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-    </row>
-    <row r="4" spans="1:13" ht="32.25" customHeight="1">
+    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="36"/>
+    </row>
+    <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="M4" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix final 2024 res model export issues (#209)
* Fix building-level unprorated predicted value calculation

It took me literally all day to figure out this single change for
multi-card prorated PINs

* Fix missing var and typos in comps report section

* Coerce n_years_exe to int to maintain Athena schema

* Set final 2024 res run for export

* Set final parameter values for 2024

* Update DR template notes and headings

* Swap card sheet column order

* Fix script ToC

* Skip recoding char_apts variable

* Adjust char_apts handling to match changes to ingest

* Replace NA handling for char_apts

* Update final run ID

* Fix char_apts display in workbooks
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27321"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{897A2092-31C1-4E99-B2C2-EC0737924189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6D96D48-2A34-4C5C-976E-A22FDC2D12B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518B7432-B237-4DFB-B6D2-C536D5B9FFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,59 +48,55 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Jean Cochrane:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm. If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
+          <t>This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm.
+If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
         </r>
       </text>
     </comment>
     <comment ref="AL6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
       <text>
-        <t>Jean Cochrane (Assessor):
-The number of apartments in a property. Only present for class 211 and class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The number of apartments in a property. Only present for class 211 and class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+        </r>
       </text>
     </comment>
     <comment ref="AM6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
       <text>
-        <t>Jean Cochrane (Assessor):
-The number of commercial units in a property. Only present for class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The number of commercial units in a property. Only present for class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
+        </r>
       </text>
     </comment>
     <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{0878E9D8-A2FA-4E71-98AD-3CB2F004A791}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Jean Cochrane:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This column represents the average similarity score for all of the comparable parcels we extracted for this property based on the model structure. (The first two comps are shown in subsequent columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
+          <t>This column represents the average similarity score for all of the comparable parcels we extracted for this property based on the model structure. (The first two comps are shown in subsequent columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
         </r>
       </text>
     </comment>
@@ -108,23 +104,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Jean Cochrane:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
+          <t>This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
         </r>
       </text>
     </comment>
@@ -132,23 +118,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
-          <t>Jean Cochrane:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This column represents the similarity score for this comparable sale, which we can interpret as the percent confidence that the model has that the parcel sold in this sale is comparable to the target parcel.</t>
+          <t>This column represents the similarity score for this comparable sale, which we can interpret as the percent confidence that the model has that the parcel sold in this sale is comparable to the target parcel.</t>
         </r>
       </text>
     </comment>
@@ -164,14 +140,30 @@
   <commentList>
     <comment ref="O4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
       <text>
-        <t>Jean Cochrane (Assessor):
-The number of apartments in a card. Only present for class 211 and 212 parcels.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The number of apartments in a card. Only present for class 211 and 212 parcels.</t>
+        </r>
       </text>
     </comment>
     <comment ref="P4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
       <text>
-        <t>Jean Cochrane (Assessor):
-The number of commercial units in a card. Only present for class 212 parcels.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The number of commercial units in a card. Only present for class 212 parcels.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -179,17 +171,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
   <si>
     <t>Run ID (res):</t>
   </si>
   <si>
-    <t>Change in value</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
     <t>Characteristics</t>
   </si>
   <si>
@@ -391,10 +377,25 @@
     <t>Detail view for comparable sales</t>
   </si>
   <si>
-    <t>Sale price</t>
-  </si>
-  <si>
-    <t>Sale date</t>
+    <t>PIN Information</t>
+  </si>
+  <si>
+    <t>Change In Value</t>
+  </si>
+  <si>
+    <t>Card Information</t>
+  </si>
+  <si>
+    <t>Card Characteristics</t>
+  </si>
+  <si>
+    <t>Sale Price</t>
+  </si>
+  <si>
+    <t>Sale Date</t>
+  </si>
+  <si>
+    <t>Sales Information</t>
   </si>
 </sst>
 </file>
@@ -407,7 +408,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -419,13 +420,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -461,13 +455,28 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,8 +519,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9CCFC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -620,33 +635,22 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -658,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -683,66 +687,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="37" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="37" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -754,6 +785,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF9CCFC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1065,13 +1101,13 @@
   <dimension ref="A1:BN1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="AF7" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AM19" sqref="AM19"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1114,17 +1150,17 @@
     <col min="57" max="57" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="21">
+    <row r="1" spans="1:66" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1182,7 +1218,7 @@
       <c r="BM1" s="5"/>
       <c r="BN1" s="5"/>
     </row>
-    <row r="2" spans="1:66">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1224,13 +1260,13 @@
       <c r="AQ2"/>
       <c r="AR2"/>
     </row>
-    <row r="3" spans="1:66" ht="15.75" customHeight="1">
+    <row r="3" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1267,7 +1303,7 @@
       <c r="AQ3"/>
       <c r="AR3"/>
     </row>
-    <row r="4" spans="1:66">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1305,421 +1341,430 @@
       <c r="AQ4"/>
       <c r="AR4"/>
     </row>
-    <row r="5" spans="1:66">
-      <c r="I5"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="30"/>
-      <c r="V5" s="30"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="35" t="s">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="B5" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="42"/>
+      <c r="X5" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA5" s="38"/>
+      <c r="AB5" s="38"/>
+      <c r="AC5" s="38"/>
+      <c r="AD5" s="38"/>
+      <c r="AE5" s="38"/>
+      <c r="AF5" s="38"/>
+      <c r="AG5" s="39"/>
+      <c r="AH5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="Y5" s="36"/>
-      <c r="Z5" s="33" t="s">
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="35"/>
+      <c r="AL5" s="35"/>
+      <c r="AM5" s="36"/>
+      <c r="AN5" s="31" t="s">
         <v>2</v>
-      </c>
-      <c r="AA5" s="33"/>
-      <c r="AB5" s="33"/>
-      <c r="AC5" s="33"/>
-      <c r="AD5" s="33"/>
-      <c r="AE5" s="33"/>
-      <c r="AF5" s="33"/>
-      <c r="AG5" s="33"/>
-      <c r="AH5" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI5" s="34"/>
-      <c r="AJ5" s="34"/>
-      <c r="AK5" s="34"/>
-      <c r="AL5" s="21"/>
-      <c r="AM5" s="21"/>
-      <c r="AN5" s="32" t="s">
-        <v>4</v>
       </c>
       <c r="AO5" s="32"/>
       <c r="AP5" s="32"/>
       <c r="AQ5" s="32"/>
-      <c r="AR5" s="32"/>
+      <c r="AR5" s="33"/>
       <c r="AS5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT5" s="29"/>
+      <c r="AU5" s="29"/>
+      <c r="AV5" s="29"/>
+      <c r="AW5" s="29"/>
+      <c r="AX5" s="29"/>
+      <c r="AY5" s="29"/>
+      <c r="AZ5" s="29"/>
+      <c r="BA5" s="29"/>
+      <c r="BB5" s="29"/>
+      <c r="BC5" s="29"/>
+      <c r="BD5" s="29"/>
+      <c r="BE5" s="30"/>
+    </row>
+    <row r="6" spans="1:66" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AT5" s="28"/>
-      <c r="AU5" s="28"/>
-      <c r="AV5" s="28"/>
-      <c r="AW5" s="28"/>
-      <c r="AX5" s="28"/>
-      <c r="AY5" s="28"/>
-      <c r="AZ5" s="28"/>
-      <c r="BA5" s="28"/>
-      <c r="BB5" s="28"/>
-      <c r="BC5" s="28"/>
-      <c r="BD5" s="28"/>
-      <c r="BE5" s="28"/>
-    </row>
-    <row r="6" spans="1:66" ht="32.25">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="I6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="J6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="K6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="O6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="P6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="Q6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="U6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="T6" s="6" t="s">
+      <c r="V6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="W6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="X6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="W6" s="7" t="s">
+      <c r="Y6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="Z6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="AA6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AB6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AC6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AD6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AE6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AF6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AG6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AF6" s="4" t="s">
+      <c r="AH6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AI6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AH6" s="19" t="s">
+      <c r="AJ6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AI6" s="6" t="s">
+      <c r="AK6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AJ6" s="6" t="s">
+      <c r="AL6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AK6" s="6" t="s">
+      <c r="AM6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AL6" s="22" t="s">
+      <c r="AN6" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AM6" s="22" t="s">
+      <c r="AO6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AN6" s="17" t="s">
+      <c r="AP6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AO6" s="8" t="s">
+      <c r="AQ6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AP6" s="8" t="s">
+      <c r="AR6" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AQ6" s="8" t="s">
+      <c r="AS6" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="AR6" s="14" t="s">
+      <c r="AT6" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="AS6" s="8" t="s">
+      <c r="AU6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AT6" s="8" t="s">
+      <c r="AV6" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="AU6" s="8" t="s">
+      <c r="AW6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="AV6" s="8" t="s">
+      <c r="AX6" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="AW6" s="8" t="s">
+      <c r="AY6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AX6" s="8" t="s">
+      <c r="AZ6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AY6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AZ6" s="8" t="s">
+      <c r="BB6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BC6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="BD6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE6" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:66">
+    </row>
+    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="AO8" s="18"/>
       <c r="AP8" s="18"/>
     </row>
-    <row r="9" spans="1:66">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
       <c r="AO9" s="18"/>
       <c r="AP9" s="18"/>
     </row>
-    <row r="1048519" spans="35:35">
+    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048519" s="13"/>
     </row>
-    <row r="1048520" spans="35:35">
+    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048520" s="13"/>
     </row>
-    <row r="1048521" spans="35:35">
+    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048521" s="13"/>
     </row>
-    <row r="1048522" spans="35:35">
+    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048522" s="13"/>
     </row>
-    <row r="1048523" spans="35:35">
+    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048523" s="13"/>
     </row>
-    <row r="1048524" spans="35:35">
+    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048524" s="13"/>
     </row>
-    <row r="1048525" spans="35:35">
+    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048525" s="13"/>
     </row>
-    <row r="1048526" spans="35:35">
+    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048526" s="13"/>
     </row>
-    <row r="1048527" spans="35:35">
+    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048527" s="13"/>
     </row>
-    <row r="1048528" spans="35:35">
+    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048528" s="13"/>
     </row>
-    <row r="1048529" spans="35:35">
+    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048529" s="13"/>
     </row>
-    <row r="1048530" spans="35:35">
+    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048530" s="13"/>
     </row>
-    <row r="1048531" spans="35:35">
+    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048531" s="13"/>
     </row>
-    <row r="1048532" spans="35:35">
+    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048532" s="13"/>
     </row>
-    <row r="1048533" spans="35:35">
+    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048533" s="13"/>
     </row>
-    <row r="1048534" spans="35:35">
+    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048534" s="13"/>
     </row>
-    <row r="1048535" spans="35:35">
+    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048535" s="13"/>
     </row>
-    <row r="1048536" spans="35:35">
+    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048536" s="13"/>
     </row>
-    <row r="1048537" spans="35:35">
+    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048537" s="13"/>
     </row>
-    <row r="1048538" spans="35:35">
+    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048538" s="13"/>
     </row>
-    <row r="1048539" spans="35:35">
+    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048539" s="13"/>
     </row>
-    <row r="1048540" spans="35:35">
+    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048540" s="13"/>
     </row>
-    <row r="1048541" spans="35:35">
+    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048541" s="13"/>
     </row>
-    <row r="1048542" spans="35:35">
+    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048542" s="13"/>
     </row>
-    <row r="1048543" spans="35:35">
+    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048543" s="13"/>
     </row>
-    <row r="1048544" spans="35:35">
+    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048544" s="13"/>
     </row>
-    <row r="1048545" spans="35:35">
+    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048545" s="13"/>
     </row>
-    <row r="1048546" spans="35:35">
+    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048546" s="13"/>
     </row>
-    <row r="1048547" spans="35:35">
+    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048547" s="13"/>
     </row>
-    <row r="1048548" spans="35:35">
+    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048548" s="13"/>
     </row>
-    <row r="1048549" spans="35:35">
+    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048549" s="13"/>
     </row>
-    <row r="1048550" spans="35:35">
+    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048550" s="13"/>
     </row>
-    <row r="1048551" spans="35:35">
+    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048551" s="13"/>
     </row>
-    <row r="1048552" spans="35:35">
+    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048552" s="13"/>
     </row>
-    <row r="1048553" spans="35:35">
+    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048553" s="13"/>
     </row>
-    <row r="1048554" spans="35:35">
+    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048554" s="13"/>
     </row>
-    <row r="1048555" spans="35:35">
+    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048555" s="13"/>
     </row>
-    <row r="1048556" spans="35:35">
+    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048556" s="13"/>
     </row>
-    <row r="1048557" spans="35:35">
+    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048557" s="13"/>
     </row>
-    <row r="1048558" spans="35:35">
+    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048558" s="13"/>
     </row>
-    <row r="1048559" spans="35:35">
+    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048559" s="13"/>
     </row>
-    <row r="1048560" spans="35:35">
+    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048560" s="13"/>
     </row>
-    <row r="1048561" spans="35:35">
+    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048561" s="13"/>
     </row>
-    <row r="1048562" spans="35:35">
+    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048562" s="13"/>
     </row>
-    <row r="1048563" spans="35:35">
+    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048563" s="13"/>
     </row>
-    <row r="1048564" spans="35:35">
+    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048564" s="13"/>
     </row>
-    <row r="1048565" spans="35:35">
+    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048565" s="13"/>
     </row>
-    <row r="1048566" spans="35:35">
+    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048566" s="13"/>
     </row>
-    <row r="1048567" spans="35:35">
+    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048567" s="13"/>
     </row>
-    <row r="1048568" spans="35:35">
+    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048568" s="13"/>
     </row>
-    <row r="1048569" spans="35:35">
+    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048569" s="13"/>
     </row>
-    <row r="1048570" spans="35:35">
+    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048570" s="13"/>
     </row>
-    <row r="1048571" spans="35:35">
+    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048571" s="13"/>
     </row>
-    <row r="1048572" spans="35:35">
+    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048572" s="13"/>
     </row>
-    <row r="1048573" spans="35:35">
+    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048573" s="13"/>
     </row>
-    <row r="1048574" spans="35:35">
+    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048574" s="13"/>
     </row>
-    <row r="1048575" spans="35:35">
+    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
@@ -1727,8 +1772,9 @@
     <mergeCell ref="P5:W5"/>
     <mergeCell ref="AN5:AR5"/>
     <mergeCell ref="Z5:AG5"/>
-    <mergeCell ref="AH5:AK5"/>
     <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="AH5:AM5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1742,12 +1788,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
@@ -1762,18 +1808,18 @@
     <col min="14" max="14" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21">
-      <c r="B1" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1788,7 +1834,7 @@
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1798,237 +1844,254 @@
       <c r="G2"/>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:23">
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="N3"/>
-    </row>
-    <row r="4" spans="1:23" ht="32.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="36"/>
+    </row>
+    <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="E4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="G4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="H4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="J4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="K4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="P4" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" s="38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="1048517" spans="12:12">
+    </row>
+    <row r="1048517" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048517" s="13"/>
     </row>
-    <row r="1048518" spans="12:12">
+    <row r="1048518" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048518" s="13"/>
     </row>
-    <row r="1048519" spans="12:12">
+    <row r="1048519" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048519" s="13"/>
     </row>
-    <row r="1048520" spans="12:12">
+    <row r="1048520" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048520" s="13"/>
     </row>
-    <row r="1048521" spans="12:12">
+    <row r="1048521" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048521" s="13"/>
     </row>
-    <row r="1048522" spans="12:12">
+    <row r="1048522" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048522" s="13"/>
     </row>
-    <row r="1048523" spans="12:12">
+    <row r="1048523" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048523" s="13"/>
     </row>
-    <row r="1048524" spans="12:12">
+    <row r="1048524" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048524" s="13"/>
     </row>
-    <row r="1048525" spans="12:12">
+    <row r="1048525" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048525" s="13"/>
     </row>
-    <row r="1048526" spans="12:12">
+    <row r="1048526" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048526" s="13"/>
     </row>
-    <row r="1048527" spans="12:12">
+    <row r="1048527" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048527" s="13"/>
     </row>
-    <row r="1048528" spans="12:12">
+    <row r="1048528" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048528" s="13"/>
     </row>
-    <row r="1048529" spans="12:12">
+    <row r="1048529" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048529" s="13"/>
     </row>
-    <row r="1048530" spans="12:12">
+    <row r="1048530" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048530" s="13"/>
     </row>
-    <row r="1048531" spans="12:12">
+    <row r="1048531" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048531" s="13"/>
     </row>
-    <row r="1048532" spans="12:12">
+    <row r="1048532" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048532" s="13"/>
     </row>
-    <row r="1048533" spans="12:12">
+    <row r="1048533" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048533" s="13"/>
     </row>
-    <row r="1048534" spans="12:12">
+    <row r="1048534" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048534" s="13"/>
     </row>
-    <row r="1048535" spans="12:12">
+    <row r="1048535" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048535" s="13"/>
     </row>
-    <row r="1048536" spans="12:12">
+    <row r="1048536" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048536" s="13"/>
     </row>
-    <row r="1048537" spans="12:12">
+    <row r="1048537" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048537" s="13"/>
     </row>
-    <row r="1048538" spans="12:12">
+    <row r="1048538" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048538" s="13"/>
     </row>
-    <row r="1048539" spans="12:12">
+    <row r="1048539" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048539" s="13"/>
     </row>
-    <row r="1048540" spans="12:12">
+    <row r="1048540" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048540" s="13"/>
     </row>
-    <row r="1048541" spans="12:12">
+    <row r="1048541" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048541" s="13"/>
     </row>
-    <row r="1048542" spans="12:12">
+    <row r="1048542" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048542" s="13"/>
     </row>
-    <row r="1048543" spans="12:12">
+    <row r="1048543" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048543" s="13"/>
     </row>
-    <row r="1048544" spans="12:12">
+    <row r="1048544" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048544" s="13"/>
     </row>
-    <row r="1048545" spans="12:12">
+    <row r="1048545" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048545" s="13"/>
     </row>
-    <row r="1048546" spans="12:12">
+    <row r="1048546" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048546" s="13"/>
     </row>
-    <row r="1048547" spans="12:12">
+    <row r="1048547" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048547" s="13"/>
     </row>
-    <row r="1048548" spans="12:12">
+    <row r="1048548" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048548" s="13"/>
     </row>
-    <row r="1048549" spans="12:12">
+    <row r="1048549" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048549" s="13"/>
     </row>
-    <row r="1048550" spans="12:12">
+    <row r="1048550" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048550" s="13"/>
     </row>
-    <row r="1048551" spans="12:12">
+    <row r="1048551" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048551" s="13"/>
     </row>
-    <row r="1048552" spans="12:12">
+    <row r="1048552" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048552" s="13"/>
     </row>
-    <row r="1048553" spans="12:12">
+    <row r="1048553" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048553" s="13"/>
     </row>
-    <row r="1048554" spans="12:12">
+    <row r="1048554" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048554" s="13"/>
     </row>
-    <row r="1048555" spans="12:12">
+    <row r="1048555" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048555" s="13"/>
     </row>
-    <row r="1048556" spans="12:12">
+    <row r="1048556" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048556" s="13"/>
     </row>
-    <row r="1048557" spans="12:12">
+    <row r="1048557" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048557" s="13"/>
     </row>
-    <row r="1048558" spans="12:12">
+    <row r="1048558" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048558" s="13"/>
     </row>
-    <row r="1048559" spans="12:12">
+    <row r="1048559" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048559" s="13"/>
     </row>
-    <row r="1048560" spans="12:12">
+    <row r="1048560" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048560" s="13"/>
     </row>
-    <row r="1048561" spans="12:12">
+    <row r="1048561" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048561" s="13"/>
     </row>
-    <row r="1048562" spans="12:12">
+    <row r="1048562" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048562" s="13"/>
     </row>
-    <row r="1048563" spans="12:12">
+    <row r="1048563" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048563" s="13"/>
     </row>
-    <row r="1048564" spans="12:12">
+    <row r="1048564" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048564" s="13"/>
     </row>
-    <row r="1048565" spans="12:12">
+    <row r="1048565" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048565" s="13"/>
     </row>
-    <row r="1048566" spans="12:12">
+    <row r="1048566" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048566" s="13"/>
     </row>
-    <row r="1048567" spans="12:12">
+    <row r="1048567" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048567" s="13"/>
     </row>
-    <row r="1048568" spans="12:12">
+    <row r="1048568" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048568" s="13"/>
     </row>
-    <row r="1048569" spans="12:12">
+    <row r="1048569" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048569" s="13"/>
     </row>
-    <row r="1048570" spans="12:12">
+    <row r="1048570" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048570" s="13"/>
     </row>
-    <row r="1048571" spans="12:12">
+    <row r="1048571" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048571" s="13"/>
     </row>
-    <row r="1048572" spans="12:12">
+    <row r="1048572" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048572" s="13"/>
     </row>
-    <row r="1048573" spans="12:12">
+    <row r="1048573" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L1048573" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2041,75 +2104,99 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="3" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="24.375" customWidth="1"/>
+    <col min="6" max="6" width="26.625" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
     <col min="9" max="10" width="15.625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="13" max="13" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1">
-      <c r="B1" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-    </row>
-    <row r="4" spans="1:13" ht="32.25" customHeight="1">
+    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="36"/>
+    </row>
+    <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="M4" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add final desk review tweaks based on stakeholder feedback
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518B7432-B237-4DFB-B6D2-C536D5B9FFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CCF6E0-7BCA-4ED2-81F8-65E680B85CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,15 @@
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
     <sheet name="Card Detail" sheetId="4" r:id="rId2"/>
     <sheet name="Comparables" sheetId="5" r:id="rId3"/>
+    <sheet name="Neighborhood Breakout" sheetId="9" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BH$7</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
+  <pivotCaches>
+    <pivotCache cacheId="1" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,21 +51,21 @@
     <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
-    <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
+    <comment ref="AC6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm.
 If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AL6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
+    <comment ref="AM6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
       <text>
         <r>
           <rPr>
@@ -72,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
+    <comment ref="AN6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
       <text>
         <r>
           <rPr>
@@ -83,20 +90,6 @@
             <scheme val="minor"/>
           </rPr>
           <t>The number of commercial units in a property. Only present for class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{0878E9D8-A2FA-4E71-98AD-3CB2F004A791}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column represents the average similarity score for all of the comparable parcels we extracted for this property based on the model structure. (The first two comps are shown in subsequent columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
         </r>
       </text>
     </comment>
@@ -125,6 +118,147 @@
             <scheme val="minor"/>
           </rPr>
           <t>This column represents the similarity score for this comparable sale, which we can interpret as the percent confidence that the model has that the parcel sold in this sale is comparable to the target parcel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{8035D120-422D-440A-8651-B1189F0D5374}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column represents the average similarity score for all of the comparable parcels we extracted for this property based on the model structure. (The first two comps are shown in subsequent columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{BC63D4E8-13FE-4190-B049-8F73F08FC6D9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This flag indicates that there is a problem with the PIN's proration, such as a group of proration rates that do not sum to 1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{8D952257-05F3-458B-BB51-489A57E1F158}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This flag indicates that the PIN's land value is in the 95th percentile of land values for its town (that is to say, it's very high).
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AY6" authorId="0" shapeId="0" xr:uid="{C3739962-30FA-49E2-B79F-736E5AEB387B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This flag indicates that the PIN's building value is in the 95th percentile of building values for its town (that is to say, it's very high).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{9B95BB78-BBFA-4D08-898D-42D9F801F5C9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This flag indicates homeownership improvement exemptions that have recently expired, implying that characteristics will be changed this tax year. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BB6" authorId="0" shapeId="0" xr:uid="{23361704-B7DC-4593-A117-F2816AD735D7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This flag indicates that the PIN's value has not changed since last year, which should be unlikely.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BD6" authorId="0" shapeId="0" xr:uid="{83117FFA-9BB4-4818-B2C6-422A3A943BE2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jean Cochrane:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This flag indicates that the estimated value for the PIN is dramatically higher than last year's value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BE6" authorId="0" shapeId="0" xr:uid="{66E115B5-8547-42A9-A19E-183D9317F2A3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This flag indicates that the estimated value of the PIN is dramatically lower than last year's value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BF6" authorId="0" shapeId="0" xr:uid="{C26E7A69-3354-428E-BBFF-70904DE96781}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jean Cochrane:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This flag indicates that one or more of the characteristics that are most important to the model are missing for this PIN.</t>
         </r>
       </text>
     </comment>
@@ -171,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -179,9 +313,6 @@
     <t>Characteristics</t>
   </si>
   <si>
-    <t>Comparables</t>
-  </si>
-  <si>
     <t>Flags</t>
   </si>
   <si>
@@ -396,19 +527,65 @@
   </si>
   <si>
     <t>Sales Information</t>
+  </si>
+  <si>
+    <t>Comparable Sales</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Valuations Notes</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Summary statistics broken out by neighborhood</t>
+  </si>
+  <si>
+    <t>Count of Class</t>
+  </si>
+  <si>
+    <t>Total AV</t>
+  </si>
+  <si>
+    <t>AV Difference</t>
+  </si>
+  <si>
+    <t>Min of Total AV</t>
+  </si>
+  <si>
+    <t>Average of Total AV</t>
+  </si>
+  <si>
+    <t>Max of Total AV</t>
+  </si>
+  <si>
+    <t>Average of AV Difference</t>
+  </si>
+  <si>
+    <t>Average of YoY ∆ %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -451,7 +628,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -475,8 +652,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +706,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF9CCFC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD1D1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,17 +771,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -642,6 +821,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -650,7 +840,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -666,10 +856,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -679,24 +869,42 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="37" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -709,12 +917,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -724,13 +926,43 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -740,39 +972,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -787,6 +986,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFD1D1"/>
       <color rgb="FFF9CCFC"/>
     </mruColors>
   </colors>
@@ -799,6 +999,405 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45330.686558449073" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="pin_detail_Range"/>
+  </cacheSource>
+  <cacheFields count="60">
+    <cacheField name="PIN" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Class" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Nbhd." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Street Address" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Municipality" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Townhome Complex ID" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="PIN Num. Cards" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Tieback Key PIN" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Tieback (Proration) Rate" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Building" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate    S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bld. Rate    S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. % of Total" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Before Rounding" numFmtId="44">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Building2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate Original" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate     Effective" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bld. Rate     S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. % of Tot." numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY ∆ $" numFmtId="164">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY ∆ %" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Valuations Notes" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Date 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Amount 1" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Non-Arm's-Length Sale Flag 1" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Doc. 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Date 2" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Amount 2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Non-Arm's-Length Sale Flag 2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Doc. 2" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Year Built" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total        Bld. S. F." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Stories" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. S. F." numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="# Res. Units" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="# Comm. Units" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Comp. 1 PIN" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Comp. 1 Score" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Comp. 2 PIN" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Comp. 2 Score" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Overall Comp. Score" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Is Prorated" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Proration Error" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Multi-Card" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Multi-Land" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. &gt;= 95% in Town" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bld. &gt;= 95% in Town" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land Value Capped" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="# Expired 288s" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Value Unchanged" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Post-Modeling Change" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY Change &gt;= 50%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY Change &lt;= -5%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Critical Char. Missing" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total AV" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="AV Difference" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+  <r>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="60">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
+    <dataField name="Min of Total AV" fld="58" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="58" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="58" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="59" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1098,13 +1697,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BN1048575"/>
+  <dimension ref="A1:BH1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1130,37 +1729,38 @@
     <col min="22" max="22" width="11.125" style="10" customWidth="1"/>
     <col min="23" max="23" width="11.625" style="11" customWidth="1"/>
     <col min="24" max="24" width="11" style="12"/>
-    <col min="25" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="10.375" customWidth="1"/>
-    <col min="27" max="27" width="13" style="10" customWidth="1"/>
-    <col min="28" max="28" width="18.625" style="10" customWidth="1"/>
-    <col min="29" max="30" width="13" style="16" customWidth="1"/>
-    <col min="31" max="31" width="13" style="10" customWidth="1"/>
-    <col min="32" max="32" width="18.625" style="10" customWidth="1"/>
-    <col min="33" max="33" width="13" style="16" customWidth="1"/>
-    <col min="37" max="40" width="11" style="13"/>
+    <col min="25" max="26" width="11" style="11"/>
+    <col min="27" max="27" width="10.375" customWidth="1"/>
+    <col min="28" max="28" width="13" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
+    <col min="30" max="31" width="13" style="16" customWidth="1"/>
+    <col min="32" max="32" width="13" style="10" customWidth="1"/>
+    <col min="33" max="33" width="18.625" style="10" customWidth="1"/>
+    <col min="34" max="34" width="13" style="16" customWidth="1"/>
+    <col min="38" max="40" width="11" style="13"/>
     <col min="41" max="41" width="15.625" style="13" customWidth="1"/>
     <col min="42" max="42" width="11" style="13"/>
     <col min="43" max="43" width="15.625" style="13" customWidth="1"/>
-    <col min="44" max="44" width="11" style="13"/>
-    <col min="53" max="53" width="14" customWidth="1"/>
-    <col min="54" max="54" width="12.375" customWidth="1"/>
-    <col min="55" max="55" width="11.875" customWidth="1"/>
-    <col min="56" max="56" width="10.875" customWidth="1"/>
-    <col min="57" max="57" width="11.5" customWidth="1"/>
+    <col min="44" max="45" width="11" style="13"/>
+    <col min="54" max="54" width="14" customWidth="1"/>
+    <col min="55" max="55" width="12.375" customWidth="1"/>
+    <col min="56" max="56" width="11.875" customWidth="1"/>
+    <col min="57" max="57" width="10.875" customWidth="1"/>
+    <col min="58" max="58" width="11.5" customWidth="1"/>
+    <col min="59" max="60" width="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:60" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1209,16 +1809,8 @@
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
-      <c r="BG1" s="5"/>
-      <c r="BH1" s="5"/>
-      <c r="BI1" s="5"/>
-      <c r="BJ1" s="5"/>
-      <c r="BK1" s="5"/>
-      <c r="BL1" s="5"/>
-      <c r="BM1" s="5"/>
-      <c r="BN1" s="5"/>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1244,14 +1836,14 @@
       <c r="W2"/>
       <c r="X2"/>
       <c r="Y2"/>
-      <c r="AA2"/>
+      <c r="Z2"/>
       <c r="AB2"/>
       <c r="AC2"/>
       <c r="AD2"/>
       <c r="AE2"/>
       <c r="AF2"/>
       <c r="AG2"/>
-      <c r="AK2"/>
+      <c r="AH2"/>
       <c r="AL2"/>
       <c r="AM2"/>
       <c r="AN2"/>
@@ -1259,14 +1851,15 @@
       <c r="AP2"/>
       <c r="AQ2"/>
       <c r="AR2"/>
-    </row>
-    <row r="3" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS2"/>
+    </row>
+    <row r="3" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1287,14 +1880,14 @@
       <c r="W3"/>
       <c r="X3"/>
       <c r="Y3"/>
-      <c r="AA3"/>
+      <c r="Z3"/>
       <c r="AB3"/>
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3"/>
       <c r="AF3"/>
       <c r="AG3"/>
-      <c r="AK3"/>
+      <c r="AH3"/>
       <c r="AL3"/>
       <c r="AM3"/>
       <c r="AN3"/>
@@ -1302,8 +1895,9 @@
       <c r="AP3"/>
       <c r="AQ3"/>
       <c r="AR3"/>
-    </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="AS3"/>
+    </row>
+    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1322,459 +1916,472 @@
       <c r="W4"/>
       <c r="X4"/>
       <c r="Y4"/>
-      <c r="AA4"/>
+      <c r="Z4"/>
       <c r="AB4"/>
       <c r="AC4"/>
       <c r="AD4"/>
       <c r="AE4"/>
       <c r="AF4"/>
       <c r="AG4"/>
-      <c r="AH4" s="20"/>
-      <c r="AI4" s="20"/>
-      <c r="AJ4" s="20"/>
-      <c r="AK4" s="20"/>
-      <c r="AL4" s="20"/>
-      <c r="AM4" s="20"/>
-      <c r="AN4"/>
+      <c r="AH4"/>
+      <c r="AI4" s="19"/>
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19"/>
+      <c r="AL4" s="19"/>
+      <c r="AM4" s="19"/>
+      <c r="AN4" s="19"/>
       <c r="AO4"/>
       <c r="AP4"/>
       <c r="AQ4"/>
       <c r="AR4"/>
-    </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="AS4"/>
+    </row>
+    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="B5" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="39"/>
+      <c r="X5" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="42"/>
-      <c r="X5" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="37" t="s">
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA5" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB5" s="42"/>
+      <c r="AC5" s="42"/>
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="42"/>
+      <c r="AF5" s="42"/>
+      <c r="AG5" s="43"/>
+      <c r="AH5" s="44"/>
+      <c r="AI5" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="51"/>
+      <c r="AK5" s="51"/>
+      <c r="AL5" s="51"/>
+      <c r="AM5" s="51"/>
+      <c r="AN5" s="51"/>
+      <c r="AO5" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="38"/>
-      <c r="AC5" s="38"/>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="38"/>
-      <c r="AF5" s="38"/>
-      <c r="AG5" s="39"/>
-      <c r="AH5" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="35"/>
-      <c r="AJ5" s="35"/>
-      <c r="AK5" s="35"/>
-      <c r="AL5" s="35"/>
-      <c r="AM5" s="36"/>
-      <c r="AN5" s="31" t="s">
+      <c r="AP5" s="40"/>
+      <c r="AQ5" s="40"/>
+      <c r="AR5" s="40"/>
+      <c r="AS5" s="21"/>
+      <c r="AT5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AO5" s="32"/>
-      <c r="AP5" s="32"/>
-      <c r="AQ5" s="32"/>
-      <c r="AR5" s="33"/>
-      <c r="AS5" s="28" t="s">
+      <c r="AU5" s="35"/>
+      <c r="AV5" s="35"/>
+      <c r="AW5" s="35"/>
+      <c r="AX5" s="35"/>
+      <c r="AY5" s="35"/>
+      <c r="AZ5" s="35"/>
+      <c r="BA5" s="35"/>
+      <c r="BB5" s="35"/>
+      <c r="BC5" s="35"/>
+      <c r="BD5" s="35"/>
+      <c r="BE5" s="35"/>
+      <c r="BF5" s="36"/>
+    </row>
+    <row r="6" spans="1:60" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AT5" s="29"/>
-      <c r="AU5" s="29"/>
-      <c r="AV5" s="29"/>
-      <c r="AW5" s="29"/>
-      <c r="AX5" s="29"/>
-      <c r="AY5" s="29"/>
-      <c r="AZ5" s="29"/>
-      <c r="BA5" s="29"/>
-      <c r="BB5" s="29"/>
-      <c r="BC5" s="29"/>
-      <c r="BD5" s="29"/>
-      <c r="BE5" s="30"/>
-    </row>
-    <row r="6" spans="1:66" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="O6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="Q6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="T6" s="6" t="s">
+      <c r="U6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="V6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="W6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="7" t="s">
+      <c r="X6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="Y6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="Z6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AB6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AC6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AD6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AE6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AF6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AG6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AF6" s="4" t="s">
+      <c r="AH6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AI6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AH6" s="19" t="s">
+      <c r="AJ6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AI6" s="6" t="s">
+      <c r="AK6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ6" s="6" t="s">
+      <c r="AL6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AK6" s="6" t="s">
+      <c r="AM6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AL6" s="9" t="s">
+      <c r="AN6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AM6" s="9" t="s">
+      <c r="AO6" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AN6" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="AQ6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR6" s="14" t="s">
+      <c r="AT6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AS6" s="26" t="s">
+      <c r="AU6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AT6" s="26" t="s">
+      <c r="AV6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AU6" s="26" t="s">
+      <c r="AW6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AV6" s="26" t="s">
+      <c r="AX6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AW6" s="26" t="s">
+      <c r="AY6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="AX6" s="26" t="s">
+      <c r="AZ6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AY6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AZ6" s="26" t="s">
+      <c r="BB6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BC6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BD6" s="9" t="s">
+      <c r="BF6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BE6" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="AO8" s="18"/>
-      <c r="AP8" s="18"/>
-    </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="AO9" s="18"/>
-      <c r="AP9" s="18"/>
-    </row>
-    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048575" s="13"/>
+      <c r="BG6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BH6" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AO8" s="17"/>
+      <c r="AP8" s="17"/>
+    </row>
+    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AO9" s="17"/>
+      <c r="AP9" s="17"/>
+    </row>
+    <row r="1048519" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AS5:BE5"/>
+    <mergeCell ref="AT5:BF5"/>
     <mergeCell ref="P5:W5"/>
-    <mergeCell ref="AN5:AR5"/>
-    <mergeCell ref="Z5:AG5"/>
+    <mergeCell ref="AO5:AR5"/>
+    <mergeCell ref="AA5:AH5"/>
     <mergeCell ref="X5:Y5"/>
     <mergeCell ref="B5:I5"/>
-    <mergeCell ref="AH5:AM5"/>
+    <mergeCell ref="AI5:AN5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1809,17 +2416,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1845,74 +2452,74 @@
       <c r="N2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="36"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="52"/>
     </row>
     <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="M4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="26" t="s">
+      <c r="O4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="P4" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="P4" s="27" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="1048517" spans="12:12" x14ac:dyDescent="0.25">
@@ -2107,7 +2714,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2122,73 +2729,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="34" t="s">
+      <c r="E3" s="48"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="36"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="52"/>
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="G4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>66</v>
-      </c>
       <c r="L4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2200,4 +2807,93 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D773A1D3-FC14-4EA4-B569-35CAE3B3E4FA}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="27"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="27"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tweak columns and fix percentage formatting for comp score columns
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CCF6E0-7BCA-4ED2-81F8-65E680B85CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843C8A6E-9047-4FAE-8F7E-1A9FCBE7FD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -69,11 +69,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color theme="1"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The number of apartments in a property. Only present for class 211 and class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
         </r>
@@ -83,11 +82,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color theme="1"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The number of commercial units in a property. Only present for class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
         </r>
@@ -97,11 +95,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
         </r>
@@ -111,11 +108,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>This column represents the similarity score for this comparable sale, which we can interpret as the percent confidence that the model has that the parcel sold in this sale is comparable to the target parcel.</t>
         </r>
@@ -130,7 +126,20 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column represents the average similarity score for all of the comparable parcels we extracted for this property based on the model structure. (The first two comps are shown in subsequent columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
+          <t>This column represents the average similarity score for all 20 of the comparable sales extracted for this property based on the model structure. (The first two of these 20 comps are shown in the preceding columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{ECF27779-F8CB-4DDB-B47A-434BDB41AF51}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the PIN is prorated.</t>
         </r>
       </text>
     </comment>
@@ -143,7 +152,33 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This flag indicates that there is a problem with the PIN's proration, such as a group of proration rates that do not sum to 1.</t>
+          <t>Indicates that there is a problem with the PIN's proration, such as a group of proration rates that do not sum to 1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{9201257A-E739-4445-9BA2-278E0B79DD9F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the PIN contains multiple cards.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{617DE059-1ED7-4DF2-ADE1-DA1638E1B1B3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the PIN spans multiple land lines.</t>
         </r>
       </text>
     </comment>
@@ -156,7 +191,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">This flag indicates that the PIN's land value is in the 95th percentile of land values for its town (that is to say, it's very high).
+          <t xml:space="preserve">Indicates that the PIN's land value is in the 95th percentile of land values for its town (that is to say, it's very high).
 </t>
         </r>
       </text>
@@ -170,7 +205,39 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This flag indicates that the PIN's building value is in the 95th percentile of building values for its town (that is to say, it's very high).</t>
+          <t>Indicates that the PIN's building value is in the 95th percentile of building values for its town (that is to say, it's very high).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AZ6" authorId="0" shapeId="0" xr:uid="{E8F31B7F-B8C2-4805-B053-4600780FD7A2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the land value for this</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PIN was artificially capped below its $/sqft rate in order to remain less than 50% of the total FMV.</t>
         </r>
       </text>
     </comment>
@@ -183,7 +250,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">This flag indicates homeownership improvement exemptions that have recently expired, implying that characteristics will be changed this tax year. 
+          <t xml:space="preserve">Indicates that the PIN has homeownership improvement exemptions that have recently expired, implying that characteristics will be changed this tax year. 
 </t>
         </r>
       </text>
@@ -197,7 +264,20 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This flag indicates that the PIN's value has not changed since last year, which should be unlikely.</t>
+          <t>Flag indicating that the PIN's value has not changed since last year, which should be unlikely.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BC6" authorId="0" shapeId="0" xr:uid="{AE640F8D-C8FE-48E7-A609-B0C718186353}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Flag indicating that an adjustment was made to this PIN's value after modeling.</t>
         </r>
       </text>
     </comment>
@@ -205,23 +285,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Jean Cochrane:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This flag indicates that the estimated value for the PIN is dramatically higher than last year's value.</t>
+          <t>Flag indicating that the estimated value for the PIN is dramatically higher than last year's value.</t>
         </r>
       </text>
     </comment>
@@ -234,7 +303,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This flag indicates that the estimated value of the PIN is dramatically lower than last year's value.</t>
+          <t>Flag indicating that the estimated value of the PIN is dramatically lower than last year's value.</t>
         </r>
       </text>
     </comment>
@@ -242,23 +311,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Jean Cochrane:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This flag indicates that one or more of the characteristics that are most important to the model are missing for this PIN.</t>
+          <t>Flag indicating that one or more of the characteristics that are most important to the model are missing for this PIN.</t>
         </r>
       </text>
     </comment>
@@ -276,11 +334,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color theme="1"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The number of apartments in a card. Only present for class 211 and 212 parcels.</t>
         </r>
@@ -290,11 +347,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color theme="1"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The number of commercial units in a card. Only present for class 212 parcels.</t>
         </r>
@@ -585,7 +641,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -639,23 +695,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1002,7 +1050,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45330.686558449073" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45331.454486226852" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1268,7 +1316,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="60">
     <pivotField showAll="0"/>
@@ -1729,8 +1777,9 @@
     <col min="22" max="22" width="11.125" style="10" customWidth="1"/>
     <col min="23" max="23" width="11.625" style="11" customWidth="1"/>
     <col min="24" max="24" width="11" style="12"/>
-    <col min="25" max="26" width="11" style="11"/>
-    <col min="27" max="27" width="10.375" customWidth="1"/>
+    <col min="25" max="25" width="11" style="11"/>
+    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
+    <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="13" style="10" customWidth="1"/>
     <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
     <col min="30" max="31" width="13" style="16" customWidth="1"/>
@@ -2397,7 +2446,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Oops, comp groupings in desk review workbook was missing a left border
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843C8A6E-9047-4FAE-8F7E-1A9FCBE7FD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D795D16A-0C6D-40C4-BFE2-04E72EA35426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -888,7 +888,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1020,6 +1020,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1050,7 +1053,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45331.454486226852" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45331.484378125002" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1751,7 +1754,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2035,7 +2038,7 @@
       <c r="AL5" s="51"/>
       <c r="AM5" s="51"/>
       <c r="AN5" s="51"/>
-      <c r="AO5" s="40" t="s">
+      <c r="AO5" s="53" t="s">
         <v>74</v>
       </c>
       <c r="AP5" s="40"/>

</xml_diff>

<commit_message>
Add final tweaks to desk review workbook based on Valuations feedback (#213)
* Add final desk review tweaks based on stakeholder feedback

* Appease pre-commit

* Tweak columns and fix percentage formatting for comp score columns

* Oops, comp groupings in desk review workbook was missing a left border
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518B7432-B237-4DFB-B6D2-C536D5B9FFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D795D16A-0C6D-40C4-BFE2-04E72EA35426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
     <sheet name="Card Detail" sheetId="4" r:id="rId2"/>
     <sheet name="Comparables" sheetId="5" r:id="rId3"/>
+    <sheet name="Neighborhood Breakout" sheetId="9" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BH$7</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
+  <pivotCaches>
+    <pivotCache cacheId="4" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,59 +51,43 @@
     <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
-    <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
+    <comment ref="AC6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm.
 If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AL6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
+    <comment ref="AM6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color theme="1"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The number of apartments in a property. Only present for class 211 and class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AM6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
+    <comment ref="AN6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color theme="1"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The number of commercial units in a property. Only present for class 212 properties. For multicard properties, this column will show a list of numbers of units, one for each card.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{0878E9D8-A2FA-4E71-98AD-3CB2F004A791}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column represents the average similarity score for all of the comparable parcels we extracted for this property based on the model structure. (The first two comps are shown in subsequent columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
         </r>
       </text>
     </comment>
@@ -104,11 +95,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
         </r>
@@ -118,13 +108,215 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>This column represents the similarity score for this comparable sale, which we can interpret as the percent confidence that the model has that the parcel sold in this sale is comparable to the target parcel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{8035D120-422D-440A-8651-B1189F0D5374}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column represents the average similarity score for all 20 of the comparable sales extracted for this property based on the model structure. (The first two of these 20 comps are shown in the preceding columns.) A high average score indicates that the model is very confident in its prediction for this parcel, since it has many similar sales to use for comparison.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{ECF27779-F8CB-4DDB-B47A-434BDB41AF51}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the PIN is prorated.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{BC63D4E8-13FE-4190-B049-8F73F08FC6D9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that there is a problem with the PIN's proration, such as a group of proration rates that do not sum to 1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{9201257A-E739-4445-9BA2-278E0B79DD9F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the PIN contains multiple cards.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{617DE059-1ED7-4DF2-ADE1-DA1638E1B1B3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the PIN spans multiple land lines.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{8D952257-05F3-458B-BB51-489A57E1F158}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Indicates that the PIN's land value is in the 95th percentile of land values for its town (that is to say, it's very high).
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AY6" authorId="0" shapeId="0" xr:uid="{C3739962-30FA-49E2-B79F-736E5AEB387B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the PIN's building value is in the 95th percentile of building values for its town (that is to say, it's very high).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AZ6" authorId="0" shapeId="0" xr:uid="{E8F31B7F-B8C2-4805-B053-4600780FD7A2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the land value for this</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PIN was artificially capped below its $/sqft rate in order to remain less than 50% of the total FMV.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{9B95BB78-BBFA-4D08-898D-42D9F801F5C9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Indicates that the PIN has homeownership improvement exemptions that have recently expired, implying that characteristics will be changed this tax year. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BB6" authorId="0" shapeId="0" xr:uid="{23361704-B7DC-4593-A117-F2816AD735D7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Flag indicating that the PIN's value has not changed since last year, which should be unlikely.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BC6" authorId="0" shapeId="0" xr:uid="{AE640F8D-C8FE-48E7-A609-B0C718186353}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Flag indicating that an adjustment was made to this PIN's value after modeling.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BD6" authorId="0" shapeId="0" xr:uid="{83117FFA-9BB4-4818-B2C6-422A3A943BE2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Flag indicating that the estimated value for the PIN is dramatically higher than last year's value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BE6" authorId="0" shapeId="0" xr:uid="{66E115B5-8547-42A9-A19E-183D9317F2A3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Flag indicating that the estimated value of the PIN is dramatically lower than last year's value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BF6" authorId="0" shapeId="0" xr:uid="{C26E7A69-3354-428E-BBFF-70904DE96781}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Flag indicating that one or more of the characteristics that are most important to the model are missing for this PIN.</t>
         </r>
       </text>
     </comment>
@@ -142,11 +334,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color theme="1"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The number of apartments in a card. Only present for class 211 and 212 parcels.</t>
         </r>
@@ -156,11 +347,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="9"/>
             <color theme="1"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The number of commercial units in a card. Only present for class 212 parcels.</t>
         </r>
@@ -171,7 +361,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -179,9 +369,6 @@
     <t>Characteristics</t>
   </si>
   <si>
-    <t>Comparables</t>
-  </si>
-  <si>
     <t>Flags</t>
   </si>
   <si>
@@ -396,17 +583,63 @@
   </si>
   <si>
     <t>Sales Information</t>
+  </si>
+  <si>
+    <t>Comparable Sales</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Valuations Notes</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Summary statistics broken out by neighborhood</t>
+  </si>
+  <si>
+    <t>Count of Class</t>
+  </si>
+  <si>
+    <t>Total AV</t>
+  </si>
+  <si>
+    <t>AV Difference</t>
+  </si>
+  <si>
+    <t>Min of Total AV</t>
+  </si>
+  <si>
+    <t>Average of Total AV</t>
+  </si>
+  <si>
+    <t>Max of Total AV</t>
+  </si>
+  <si>
+    <t>Average of AV Difference</t>
+  </si>
+  <si>
+    <t>Average of YoY ∆ %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -451,7 +684,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -462,21 +695,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +754,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF9CCFC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD1D1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,17 +819,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -642,6 +869,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -650,7 +888,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -666,10 +904,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -679,24 +917,42 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="37" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -709,12 +965,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -724,13 +974,43 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -742,37 +1022,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -787,6 +1037,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFD1D1"/>
       <color rgb="FFF9CCFC"/>
     </mruColors>
   </colors>
@@ -799,6 +1050,405 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45331.484378125002" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="pin_detail_Range"/>
+  </cacheSource>
+  <cacheFields count="60">
+    <cacheField name="PIN" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Class" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Nbhd." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Street Address" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Municipality" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Townhome Complex ID" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="PIN Num. Cards" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Tieback Key PIN" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Tieback (Proration) Rate" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Building" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate    S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bld. Rate    S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. % of Total" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Before Rounding" numFmtId="44">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Building2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate Original" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate     Effective" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bld. Rate     S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. % of Tot." numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY ∆ $" numFmtId="164">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY ∆ %" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Valuations Notes" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Date 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Amount 1" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Non-Arm's-Length Sale Flag 1" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Doc. 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Date 2" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Amount 2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Non-Arm's-Length Sale Flag 2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Doc. 2" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Year Built" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total        Bld. S. F." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Stories" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. S. F." numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="# Res. Units" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="# Comm. Units" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Comp. 1 PIN" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Comp. 1 Score" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Comp. 2 PIN" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Comp. 2 Score" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Overall Comp. Score" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Is Prorated" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Proration Error" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Multi-Card" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Multi-Land" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. &gt;= 95% in Town" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bld. &gt;= 95% in Town" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land Value Capped" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="# Expired 288s" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Value Unchanged" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Post-Modeling Change" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY Change &gt;= 50%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY Change &lt;= -5%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Critical Char. Missing" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total AV" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="AV Difference" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+  <r>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="60">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
+    <dataField name="Min of Total AV" fld="58" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="58" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="58" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="59" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1098,13 +1748,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BN1048575"/>
+  <dimension ref="A1:BH1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1131,36 +1781,38 @@
     <col min="23" max="23" width="11.625" style="11" customWidth="1"/>
     <col min="24" max="24" width="11" style="12"/>
     <col min="25" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="10.375" customWidth="1"/>
-    <col min="27" max="27" width="13" style="10" customWidth="1"/>
-    <col min="28" max="28" width="18.625" style="10" customWidth="1"/>
-    <col min="29" max="30" width="13" style="16" customWidth="1"/>
-    <col min="31" max="31" width="13" style="10" customWidth="1"/>
-    <col min="32" max="32" width="18.625" style="10" customWidth="1"/>
-    <col min="33" max="33" width="13" style="16" customWidth="1"/>
-    <col min="37" max="40" width="11" style="13"/>
+    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
+    <col min="27" max="27" width="13" customWidth="1"/>
+    <col min="28" max="28" width="13" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
+    <col min="30" max="31" width="13" style="16" customWidth="1"/>
+    <col min="32" max="32" width="13" style="10" customWidth="1"/>
+    <col min="33" max="33" width="18.625" style="10" customWidth="1"/>
+    <col min="34" max="34" width="13" style="16" customWidth="1"/>
+    <col min="38" max="40" width="11" style="13"/>
     <col min="41" max="41" width="15.625" style="13" customWidth="1"/>
     <col min="42" max="42" width="11" style="13"/>
     <col min="43" max="43" width="15.625" style="13" customWidth="1"/>
-    <col min="44" max="44" width="11" style="13"/>
-    <col min="53" max="53" width="14" customWidth="1"/>
-    <col min="54" max="54" width="12.375" customWidth="1"/>
-    <col min="55" max="55" width="11.875" customWidth="1"/>
-    <col min="56" max="56" width="10.875" customWidth="1"/>
-    <col min="57" max="57" width="11.5" customWidth="1"/>
+    <col min="44" max="45" width="11" style="13"/>
+    <col min="54" max="54" width="14" customWidth="1"/>
+    <col min="55" max="55" width="12.375" customWidth="1"/>
+    <col min="56" max="56" width="11.875" customWidth="1"/>
+    <col min="57" max="57" width="10.875" customWidth="1"/>
+    <col min="58" max="58" width="11.5" customWidth="1"/>
+    <col min="59" max="60" width="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:60" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1209,16 +1861,8 @@
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
-      <c r="BG1" s="5"/>
-      <c r="BH1" s="5"/>
-      <c r="BI1" s="5"/>
-      <c r="BJ1" s="5"/>
-      <c r="BK1" s="5"/>
-      <c r="BL1" s="5"/>
-      <c r="BM1" s="5"/>
-      <c r="BN1" s="5"/>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1244,14 +1888,14 @@
       <c r="W2"/>
       <c r="X2"/>
       <c r="Y2"/>
-      <c r="AA2"/>
+      <c r="Z2"/>
       <c r="AB2"/>
       <c r="AC2"/>
       <c r="AD2"/>
       <c r="AE2"/>
       <c r="AF2"/>
       <c r="AG2"/>
-      <c r="AK2"/>
+      <c r="AH2"/>
       <c r="AL2"/>
       <c r="AM2"/>
       <c r="AN2"/>
@@ -1259,14 +1903,15 @@
       <c r="AP2"/>
       <c r="AQ2"/>
       <c r="AR2"/>
-    </row>
-    <row r="3" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS2"/>
+    </row>
+    <row r="3" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1287,14 +1932,14 @@
       <c r="W3"/>
       <c r="X3"/>
       <c r="Y3"/>
-      <c r="AA3"/>
+      <c r="Z3"/>
       <c r="AB3"/>
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3"/>
       <c r="AF3"/>
       <c r="AG3"/>
-      <c r="AK3"/>
+      <c r="AH3"/>
       <c r="AL3"/>
       <c r="AM3"/>
       <c r="AN3"/>
@@ -1302,8 +1947,9 @@
       <c r="AP3"/>
       <c r="AQ3"/>
       <c r="AR3"/>
-    </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="AS3"/>
+    </row>
+    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1322,459 +1968,472 @@
       <c r="W4"/>
       <c r="X4"/>
       <c r="Y4"/>
-      <c r="AA4"/>
+      <c r="Z4"/>
       <c r="AB4"/>
       <c r="AC4"/>
       <c r="AD4"/>
       <c r="AE4"/>
       <c r="AF4"/>
       <c r="AG4"/>
-      <c r="AH4" s="20"/>
-      <c r="AI4" s="20"/>
-      <c r="AJ4" s="20"/>
-      <c r="AK4" s="20"/>
-      <c r="AL4" s="20"/>
-      <c r="AM4" s="20"/>
-      <c r="AN4"/>
+      <c r="AH4"/>
+      <c r="AI4" s="19"/>
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19"/>
+      <c r="AL4" s="19"/>
+      <c r="AM4" s="19"/>
+      <c r="AN4" s="19"/>
       <c r="AO4"/>
       <c r="AP4"/>
       <c r="AQ4"/>
       <c r="AR4"/>
-    </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="AS4"/>
+    </row>
+    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="B5" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="39"/>
+      <c r="X5" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="42"/>
-      <c r="X5" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="37" t="s">
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA5" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB5" s="42"/>
+      <c r="AC5" s="42"/>
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="42"/>
+      <c r="AF5" s="42"/>
+      <c r="AG5" s="43"/>
+      <c r="AH5" s="44"/>
+      <c r="AI5" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="51"/>
+      <c r="AK5" s="51"/>
+      <c r="AL5" s="51"/>
+      <c r="AM5" s="51"/>
+      <c r="AN5" s="51"/>
+      <c r="AO5" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="38"/>
-      <c r="AC5" s="38"/>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="38"/>
-      <c r="AF5" s="38"/>
-      <c r="AG5" s="39"/>
-      <c r="AH5" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="35"/>
-      <c r="AJ5" s="35"/>
-      <c r="AK5" s="35"/>
-      <c r="AL5" s="35"/>
-      <c r="AM5" s="36"/>
-      <c r="AN5" s="31" t="s">
+      <c r="AP5" s="40"/>
+      <c r="AQ5" s="40"/>
+      <c r="AR5" s="40"/>
+      <c r="AS5" s="21"/>
+      <c r="AT5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AO5" s="32"/>
-      <c r="AP5" s="32"/>
-      <c r="AQ5" s="32"/>
-      <c r="AR5" s="33"/>
-      <c r="AS5" s="28" t="s">
+      <c r="AU5" s="35"/>
+      <c r="AV5" s="35"/>
+      <c r="AW5" s="35"/>
+      <c r="AX5" s="35"/>
+      <c r="AY5" s="35"/>
+      <c r="AZ5" s="35"/>
+      <c r="BA5" s="35"/>
+      <c r="BB5" s="35"/>
+      <c r="BC5" s="35"/>
+      <c r="BD5" s="35"/>
+      <c r="BE5" s="35"/>
+      <c r="BF5" s="36"/>
+    </row>
+    <row r="6" spans="1:60" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AT5" s="29"/>
-      <c r="AU5" s="29"/>
-      <c r="AV5" s="29"/>
-      <c r="AW5" s="29"/>
-      <c r="AX5" s="29"/>
-      <c r="AY5" s="29"/>
-      <c r="AZ5" s="29"/>
-      <c r="BA5" s="29"/>
-      <c r="BB5" s="29"/>
-      <c r="BC5" s="29"/>
-      <c r="BD5" s="29"/>
-      <c r="BE5" s="30"/>
-    </row>
-    <row r="6" spans="1:66" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="O6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="Q6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="T6" s="6" t="s">
+      <c r="U6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="V6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="W6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="7" t="s">
+      <c r="X6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="Y6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="Z6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AB6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AC6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AD6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AE6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AF6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AG6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AF6" s="4" t="s">
+      <c r="AH6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AI6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AH6" s="19" t="s">
+      <c r="AJ6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AI6" s="6" t="s">
+      <c r="AK6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ6" s="6" t="s">
+      <c r="AL6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AK6" s="6" t="s">
+      <c r="AM6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AL6" s="9" t="s">
+      <c r="AN6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AM6" s="9" t="s">
+      <c r="AO6" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AN6" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="AQ6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR6" s="14" t="s">
+      <c r="AT6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AS6" s="26" t="s">
+      <c r="AU6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AT6" s="26" t="s">
+      <c r="AV6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AU6" s="26" t="s">
+      <c r="AW6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AV6" s="26" t="s">
+      <c r="AX6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AW6" s="26" t="s">
+      <c r="AY6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="AX6" s="26" t="s">
+      <c r="AZ6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AY6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AZ6" s="26" t="s">
+      <c r="BB6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BC6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BD6" s="9" t="s">
+      <c r="BF6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BE6" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="AO8" s="18"/>
-      <c r="AP8" s="18"/>
-    </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="AO9" s="18"/>
-      <c r="AP9" s="18"/>
-    </row>
-    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048575" s="13"/>
+      <c r="BG6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BH6" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AO8" s="17"/>
+      <c r="AP8" s="17"/>
+    </row>
+    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AO9" s="17"/>
+      <c r="AP9" s="17"/>
+    </row>
+    <row r="1048519" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AS5:BE5"/>
+    <mergeCell ref="AT5:BF5"/>
     <mergeCell ref="P5:W5"/>
-    <mergeCell ref="AN5:AR5"/>
-    <mergeCell ref="Z5:AG5"/>
+    <mergeCell ref="AO5:AR5"/>
+    <mergeCell ref="AA5:AH5"/>
     <mergeCell ref="X5:Y5"/>
     <mergeCell ref="B5:I5"/>
-    <mergeCell ref="AH5:AM5"/>
+    <mergeCell ref="AI5:AN5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1790,7 +2449,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1809,17 +2468,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1845,74 +2504,74 @@
       <c r="N2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="36"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="52"/>
     </row>
     <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="M4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="26" t="s">
+      <c r="O4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="P4" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="P4" s="27" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="1048517" spans="12:12" x14ac:dyDescent="0.25">
@@ -2107,7 +2766,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2122,73 +2781,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="34" t="s">
+      <c r="E3" s="48"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="36"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="52"/>
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="G4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>66</v>
-      </c>
       <c r="L4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2200,4 +2859,93 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D773A1D3-FC14-4EA4-B569-35CAE3B3E4FA}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="27"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="27"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix note for land/bldg percentile flag in desk review workbook
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D795D16A-0C6D-40C4-BFE2-04E72EA35426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB52CDE-7938-4BF3-8A6C-662535FB18F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -191,7 +191,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Indicates that the PIN's land value is in the 95th percentile of land values for its town (that is to say, it's very high).
+          <t xml:space="preserve">Indicates that the PIN's land square footage is in the 95th percentile of land S. F. for its town (that is to say, it's very high).
 </t>
         </r>
       </text>
@@ -205,7 +205,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates that the PIN's building value is in the 95th percentile of building values for its town (that is to say, it's very high).</t>
+          <t>Indicates that the PIN's building square footage is in the 95th percentile of building S. F. for its town (that is to say, it's very high).</t>
         </r>
       </text>
     </comment>
@@ -983,6 +983,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1020,9 +1023,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1053,7 +1053,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45331.484378125002" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45335.445374768518" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1989,16 +1989,16 @@
       <c r="AS4"/>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="31"/>
       <c r="K5" s="32"/>
       <c r="L5" s="32"/>
@@ -2013,37 +2013,37 @@
       <c r="U5" s="38"/>
       <c r="V5" s="38"/>
       <c r="W5" s="39"/>
-      <c r="X5" s="45" t="s">
+      <c r="X5" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="Y5" s="46"/>
+      <c r="Y5" s="47"/>
       <c r="Z5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AA5" s="41" t="s">
+      <c r="AA5" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="AB5" s="42"/>
-      <c r="AC5" s="42"/>
-      <c r="AD5" s="43"/>
-      <c r="AE5" s="42"/>
-      <c r="AF5" s="42"/>
-      <c r="AG5" s="43"/>
-      <c r="AH5" s="44"/>
-      <c r="AI5" s="50" t="s">
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="43"/>
+      <c r="AF5" s="43"/>
+      <c r="AG5" s="44"/>
+      <c r="AH5" s="45"/>
+      <c r="AI5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AJ5" s="51"/>
-      <c r="AK5" s="51"/>
-      <c r="AL5" s="51"/>
-      <c r="AM5" s="51"/>
-      <c r="AN5" s="51"/>
-      <c r="AO5" s="53" t="s">
+      <c r="AJ5" s="52"/>
+      <c r="AK5" s="52"/>
+      <c r="AL5" s="52"/>
+      <c r="AM5" s="52"/>
+      <c r="AN5" s="52"/>
+      <c r="AO5" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="AP5" s="40"/>
-      <c r="AQ5" s="40"/>
-      <c r="AR5" s="40"/>
+      <c r="AP5" s="41"/>
+      <c r="AQ5" s="41"/>
+      <c r="AR5" s="41"/>
       <c r="AS5" s="21"/>
       <c r="AT5" s="34" t="s">
         <v>2</v>
@@ -2449,7 +2449,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2504,25 +2504,25 @@
       <c r="N2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="37"/>
       <c r="F3" s="38"/>
       <c r="G3" s="39"/>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="53"/>
     </row>
     <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2766,7 +2766,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:F1"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2790,24 +2790,24 @@
       <c r="F1" s="30"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="47" t="s">
+      <c r="C3" s="43"/>
+      <c r="D3" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50" t="s">
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="53"/>
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2866,7 +2866,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix note for land/bldg percentile flag in desk review workbook (#214)
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D795D16A-0C6D-40C4-BFE2-04E72EA35426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB52CDE-7938-4BF3-8A6C-662535FB18F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -191,7 +191,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Indicates that the PIN's land value is in the 95th percentile of land values for its town (that is to say, it's very high).
+          <t xml:space="preserve">Indicates that the PIN's land square footage is in the 95th percentile of land S. F. for its town (that is to say, it's very high).
 </t>
         </r>
       </text>
@@ -205,7 +205,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates that the PIN's building value is in the 95th percentile of building values for its town (that is to say, it's very high).</t>
+          <t>Indicates that the PIN's building square footage is in the 95th percentile of building S. F. for its town (that is to say, it's very high).</t>
         </r>
       </text>
     </comment>
@@ -983,6 +983,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1020,9 +1023,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1053,7 +1053,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45331.484378125002" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45335.445374768518" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1989,16 +1989,16 @@
       <c r="AS4"/>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="31"/>
       <c r="K5" s="32"/>
       <c r="L5" s="32"/>
@@ -2013,37 +2013,37 @@
       <c r="U5" s="38"/>
       <c r="V5" s="38"/>
       <c r="W5" s="39"/>
-      <c r="X5" s="45" t="s">
+      <c r="X5" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="Y5" s="46"/>
+      <c r="Y5" s="47"/>
       <c r="Z5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AA5" s="41" t="s">
+      <c r="AA5" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="AB5" s="42"/>
-      <c r="AC5" s="42"/>
-      <c r="AD5" s="43"/>
-      <c r="AE5" s="42"/>
-      <c r="AF5" s="42"/>
-      <c r="AG5" s="43"/>
-      <c r="AH5" s="44"/>
-      <c r="AI5" s="50" t="s">
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="43"/>
+      <c r="AF5" s="43"/>
+      <c r="AG5" s="44"/>
+      <c r="AH5" s="45"/>
+      <c r="AI5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AJ5" s="51"/>
-      <c r="AK5" s="51"/>
-      <c r="AL5" s="51"/>
-      <c r="AM5" s="51"/>
-      <c r="AN5" s="51"/>
-      <c r="AO5" s="53" t="s">
+      <c r="AJ5" s="52"/>
+      <c r="AK5" s="52"/>
+      <c r="AL5" s="52"/>
+      <c r="AM5" s="52"/>
+      <c r="AN5" s="52"/>
+      <c r="AO5" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="AP5" s="40"/>
-      <c r="AQ5" s="40"/>
-      <c r="AR5" s="40"/>
+      <c r="AP5" s="41"/>
+      <c r="AQ5" s="41"/>
+      <c r="AR5" s="41"/>
       <c r="AS5" s="21"/>
       <c r="AT5" s="34" t="s">
         <v>2</v>
@@ -2449,7 +2449,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2504,25 +2504,25 @@
       <c r="N2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="37"/>
       <c r="F3" s="38"/>
       <c r="G3" s="39"/>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="53"/>
     </row>
     <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2766,7 +2766,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:F1"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2790,24 +2790,24 @@
       <c r="F1" s="30"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="47" t="s">
+      <c r="C3" s="43"/>
+      <c r="D3" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50" t="s">
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="53"/>
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2866,7 +2866,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Make desk review sale ratio column permanent
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB52CDE-7938-4BF3-8A6C-662535FB18F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0C9385-FEC3-4E9F-ADCB-5E04981AE821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Neighborhood Breakout" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BH$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BI$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
@@ -51,7 +51,20 @@
     <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
-    <comment ref="AC6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
+    <comment ref="Z6" authorId="0" shapeId="0" xr:uid="{B959BBC6-269B-40A9-8222-4E035C25B553}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The estimated value for the parcel (Total) divided by the amount of its most recent sale, if one exists (Sale Amount 1). Empty if no recent sales exist. If the most recent sale exists but is flagged as a non-arm's-length sale, this ratio will likely not be accurate.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
       <text>
         <r>
           <rPr>
@@ -65,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
+    <comment ref="AN6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
       <text>
         <r>
           <rPr>
@@ -78,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
+    <comment ref="AO6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
       <text>
         <r>
           <rPr>
@@ -91,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
       <text>
         <r>
           <rPr>
@@ -104,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
+    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
       <text>
         <r>
           <rPr>
@@ -117,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{8035D120-422D-440A-8651-B1189F0D5374}">
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{8035D120-422D-440A-8651-B1189F0D5374}">
       <text>
         <r>
           <rPr>
@@ -130,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{ECF27779-F8CB-4DDB-B47A-434BDB41AF51}">
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{ECF27779-F8CB-4DDB-B47A-434BDB41AF51}">
       <text>
         <r>
           <rPr>
@@ -143,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{BC63D4E8-13FE-4190-B049-8F73F08FC6D9}">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{BC63D4E8-13FE-4190-B049-8F73F08FC6D9}">
       <text>
         <r>
           <rPr>
@@ -156,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{9201257A-E739-4445-9BA2-278E0B79DD9F}">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{9201257A-E739-4445-9BA2-278E0B79DD9F}">
       <text>
         <r>
           <rPr>
@@ -169,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{617DE059-1ED7-4DF2-ADE1-DA1638E1B1B3}">
+    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{617DE059-1ED7-4DF2-ADE1-DA1638E1B1B3}">
       <text>
         <r>
           <rPr>
@@ -182,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{8D952257-05F3-458B-BB51-489A57E1F158}">
+    <comment ref="AY6" authorId="0" shapeId="0" xr:uid="{8D952257-05F3-458B-BB51-489A57E1F158}">
       <text>
         <r>
           <rPr>
@@ -196,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY6" authorId="0" shapeId="0" xr:uid="{C3739962-30FA-49E2-B79F-736E5AEB387B}">
+    <comment ref="AZ6" authorId="0" shapeId="0" xr:uid="{C3739962-30FA-49E2-B79F-736E5AEB387B}">
       <text>
         <r>
           <rPr>
@@ -209,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ6" authorId="0" shapeId="0" xr:uid="{E8F31B7F-B8C2-4805-B053-4600780FD7A2}">
+    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{E8F31B7F-B8C2-4805-B053-4600780FD7A2}">
       <text>
         <r>
           <rPr>
@@ -241,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{9B95BB78-BBFA-4D08-898D-42D9F801F5C9}">
+    <comment ref="BB6" authorId="0" shapeId="0" xr:uid="{9B95BB78-BBFA-4D08-898D-42D9F801F5C9}">
       <text>
         <r>
           <rPr>
@@ -255,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB6" authorId="0" shapeId="0" xr:uid="{23361704-B7DC-4593-A117-F2816AD735D7}">
+    <comment ref="BC6" authorId="0" shapeId="0" xr:uid="{23361704-B7DC-4593-A117-F2816AD735D7}">
       <text>
         <r>
           <rPr>
@@ -268,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BC6" authorId="0" shapeId="0" xr:uid="{AE640F8D-C8FE-48E7-A609-B0C718186353}">
+    <comment ref="BD6" authorId="0" shapeId="0" xr:uid="{AE640F8D-C8FE-48E7-A609-B0C718186353}">
       <text>
         <r>
           <rPr>
@@ -281,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BD6" authorId="0" shapeId="0" xr:uid="{83117FFA-9BB4-4818-B2C6-422A3A943BE2}">
+    <comment ref="BE6" authorId="0" shapeId="0" xr:uid="{83117FFA-9BB4-4818-B2C6-422A3A943BE2}">
       <text>
         <r>
           <rPr>
@@ -294,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BE6" authorId="0" shapeId="0" xr:uid="{66E115B5-8547-42A9-A19E-183D9317F2A3}">
+    <comment ref="BF6" authorId="0" shapeId="0" xr:uid="{66E115B5-8547-42A9-A19E-183D9317F2A3}">
       <text>
         <r>
           <rPr>
@@ -307,7 +320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BF6" authorId="0" shapeId="0" xr:uid="{C26E7A69-3354-428E-BBFF-70904DE96781}">
+    <comment ref="BG6" authorId="0" shapeId="0" xr:uid="{C26E7A69-3354-428E-BBFF-70904DE96781}">
       <text>
         <r>
           <rPr>
@@ -361,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -628,6 +641,9 @@
   </si>
   <si>
     <t>Average of YoY ∆ %</t>
+  </si>
+  <si>
+    <t>Sale Ratio</t>
   </si>
 </sst>
 </file>
@@ -641,7 +657,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -707,6 +723,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -764,7 +786,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -880,6 +902,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -888,7 +919,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -950,6 +981,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1004,9 +1038,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1024,6 +1055,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1052,8 +1089,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45335.445374768518" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45343.643762500004" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1748,7 +1789,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH1048575"/>
+  <dimension ref="A1:BI1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -1780,39 +1821,39 @@
     <col min="22" max="22" width="11.125" style="10" customWidth="1"/>
     <col min="23" max="23" width="11.625" style="11" customWidth="1"/>
     <col min="24" max="24" width="11" style="12"/>
-    <col min="25" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
-    <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="28" width="13" style="10" customWidth="1"/>
-    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
-    <col min="30" max="31" width="13" style="16" customWidth="1"/>
-    <col min="32" max="32" width="13" style="10" customWidth="1"/>
-    <col min="33" max="33" width="18.625" style="10" customWidth="1"/>
-    <col min="34" max="34" width="13" style="16" customWidth="1"/>
-    <col min="38" max="40" width="11" style="13"/>
-    <col min="41" max="41" width="15.625" style="13" customWidth="1"/>
-    <col min="42" max="42" width="11" style="13"/>
-    <col min="43" max="43" width="15.625" style="13" customWidth="1"/>
-    <col min="44" max="45" width="11" style="13"/>
-    <col min="54" max="54" width="14" customWidth="1"/>
-    <col min="55" max="55" width="12.375" customWidth="1"/>
-    <col min="56" max="56" width="11.875" customWidth="1"/>
-    <col min="57" max="57" width="10.875" customWidth="1"/>
-    <col min="58" max="58" width="11.5" customWidth="1"/>
-    <col min="59" max="60" width="11" hidden="1" customWidth="1"/>
+    <col min="25" max="26" width="11" style="11"/>
+    <col min="27" max="27" width="21.125" style="11" customWidth="1"/>
+    <col min="28" max="28" width="13" customWidth="1"/>
+    <col min="29" max="29" width="13" style="10" customWidth="1"/>
+    <col min="30" max="30" width="18.625" style="10" customWidth="1"/>
+    <col min="31" max="32" width="13" style="16" customWidth="1"/>
+    <col min="33" max="33" width="13" style="10" customWidth="1"/>
+    <col min="34" max="34" width="18.625" style="10" customWidth="1"/>
+    <col min="35" max="35" width="13" style="16" customWidth="1"/>
+    <col min="39" max="41" width="11" style="13"/>
+    <col min="42" max="42" width="15.625" style="13" customWidth="1"/>
+    <col min="43" max="43" width="11" style="13"/>
+    <col min="44" max="44" width="15.625" style="13" customWidth="1"/>
+    <col min="45" max="46" width="11" style="13"/>
+    <col min="55" max="55" width="14" customWidth="1"/>
+    <col min="56" max="56" width="12.375" customWidth="1"/>
+    <col min="57" max="57" width="11.875" customWidth="1"/>
+    <col min="58" max="58" width="10.875" customWidth="1"/>
+    <col min="59" max="59" width="11.5" customWidth="1"/>
+    <col min="60" max="61" width="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:61" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1861,8 +1902,9 @@
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
-    </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="BG1" s="5"/>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1889,14 +1931,14 @@
       <c r="X2"/>
       <c r="Y2"/>
       <c r="Z2"/>
-      <c r="AB2"/>
+      <c r="AA2"/>
       <c r="AC2"/>
       <c r="AD2"/>
       <c r="AE2"/>
       <c r="AF2"/>
       <c r="AG2"/>
       <c r="AH2"/>
-      <c r="AL2"/>
+      <c r="AI2"/>
       <c r="AM2"/>
       <c r="AN2"/>
       <c r="AO2"/>
@@ -1904,14 +1946,15 @@
       <c r="AQ2"/>
       <c r="AR2"/>
       <c r="AS2"/>
-    </row>
-    <row r="3" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT2"/>
+    </row>
+    <row r="3" spans="1:61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1933,14 +1976,14 @@
       <c r="X3"/>
       <c r="Y3"/>
       <c r="Z3"/>
-      <c r="AB3"/>
+      <c r="AA3"/>
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3"/>
       <c r="AF3"/>
       <c r="AG3"/>
       <c r="AH3"/>
-      <c r="AL3"/>
+      <c r="AI3"/>
       <c r="AM3"/>
       <c r="AN3"/>
       <c r="AO3"/>
@@ -1948,8 +1991,9 @@
       <c r="AQ3"/>
       <c r="AR3"/>
       <c r="AS3"/>
-    </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AT3"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1969,26 +2013,27 @@
       <c r="X4"/>
       <c r="Y4"/>
       <c r="Z4"/>
-      <c r="AB4"/>
+      <c r="AA4"/>
       <c r="AC4"/>
       <c r="AD4"/>
       <c r="AE4"/>
       <c r="AF4"/>
       <c r="AG4"/>
       <c r="AH4"/>
-      <c r="AI4" s="19"/>
+      <c r="AI4"/>
       <c r="AJ4" s="19"/>
       <c r="AK4" s="19"/>
       <c r="AL4" s="19"/>
       <c r="AM4" s="19"/>
       <c r="AN4" s="19"/>
-      <c r="AO4"/>
+      <c r="AO4" s="19"/>
       <c r="AP4"/>
       <c r="AQ4"/>
       <c r="AR4"/>
       <c r="AS4"/>
-    </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AT4"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
         <v>67</v>
       </c>
@@ -1999,69 +2044,70 @@
       <c r="G5" s="49"/>
       <c r="H5" s="49"/>
       <c r="I5" s="50"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="39"/>
-      <c r="X5" s="46" t="s">
+      <c r="J5" s="32"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="39"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="39"/>
+      <c r="V5" s="39"/>
+      <c r="W5" s="40"/>
+      <c r="X5" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="24" t="s">
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AA5" s="42" t="s">
+      <c r="AB5" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="AB5" s="43"/>
-      <c r="AC5" s="43"/>
+      <c r="AC5" s="44"/>
       <c r="AD5" s="44"/>
-      <c r="AE5" s="43"/>
-      <c r="AF5" s="43"/>
+      <c r="AE5" s="45"/>
+      <c r="AF5" s="44"/>
       <c r="AG5" s="44"/>
       <c r="AH5" s="45"/>
-      <c r="AI5" s="51" t="s">
+      <c r="AI5" s="46"/>
+      <c r="AJ5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AJ5" s="52"/>
       <c r="AK5" s="52"/>
       <c r="AL5" s="52"/>
       <c r="AM5" s="52"/>
       <c r="AN5" s="52"/>
-      <c r="AO5" s="40" t="s">
+      <c r="AO5" s="52"/>
+      <c r="AP5" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="AP5" s="41"/>
-      <c r="AQ5" s="41"/>
-      <c r="AR5" s="41"/>
-      <c r="AS5" s="21"/>
-      <c r="AT5" s="34" t="s">
+      <c r="AQ5" s="42"/>
+      <c r="AR5" s="42"/>
+      <c r="AS5" s="42"/>
+      <c r="AT5" s="21"/>
+      <c r="AU5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="AU5" s="35"/>
-      <c r="AV5" s="35"/>
-      <c r="AW5" s="35"/>
-      <c r="AX5" s="35"/>
-      <c r="AY5" s="35"/>
-      <c r="AZ5" s="35"/>
-      <c r="BA5" s="35"/>
-      <c r="BB5" s="35"/>
-      <c r="BC5" s="35"/>
-      <c r="BD5" s="35"/>
-      <c r="BE5" s="35"/>
+      <c r="AV5" s="36"/>
+      <c r="AW5" s="36"/>
+      <c r="AX5" s="36"/>
+      <c r="AY5" s="36"/>
+      <c r="AZ5" s="36"/>
+      <c r="BA5" s="36"/>
+      <c r="BB5" s="36"/>
+      <c r="BC5" s="36"/>
+      <c r="BD5" s="36"/>
+      <c r="BE5" s="36"/>
       <c r="BF5" s="36"/>
-    </row>
-    <row r="6" spans="1:60" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="BG5" s="37"/>
+    </row>
+    <row r="6" spans="1:61" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2134,306 +2180,309 @@
       <c r="X6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="Y6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="Z6" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AB6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB6" s="8" t="s">
+      <c r="AC6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AD6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AD6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF6" s="8" t="s">
+      <c r="AG6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AG6" s="8" t="s">
+      <c r="AH6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AI6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI6" s="18" t="s">
+      <c r="AJ6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AJ6" s="6" t="s">
+      <c r="AK6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AK6" s="6" t="s">
+      <c r="AL6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AL6" s="6" t="s">
+      <c r="AM6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AM6" s="9" t="s">
+      <c r="AN6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AN6" s="9" t="s">
+      <c r="AO6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AO6" s="23" t="s">
+      <c r="AP6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AP6" s="14" t="s">
+      <c r="AQ6" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AQ6" s="9" t="s">
+      <c r="AR6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AR6" s="14" t="s">
+      <c r="AS6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="AS6" s="14" t="s">
+      <c r="AT6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AT6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AV6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AV6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AW6" s="9" t="s">
+      <c r="AX6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AX6" s="9" t="s">
+      <c r="AY6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AY6" s="9" t="s">
+      <c r="AZ6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="AZ6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BB6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BC6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BD6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BE6" s="9" t="s">
+      <c r="BF6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BF6" s="14" t="s">
+      <c r="BG6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BG6" s="2" t="s">
+      <c r="BH6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BH6" s="4" t="s">
+      <c r="BI6" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="AO8" s="17"/>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
       <c r="AP8" s="17"/>
-    </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="AO9" s="17"/>
+      <c r="AQ8" s="17"/>
+    </row>
+    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
       <c r="AP9" s="17"/>
-    </row>
-    <row r="1048519" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048575" s="13"/>
+      <c r="AQ9" s="17"/>
+    </row>
+    <row r="1048519" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AT5:BF5"/>
+    <mergeCell ref="AU5:BG5"/>
     <mergeCell ref="P5:W5"/>
-    <mergeCell ref="AO5:AR5"/>
-    <mergeCell ref="AA5:AH5"/>
+    <mergeCell ref="AP5:AS5"/>
+    <mergeCell ref="AB5:AI5"/>
     <mergeCell ref="X5:Y5"/>
     <mergeCell ref="B5:I5"/>
-    <mergeCell ref="AI5:AN5"/>
+    <mergeCell ref="AJ5:AO5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2468,17 +2517,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -2509,9 +2558,9 @@
       </c>
       <c r="C3" s="49"/>
       <c r="D3" s="50"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="51" t="s">
         <v>70</v>
       </c>
@@ -2781,19 +2830,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="43"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="48" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
Add basement type and finish to card/comps sheets in desk review workbook
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0C9385-FEC3-4E9F-ADCB-5E04981AE821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D85A2-4FC0-49EA-AD11-CB31371E6A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>The estimated value for the parcel (Total) divided by the amount of its most recent sale, if one exists (Sale Amount 1). Empty if no recent sales exist. If the most recent sale exists but is flagged as a non-arm's-length sale, this ratio will likely not be accurate.</t>
+          <t>The estimated value for the parcel (Total) divided by the amount of its most recent sale, if one exists (Sale Amount 1). Empty if no recent sales exist. If a recent sale exists but is flagged as a non-arm's-length sale, this ratio will likely not be accurate.</t>
         </r>
       </text>
     </comment>
@@ -343,7 +343,7 @@
     <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
-    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
       <text>
         <r>
           <rPr>
@@ -356,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
       <text>
         <r>
           <rPr>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -644,6 +644,12 @@
   </si>
   <si>
     <t>Sale Ratio</t>
+  </si>
+  <si>
+    <t>Bsmt. Type</t>
+  </si>
+  <si>
+    <t>Bsmt. Finish</t>
   </si>
 </sst>
 </file>
@@ -919,7 +925,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -981,86 +987,89 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1089,16 +1098,12 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45343.643762500004" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45343.715909837963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
-  <cacheFields count="60">
+  <cacheFields count="61">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1176,6 +1181,9 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="YoY ∆ %" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Ratio" numFmtId="9">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Valuations Notes" numFmtId="9">
@@ -1355,6 +1363,7 @@
     <m/>
     <m/>
     <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -1362,7 +1371,7 @@
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="60">
+  <pivotFields count="61">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="2">
@@ -1398,6 +1407,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1474,10 +1484,10 @@
   </colItems>
   <dataFields count="6">
     <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
-    <dataField name="Min of Total AV" fld="58" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total AV" fld="58" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total AV" fld="58" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of AV Difference" fld="59" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min of Total AV" fld="59" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="59" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="59" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="60" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1845,15 +1855,15 @@
   <sheetData>
     <row r="1" spans="1:61" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1952,9 +1962,9 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2044,38 +2054,38 @@
       <c r="G5" s="49"/>
       <c r="H5" s="49"/>
       <c r="I5" s="50"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="39"/>
-      <c r="V5" s="39"/>
-      <c r="W5" s="40"/>
-      <c r="X5" s="47" t="s">
+      <c r="J5" s="33"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="53" t="s">
         <v>68</v>
       </c>
       <c r="Y5" s="54"/>
-      <c r="Z5" s="29"/>
+      <c r="Z5" s="55"/>
       <c r="AA5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AB5" s="43" t="s">
+      <c r="AB5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="45"/>
-      <c r="AF5" s="44"/>
-      <c r="AG5" s="44"/>
-      <c r="AH5" s="45"/>
-      <c r="AI5" s="46"/>
+      <c r="AC5" s="45"/>
+      <c r="AD5" s="45"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="45"/>
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="47"/>
       <c r="AJ5" s="51" t="s">
         <v>1</v>
       </c>
@@ -2084,28 +2094,28 @@
       <c r="AM5" s="52"/>
       <c r="AN5" s="52"/>
       <c r="AO5" s="52"/>
-      <c r="AP5" s="41" t="s">
+      <c r="AP5" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="AQ5" s="42"/>
-      <c r="AR5" s="42"/>
-      <c r="AS5" s="42"/>
+      <c r="AQ5" s="43"/>
+      <c r="AR5" s="43"/>
+      <c r="AS5" s="43"/>
       <c r="AT5" s="21"/>
-      <c r="AU5" s="35" t="s">
+      <c r="AU5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="AV5" s="36"/>
-      <c r="AW5" s="36"/>
-      <c r="AX5" s="36"/>
-      <c r="AY5" s="36"/>
-      <c r="AZ5" s="36"/>
-      <c r="BA5" s="36"/>
-      <c r="BB5" s="36"/>
-      <c r="BC5" s="36"/>
-      <c r="BD5" s="36"/>
-      <c r="BE5" s="36"/>
-      <c r="BF5" s="36"/>
-      <c r="BG5" s="37"/>
+      <c r="AV5" s="37"/>
+      <c r="AW5" s="37"/>
+      <c r="AX5" s="37"/>
+      <c r="AY5" s="37"/>
+      <c r="AZ5" s="37"/>
+      <c r="BA5" s="37"/>
+      <c r="BB5" s="37"/>
+      <c r="BC5" s="37"/>
+      <c r="BD5" s="37"/>
+      <c r="BE5" s="37"/>
+      <c r="BF5" s="37"/>
+      <c r="BG5" s="38"/>
     </row>
     <row r="6" spans="1:61" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -2183,7 +2193,7 @@
       <c r="Y6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z6" s="55" t="s">
+      <c r="Z6" s="29" t="s">
         <v>89</v>
       </c>
       <c r="AA6" s="3" t="s">
@@ -2480,9 +2490,9 @@
     <mergeCell ref="P5:W5"/>
     <mergeCell ref="AP5:AS5"/>
     <mergeCell ref="AB5:AI5"/>
-    <mergeCell ref="X5:Y5"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="AJ5:AO5"/>
+    <mergeCell ref="X5:Z5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2492,7 +2502,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W1048573"/>
+  <dimension ref="A1:Y1048573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
@@ -2511,25 +2521,27 @@
     <col min="6" max="7" width="14.625" style="10" customWidth="1"/>
     <col min="9" max="9" width="9.25" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
-    <col min="11" max="11" width="15.75" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="11" style="13"/>
+    <col min="11" max="11" width="13.75" customWidth="1"/>
+    <col min="12" max="12" width="15.625" customWidth="1"/>
+    <col min="13" max="13" width="15.75" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="31" t="s">
+    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -2541,8 +2553,10 @@
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2550,17 +2564,17 @@
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
-      <c r="N2"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P2"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="48" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="49"/>
       <c r="D3" s="50"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="51" t="s">
         <v>70</v>
       </c>
@@ -2571,12 +2585,11 @@
       <c r="M3" s="52"/>
       <c r="N3" s="52"/>
       <c r="O3" s="52"/>
-      <c r="P3" s="53"/>
-    </row>
-    <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="56"/>
+    </row>
+    <row r="4" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>58</v>
       </c>
@@ -2605,201 +2618,207 @@
         <v>63</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="R4" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="1048517" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048517" s="13"/>
-    </row>
-    <row r="1048518" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048518" s="13"/>
-    </row>
-    <row r="1048519" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048573" s="13"/>
+    <row r="1048517" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048517" s="13"/>
+    </row>
+    <row r="1048518" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048518" s="13"/>
+    </row>
+    <row r="1048519" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048573" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="H3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2809,7 +2828,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
@@ -2824,25 +2843,27 @@
     <col min="2" max="3" width="11.625" customWidth="1"/>
     <col min="6" max="6" width="26.625" customWidth="1"/>
     <col min="7" max="7" width="11.875" customWidth="1"/>
-    <col min="9" max="10" width="15.625" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="13" max="13" width="11.625" customWidth="1"/>
+    <col min="9" max="9" width="15.625" customWidth="1"/>
+    <col min="10" max="10" width="13.75" customWidth="1"/>
+    <col min="11" max="12" width="15.625" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="15" max="15" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="31" t="s">
+    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="44"/>
+      <c r="C3" s="45"/>
       <c r="D3" s="48" t="s">
         <v>67</v>
       </c>
@@ -2856,9 +2877,11 @@
       <c r="J3" s="52"/>
       <c r="K3" s="52"/>
       <c r="L3" s="52"/>
-      <c r="M3" s="53"/>
-    </row>
-    <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="56"/>
+    </row>
+    <row r="4" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -2886,16 +2909,22 @@
       <c r="I4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="O4" s="14" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2904,7 +2933,7 @@
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="G3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add basement chars and sale ratio columns to desk review workbooks (#216)
* Make desk review sale ratio column permanent

* Add basement type and finish to card/comps sheets in desk review workbook
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB52CDE-7938-4BF3-8A6C-662535FB18F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D85A2-4FC0-49EA-AD11-CB31371E6A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Neighborhood Breakout" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BH$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BI$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
@@ -51,7 +51,20 @@
     <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
-    <comment ref="AC6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
+    <comment ref="Z6" authorId="0" shapeId="0" xr:uid="{B959BBC6-269B-40A9-8222-4E035C25B553}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The estimated value for the parcel (Total) divided by the amount of its most recent sale, if one exists (Sale Amount 1). Empty if no recent sales exist. If a recent sale exists but is flagged as a non-arm's-length sale, this ratio will likely not be accurate.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD6" authorId="0" shapeId="0" xr:uid="{E1258316-8105-4C22-B533-C12DB8E47009}">
       <text>
         <r>
           <rPr>
@@ -65,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
+    <comment ref="AN6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
       <text>
         <r>
           <rPr>
@@ -78,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
+    <comment ref="AO6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
       <text>
         <r>
           <rPr>
@@ -91,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
       <text>
         <r>
           <rPr>
@@ -104,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
+    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
       <text>
         <r>
           <rPr>
@@ -117,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{8035D120-422D-440A-8651-B1189F0D5374}">
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{8035D120-422D-440A-8651-B1189F0D5374}">
       <text>
         <r>
           <rPr>
@@ -130,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{ECF27779-F8CB-4DDB-B47A-434BDB41AF51}">
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{ECF27779-F8CB-4DDB-B47A-434BDB41AF51}">
       <text>
         <r>
           <rPr>
@@ -143,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{BC63D4E8-13FE-4190-B049-8F73F08FC6D9}">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{BC63D4E8-13FE-4190-B049-8F73F08FC6D9}">
       <text>
         <r>
           <rPr>
@@ -156,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{9201257A-E739-4445-9BA2-278E0B79DD9F}">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{9201257A-E739-4445-9BA2-278E0B79DD9F}">
       <text>
         <r>
           <rPr>
@@ -169,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{617DE059-1ED7-4DF2-ADE1-DA1638E1B1B3}">
+    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{617DE059-1ED7-4DF2-ADE1-DA1638E1B1B3}">
       <text>
         <r>
           <rPr>
@@ -182,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{8D952257-05F3-458B-BB51-489A57E1F158}">
+    <comment ref="AY6" authorId="0" shapeId="0" xr:uid="{8D952257-05F3-458B-BB51-489A57E1F158}">
       <text>
         <r>
           <rPr>
@@ -196,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY6" authorId="0" shapeId="0" xr:uid="{C3739962-30FA-49E2-B79F-736E5AEB387B}">
+    <comment ref="AZ6" authorId="0" shapeId="0" xr:uid="{C3739962-30FA-49E2-B79F-736E5AEB387B}">
       <text>
         <r>
           <rPr>
@@ -209,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ6" authorId="0" shapeId="0" xr:uid="{E8F31B7F-B8C2-4805-B053-4600780FD7A2}">
+    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{E8F31B7F-B8C2-4805-B053-4600780FD7A2}">
       <text>
         <r>
           <rPr>
@@ -241,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{9B95BB78-BBFA-4D08-898D-42D9F801F5C9}">
+    <comment ref="BB6" authorId="0" shapeId="0" xr:uid="{9B95BB78-BBFA-4D08-898D-42D9F801F5C9}">
       <text>
         <r>
           <rPr>
@@ -255,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB6" authorId="0" shapeId="0" xr:uid="{23361704-B7DC-4593-A117-F2816AD735D7}">
+    <comment ref="BC6" authorId="0" shapeId="0" xr:uid="{23361704-B7DC-4593-A117-F2816AD735D7}">
       <text>
         <r>
           <rPr>
@@ -268,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BC6" authorId="0" shapeId="0" xr:uid="{AE640F8D-C8FE-48E7-A609-B0C718186353}">
+    <comment ref="BD6" authorId="0" shapeId="0" xr:uid="{AE640F8D-C8FE-48E7-A609-B0C718186353}">
       <text>
         <r>
           <rPr>
@@ -281,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BD6" authorId="0" shapeId="0" xr:uid="{83117FFA-9BB4-4818-B2C6-422A3A943BE2}">
+    <comment ref="BE6" authorId="0" shapeId="0" xr:uid="{83117FFA-9BB4-4818-B2C6-422A3A943BE2}">
       <text>
         <r>
           <rPr>
@@ -294,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BE6" authorId="0" shapeId="0" xr:uid="{66E115B5-8547-42A9-A19E-183D9317F2A3}">
+    <comment ref="BF6" authorId="0" shapeId="0" xr:uid="{66E115B5-8547-42A9-A19E-183D9317F2A3}">
       <text>
         <r>
           <rPr>
@@ -307,7 +320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BF6" authorId="0" shapeId="0" xr:uid="{C26E7A69-3354-428E-BBFF-70904DE96781}">
+    <comment ref="BG6" authorId="0" shapeId="0" xr:uid="{C26E7A69-3354-428E-BBFF-70904DE96781}">
       <text>
         <r>
           <rPr>
@@ -330,7 +343,7 @@
     <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
-    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
       <text>
         <r>
           <rPr>
@@ -343,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
       <text>
         <r>
           <rPr>
@@ -361,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -628,6 +641,15 @@
   </si>
   <si>
     <t>Average of YoY ∆ %</t>
+  </si>
+  <si>
+    <t>Sale Ratio</t>
+  </si>
+  <si>
+    <t>Bsmt. Type</t>
+  </si>
+  <si>
+    <t>Bsmt. Finish</t>
   </si>
 </sst>
 </file>
@@ -641,7 +663,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -707,6 +729,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -764,7 +792,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -880,6 +908,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -888,7 +925,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -950,6 +987,12 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1001,25 +1044,28 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1053,11 +1099,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45335.445374768518" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45343.715909837963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
-  <cacheFields count="60">
+  <cacheFields count="61">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1135,6 +1181,9 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="YoY ∆ %" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Ratio" numFmtId="9">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Valuations Notes" numFmtId="9">
@@ -1314,6 +1363,7 @@
     <m/>
     <m/>
     <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -1321,7 +1371,7 @@
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="60">
+  <pivotFields count="61">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="2">
@@ -1357,6 +1407,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1433,10 +1484,10 @@
   </colItems>
   <dataFields count="6">
     <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
-    <dataField name="Min of Total AV" fld="58" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total AV" fld="58" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total AV" fld="58" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of AV Difference" fld="59" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min of Total AV" fld="59" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="59" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="59" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="60" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1748,7 +1799,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH1048575"/>
+  <dimension ref="A1:BI1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -1780,39 +1831,39 @@
     <col min="22" max="22" width="11.125" style="10" customWidth="1"/>
     <col min="23" max="23" width="11.625" style="11" customWidth="1"/>
     <col min="24" max="24" width="11" style="12"/>
-    <col min="25" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
-    <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="28" width="13" style="10" customWidth="1"/>
-    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
-    <col min="30" max="31" width="13" style="16" customWidth="1"/>
-    <col min="32" max="32" width="13" style="10" customWidth="1"/>
-    <col min="33" max="33" width="18.625" style="10" customWidth="1"/>
-    <col min="34" max="34" width="13" style="16" customWidth="1"/>
-    <col min="38" max="40" width="11" style="13"/>
-    <col min="41" max="41" width="15.625" style="13" customWidth="1"/>
-    <col min="42" max="42" width="11" style="13"/>
-    <col min="43" max="43" width="15.625" style="13" customWidth="1"/>
-    <col min="44" max="45" width="11" style="13"/>
-    <col min="54" max="54" width="14" customWidth="1"/>
-    <col min="55" max="55" width="12.375" customWidth="1"/>
-    <col min="56" max="56" width="11.875" customWidth="1"/>
-    <col min="57" max="57" width="10.875" customWidth="1"/>
-    <col min="58" max="58" width="11.5" customWidth="1"/>
-    <col min="59" max="60" width="11" hidden="1" customWidth="1"/>
+    <col min="25" max="26" width="11" style="11"/>
+    <col min="27" max="27" width="21.125" style="11" customWidth="1"/>
+    <col min="28" max="28" width="13" customWidth="1"/>
+    <col min="29" max="29" width="13" style="10" customWidth="1"/>
+    <col min="30" max="30" width="18.625" style="10" customWidth="1"/>
+    <col min="31" max="32" width="13" style="16" customWidth="1"/>
+    <col min="33" max="33" width="13" style="10" customWidth="1"/>
+    <col min="34" max="34" width="18.625" style="10" customWidth="1"/>
+    <col min="35" max="35" width="13" style="16" customWidth="1"/>
+    <col min="39" max="41" width="11" style="13"/>
+    <col min="42" max="42" width="15.625" style="13" customWidth="1"/>
+    <col min="43" max="43" width="11" style="13"/>
+    <col min="44" max="44" width="15.625" style="13" customWidth="1"/>
+    <col min="45" max="46" width="11" style="13"/>
+    <col min="55" max="55" width="14" customWidth="1"/>
+    <col min="56" max="56" width="12.375" customWidth="1"/>
+    <col min="57" max="57" width="11.875" customWidth="1"/>
+    <col min="58" max="58" width="10.875" customWidth="1"/>
+    <col min="59" max="59" width="11.5" customWidth="1"/>
+    <col min="60" max="61" width="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:61" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1861,8 +1912,9 @@
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
-    </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="BG1" s="5"/>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1889,14 +1941,14 @@
       <c r="X2"/>
       <c r="Y2"/>
       <c r="Z2"/>
-      <c r="AB2"/>
+      <c r="AA2"/>
       <c r="AC2"/>
       <c r="AD2"/>
       <c r="AE2"/>
       <c r="AF2"/>
       <c r="AG2"/>
       <c r="AH2"/>
-      <c r="AL2"/>
+      <c r="AI2"/>
       <c r="AM2"/>
       <c r="AN2"/>
       <c r="AO2"/>
@@ -1904,14 +1956,15 @@
       <c r="AQ2"/>
       <c r="AR2"/>
       <c r="AS2"/>
-    </row>
-    <row r="3" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT2"/>
+    </row>
+    <row r="3" spans="1:61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1933,14 +1986,14 @@
       <c r="X3"/>
       <c r="Y3"/>
       <c r="Z3"/>
-      <c r="AB3"/>
+      <c r="AA3"/>
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3"/>
       <c r="AF3"/>
       <c r="AG3"/>
       <c r="AH3"/>
-      <c r="AL3"/>
+      <c r="AI3"/>
       <c r="AM3"/>
       <c r="AN3"/>
       <c r="AO3"/>
@@ -1948,8 +2001,9 @@
       <c r="AQ3"/>
       <c r="AR3"/>
       <c r="AS3"/>
-    </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AT3"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1969,26 +2023,27 @@
       <c r="X4"/>
       <c r="Y4"/>
       <c r="Z4"/>
-      <c r="AB4"/>
+      <c r="AA4"/>
       <c r="AC4"/>
       <c r="AD4"/>
       <c r="AE4"/>
       <c r="AF4"/>
       <c r="AG4"/>
       <c r="AH4"/>
-      <c r="AI4" s="19"/>
+      <c r="AI4"/>
       <c r="AJ4" s="19"/>
       <c r="AK4" s="19"/>
       <c r="AL4" s="19"/>
       <c r="AM4" s="19"/>
       <c r="AN4" s="19"/>
-      <c r="AO4"/>
+      <c r="AO4" s="19"/>
       <c r="AP4"/>
       <c r="AQ4"/>
       <c r="AR4"/>
       <c r="AS4"/>
-    </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AT4"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
         <v>67</v>
       </c>
@@ -1999,69 +2054,70 @@
       <c r="G5" s="49"/>
       <c r="H5" s="49"/>
       <c r="I5" s="50"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="39"/>
-      <c r="X5" s="46" t="s">
+      <c r="J5" s="33"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="24" t="s">
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="55"/>
+      <c r="AA5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AA5" s="42" t="s">
+      <c r="AB5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AB5" s="43"/>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="43"/>
-      <c r="AF5" s="43"/>
-      <c r="AG5" s="44"/>
-      <c r="AH5" s="45"/>
-      <c r="AI5" s="51" t="s">
+      <c r="AC5" s="45"/>
+      <c r="AD5" s="45"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="45"/>
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AJ5" s="52"/>
       <c r="AK5" s="52"/>
       <c r="AL5" s="52"/>
       <c r="AM5" s="52"/>
       <c r="AN5" s="52"/>
-      <c r="AO5" s="40" t="s">
+      <c r="AO5" s="52"/>
+      <c r="AP5" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="AP5" s="41"/>
-      <c r="AQ5" s="41"/>
-      <c r="AR5" s="41"/>
-      <c r="AS5" s="21"/>
-      <c r="AT5" s="34" t="s">
+      <c r="AQ5" s="43"/>
+      <c r="AR5" s="43"/>
+      <c r="AS5" s="43"/>
+      <c r="AT5" s="21"/>
+      <c r="AU5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="AU5" s="35"/>
-      <c r="AV5" s="35"/>
-      <c r="AW5" s="35"/>
-      <c r="AX5" s="35"/>
-      <c r="AY5" s="35"/>
-      <c r="AZ5" s="35"/>
-      <c r="BA5" s="35"/>
-      <c r="BB5" s="35"/>
-      <c r="BC5" s="35"/>
-      <c r="BD5" s="35"/>
-      <c r="BE5" s="35"/>
-      <c r="BF5" s="36"/>
-    </row>
-    <row r="6" spans="1:60" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="AV5" s="37"/>
+      <c r="AW5" s="37"/>
+      <c r="AX5" s="37"/>
+      <c r="AY5" s="37"/>
+      <c r="AZ5" s="37"/>
+      <c r="BA5" s="37"/>
+      <c r="BB5" s="37"/>
+      <c r="BC5" s="37"/>
+      <c r="BD5" s="37"/>
+      <c r="BE5" s="37"/>
+      <c r="BF5" s="37"/>
+      <c r="BG5" s="38"/>
+    </row>
+    <row r="6" spans="1:61" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2134,306 +2190,309 @@
       <c r="X6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="Y6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="Z6" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AB6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB6" s="8" t="s">
+      <c r="AC6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AD6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AD6" s="14" t="s">
+      <c r="AE6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF6" s="8" t="s">
+      <c r="AG6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AG6" s="8" t="s">
+      <c r="AH6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AI6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI6" s="18" t="s">
+      <c r="AJ6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AJ6" s="6" t="s">
+      <c r="AK6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AK6" s="6" t="s">
+      <c r="AL6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AL6" s="6" t="s">
+      <c r="AM6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AM6" s="9" t="s">
+      <c r="AN6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AN6" s="9" t="s">
+      <c r="AO6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AO6" s="23" t="s">
+      <c r="AP6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AP6" s="14" t="s">
+      <c r="AQ6" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AQ6" s="9" t="s">
+      <c r="AR6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AR6" s="14" t="s">
+      <c r="AS6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="AS6" s="14" t="s">
+      <c r="AT6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AT6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AV6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AV6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AW6" s="9" t="s">
+      <c r="AX6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AX6" s="9" t="s">
+      <c r="AY6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AY6" s="9" t="s">
+      <c r="AZ6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="AZ6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BB6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BC6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BD6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BE6" s="9" t="s">
+      <c r="BF6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BF6" s="14" t="s">
+      <c r="BG6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BG6" s="2" t="s">
+      <c r="BH6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BH6" s="4" t="s">
+      <c r="BI6" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="AO8" s="17"/>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
       <c r="AP8" s="17"/>
-    </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="AO9" s="17"/>
+      <c r="AQ8" s="17"/>
+    </row>
+    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
       <c r="AP9" s="17"/>
-    </row>
-    <row r="1048519" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="36:36" x14ac:dyDescent="0.25">
-      <c r="AJ1048575" s="13"/>
+      <c r="AQ9" s="17"/>
+    </row>
+    <row r="1048519" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AT5:BF5"/>
+    <mergeCell ref="AU5:BG5"/>
     <mergeCell ref="P5:W5"/>
-    <mergeCell ref="AO5:AR5"/>
-    <mergeCell ref="AA5:AH5"/>
-    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="AP5:AS5"/>
+    <mergeCell ref="AB5:AI5"/>
     <mergeCell ref="B5:I5"/>
-    <mergeCell ref="AI5:AN5"/>
+    <mergeCell ref="AJ5:AO5"/>
+    <mergeCell ref="X5:Z5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2443,7 +2502,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W1048573"/>
+  <dimension ref="A1:Y1048573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
@@ -2462,25 +2521,27 @@
     <col min="6" max="7" width="14.625" style="10" customWidth="1"/>
     <col min="9" max="9" width="9.25" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
-    <col min="11" max="11" width="15.75" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="11" style="13"/>
+    <col min="11" max="11" width="13.75" customWidth="1"/>
+    <col min="12" max="12" width="15.625" customWidth="1"/>
+    <col min="13" max="13" width="15.75" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -2492,8 +2553,10 @@
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2501,17 +2564,17 @@
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
-      <c r="N2"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P2"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="48" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="49"/>
       <c r="D3" s="50"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="51" t="s">
         <v>70</v>
       </c>
@@ -2522,12 +2585,11 @@
       <c r="M3" s="52"/>
       <c r="N3" s="52"/>
       <c r="O3" s="52"/>
-      <c r="P3" s="53"/>
-    </row>
-    <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="56"/>
+    </row>
+    <row r="4" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>58</v>
       </c>
@@ -2556,201 +2618,207 @@
         <v>63</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="R4" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="1048517" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048517" s="13"/>
-    </row>
-    <row r="1048518" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048518" s="13"/>
-    </row>
-    <row r="1048519" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L1048573" s="13"/>
+    <row r="1048517" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048517" s="13"/>
+    </row>
+    <row r="1048518" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048518" s="13"/>
+    </row>
+    <row r="1048519" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N1048573" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="H3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2760,7 +2828,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
@@ -2775,25 +2843,27 @@
     <col min="2" max="3" width="11.625" customWidth="1"/>
     <col min="6" max="6" width="26.625" customWidth="1"/>
     <col min="7" max="7" width="11.875" customWidth="1"/>
-    <col min="9" max="10" width="15.625" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="13" max="13" width="11.625" customWidth="1"/>
+    <col min="9" max="9" width="15.625" customWidth="1"/>
+    <col min="10" max="10" width="13.75" customWidth="1"/>
+    <col min="11" max="12" width="15.625" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="15" max="15" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="43"/>
+      <c r="C3" s="45"/>
       <c r="D3" s="48" t="s">
         <v>67</v>
       </c>
@@ -2807,9 +2877,11 @@
       <c r="J3" s="52"/>
       <c r="K3" s="52"/>
       <c r="L3" s="52"/>
-      <c r="M3" s="53"/>
-    </row>
-    <row r="4" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="56"/>
+    </row>
+    <row r="4" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -2837,16 +2909,22 @@
       <c r="I4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="O4" s="14" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2855,7 +2933,7 @@
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="G3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Flesh out characteristics in desk review workbooks
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D85A2-4FC0-49EA-AD11-CB31371E6A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED8302D-952E-49F2-A852-F24F8E33C761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <sheet name="Neighborhood Breakout" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BI$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BO$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
+    <pivotCache cacheId="14" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
+    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
+    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
       <text>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
       <text>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
       <text>
         <r>
           <rPr>
@@ -130,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{8035D120-422D-440A-8651-B1189F0D5374}">
+    <comment ref="AZ6" authorId="0" shapeId="0" xr:uid="{8035D120-422D-440A-8651-B1189F0D5374}">
       <text>
         <r>
           <rPr>
@@ -143,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{ECF27779-F8CB-4DDB-B47A-434BDB41AF51}">
+    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{ECF27779-F8CB-4DDB-B47A-434BDB41AF51}">
       <text>
         <r>
           <rPr>
@@ -156,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{BC63D4E8-13FE-4190-B049-8F73F08FC6D9}">
+    <comment ref="BB6" authorId="0" shapeId="0" xr:uid="{BC63D4E8-13FE-4190-B049-8F73F08FC6D9}">
       <text>
         <r>
           <rPr>
@@ -169,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{9201257A-E739-4445-9BA2-278E0B79DD9F}">
+    <comment ref="BC6" authorId="0" shapeId="0" xr:uid="{9201257A-E739-4445-9BA2-278E0B79DD9F}">
       <text>
         <r>
           <rPr>
@@ -182,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{617DE059-1ED7-4DF2-ADE1-DA1638E1B1B3}">
+    <comment ref="BD6" authorId="0" shapeId="0" xr:uid="{617DE059-1ED7-4DF2-ADE1-DA1638E1B1B3}">
       <text>
         <r>
           <rPr>
@@ -195,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY6" authorId="0" shapeId="0" xr:uid="{8D952257-05F3-458B-BB51-489A57E1F158}">
+    <comment ref="BE6" authorId="0" shapeId="0" xr:uid="{8D952257-05F3-458B-BB51-489A57E1F158}">
       <text>
         <r>
           <rPr>
@@ -209,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ6" authorId="0" shapeId="0" xr:uid="{C3739962-30FA-49E2-B79F-736E5AEB387B}">
+    <comment ref="BF6" authorId="0" shapeId="0" xr:uid="{C3739962-30FA-49E2-B79F-736E5AEB387B}">
       <text>
         <r>
           <rPr>
@@ -222,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{E8F31B7F-B8C2-4805-B053-4600780FD7A2}">
+    <comment ref="BG6" authorId="0" shapeId="0" xr:uid="{E8F31B7F-B8C2-4805-B053-4600780FD7A2}">
       <text>
         <r>
           <rPr>
@@ -254,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB6" authorId="0" shapeId="0" xr:uid="{9B95BB78-BBFA-4D08-898D-42D9F801F5C9}">
+    <comment ref="BH6" authorId="0" shapeId="0" xr:uid="{9B95BB78-BBFA-4D08-898D-42D9F801F5C9}">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BC6" authorId="0" shapeId="0" xr:uid="{23361704-B7DC-4593-A117-F2816AD735D7}">
+    <comment ref="BI6" authorId="0" shapeId="0" xr:uid="{23361704-B7DC-4593-A117-F2816AD735D7}">
       <text>
         <r>
           <rPr>
@@ -281,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BD6" authorId="0" shapeId="0" xr:uid="{AE640F8D-C8FE-48E7-A609-B0C718186353}">
+    <comment ref="BJ6" authorId="0" shapeId="0" xr:uid="{AE640F8D-C8FE-48E7-A609-B0C718186353}">
       <text>
         <r>
           <rPr>
@@ -294,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BE6" authorId="0" shapeId="0" xr:uid="{83117FFA-9BB4-4818-B2C6-422A3A943BE2}">
+    <comment ref="BK6" authorId="0" shapeId="0" xr:uid="{83117FFA-9BB4-4818-B2C6-422A3A943BE2}">
       <text>
         <r>
           <rPr>
@@ -307,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BF6" authorId="0" shapeId="0" xr:uid="{66E115B5-8547-42A9-A19E-183D9317F2A3}">
+    <comment ref="BL6" authorId="0" shapeId="0" xr:uid="{66E115B5-8547-42A9-A19E-183D9317F2A3}">
       <text>
         <r>
           <rPr>
@@ -320,7 +320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BG6" authorId="0" shapeId="0" xr:uid="{C26E7A69-3354-428E-BBFF-70904DE96781}">
+    <comment ref="BM6" authorId="0" shapeId="0" xr:uid="{C26E7A69-3354-428E-BBFF-70904DE96781}">
       <text>
         <r>
           <rPr>
@@ -343,7 +343,7 @@
     <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
-    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
       <text>
         <r>
           <rPr>
@@ -356,7 +356,43 @@
         </r>
       </text>
     </comment>
-    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
+    <comment ref="S4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color theme="1"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The number of commercial units in a card. Only present for class 212 parcels.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean Cochrane (Assessor)</author>
+  </authors>
+  <commentList>
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{631EDC07-49FD-49B1-BCE6-37E31B1ACEE7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color theme="1"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The number of apartments in a card. Only present for class 211 and 212 parcels.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{0C3D05B0-7DDF-44DF-B6CD-F791DF4DB5A2}">
       <text>
         <r>
           <rPr>
@@ -374,7 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="93">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -650,6 +686,9 @@
   </si>
   <si>
     <t>Bsmt. Finish</t>
+  </si>
+  <si>
+    <t>Central Air</t>
   </si>
 </sst>
 </file>
@@ -925,7 +964,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1069,6 +1108,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1099,11 +1141,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45343.715909837963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45349.476784375001" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
-  <cacheFields count="61">
+  <cacheFields count="67">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1214,6 +1256,24 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Year Built" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="# Beds" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Ext. Wall" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bsmt. Type" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bsmt. Finish" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Central Air" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Heat" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total        Bld. S. F." numFmtId="0">
@@ -1364,14 +1424,20 @@
     <m/>
     <m/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="61">
+  <pivotFields count="67">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="2">
@@ -1407,6 +1473,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1484,10 +1556,10 @@
   </colItems>
   <dataFields count="6">
     <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
-    <dataField name="Min of Total AV" fld="59" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total AV" fld="59" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total AV" fld="59" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of AV Difference" fld="60" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min of Total AV" fld="65" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="65" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="65" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="66" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1799,10 +1871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI1048575"/>
+  <dimension ref="A1:BO1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
@@ -1840,20 +1912,26 @@
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
     <col min="34" max="34" width="18.625" style="10" customWidth="1"/>
     <col min="35" max="35" width="13" style="16" customWidth="1"/>
-    <col min="39" max="41" width="11" style="13"/>
-    <col min="42" max="42" width="15.625" style="13" customWidth="1"/>
-    <col min="43" max="43" width="11" style="13"/>
-    <col min="44" max="44" width="15.625" style="13" customWidth="1"/>
-    <col min="45" max="46" width="11" style="13"/>
-    <col min="55" max="55" width="14" customWidth="1"/>
-    <col min="56" max="56" width="12.375" customWidth="1"/>
-    <col min="57" max="57" width="11.875" customWidth="1"/>
-    <col min="58" max="58" width="10.875" customWidth="1"/>
-    <col min="59" max="59" width="11.5" customWidth="1"/>
-    <col min="60" max="61" width="11" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="9.25" customWidth="1"/>
+    <col min="38" max="38" width="7.375" customWidth="1"/>
+    <col min="40" max="40" width="15.125" customWidth="1"/>
+    <col min="41" max="41" width="15.625" customWidth="1"/>
+    <col min="42" max="42" width="15.375" customWidth="1"/>
+    <col min="44" max="44" width="8.125" customWidth="1"/>
+    <col min="45" max="47" width="11" style="13"/>
+    <col min="48" max="48" width="15.625" style="13" customWidth="1"/>
+    <col min="49" max="49" width="11" style="13"/>
+    <col min="50" max="50" width="15.625" style="13" customWidth="1"/>
+    <col min="51" max="52" width="11" style="13"/>
+    <col min="61" max="61" width="14" customWidth="1"/>
+    <col min="62" max="62" width="12.375" customWidth="1"/>
+    <col min="63" max="63" width="11.875" customWidth="1"/>
+    <col min="64" max="64" width="10.875" customWidth="1"/>
+    <col min="65" max="65" width="11.5" customWidth="1"/>
+    <col min="66" max="67" width="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:67" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -1913,8 +1991,14 @@
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
       <c r="BG1" s="5"/>
-    </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
+      <c r="BJ1" s="5"/>
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="5"/>
+      <c r="BM1" s="5"/>
+    </row>
+    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1949,16 +2033,16 @@
       <c r="AG2"/>
       <c r="AH2"/>
       <c r="AI2"/>
-      <c r="AM2"/>
-      <c r="AN2"/>
-      <c r="AO2"/>
-      <c r="AP2"/>
-      <c r="AQ2"/>
-      <c r="AR2"/>
       <c r="AS2"/>
       <c r="AT2"/>
-    </row>
-    <row r="3" spans="1:61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+      <c r="AZ2"/>
+    </row>
+    <row r="3" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1994,16 +2078,16 @@
       <c r="AG3"/>
       <c r="AH3"/>
       <c r="AI3"/>
-      <c r="AM3"/>
-      <c r="AN3"/>
-      <c r="AO3"/>
-      <c r="AP3"/>
-      <c r="AQ3"/>
-      <c r="AR3"/>
       <c r="AS3"/>
       <c r="AT3"/>
-    </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AU3"/>
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3"/>
+      <c r="AY3"/>
+      <c r="AZ3"/>
+    </row>
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2037,13 +2121,19 @@
       <c r="AM4" s="19"/>
       <c r="AN4" s="19"/>
       <c r="AO4" s="19"/>
-      <c r="AP4"/>
-      <c r="AQ4"/>
-      <c r="AR4"/>
-      <c r="AS4"/>
-      <c r="AT4"/>
-    </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AP4" s="19"/>
+      <c r="AQ4" s="19"/>
+      <c r="AR4" s="19"/>
+      <c r="AS4" s="19"/>
+      <c r="AT4" s="19"/>
+      <c r="AU4" s="19"/>
+      <c r="AV4"/>
+      <c r="AW4"/>
+      <c r="AX4"/>
+      <c r="AY4"/>
+      <c r="AZ4"/>
+    </row>
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
         <v>67</v>
       </c>
@@ -2094,30 +2184,36 @@
       <c r="AM5" s="52"/>
       <c r="AN5" s="52"/>
       <c r="AO5" s="52"/>
-      <c r="AP5" s="42" t="s">
+      <c r="AP5" s="52"/>
+      <c r="AQ5" s="52"/>
+      <c r="AR5" s="52"/>
+      <c r="AS5" s="52"/>
+      <c r="AT5" s="52"/>
+      <c r="AU5" s="52"/>
+      <c r="AV5" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="AQ5" s="43"/>
-      <c r="AR5" s="43"/>
-      <c r="AS5" s="43"/>
-      <c r="AT5" s="21"/>
-      <c r="AU5" s="36" t="s">
+      <c r="AW5" s="43"/>
+      <c r="AX5" s="43"/>
+      <c r="AY5" s="43"/>
+      <c r="AZ5" s="21"/>
+      <c r="BA5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="AV5" s="37"/>
-      <c r="AW5" s="37"/>
-      <c r="AX5" s="37"/>
-      <c r="AY5" s="37"/>
-      <c r="AZ5" s="37"/>
-      <c r="BA5" s="37"/>
       <c r="BB5" s="37"/>
       <c r="BC5" s="37"/>
       <c r="BD5" s="37"/>
       <c r="BE5" s="37"/>
       <c r="BF5" s="37"/>
-      <c r="BG5" s="38"/>
-    </row>
-    <row r="6" spans="1:61" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="BG5" s="37"/>
+      <c r="BH5" s="37"/>
+      <c r="BI5" s="37"/>
+      <c r="BJ5" s="37"/>
+      <c r="BK5" s="37"/>
+      <c r="BL5" s="37"/>
+      <c r="BM5" s="38"/>
+    </row>
+    <row r="6" spans="1:67" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2227,271 +2323,289 @@
         <v>33</v>
       </c>
       <c r="AK6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO6" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AL6" s="6" t="s">
+      <c r="AR6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AM6" s="6" t="s">
+      <c r="AS6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AN6" s="9" t="s">
+      <c r="AT6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AO6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AP6" s="23" t="s">
+      <c r="AV6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AQ6" s="14" t="s">
+      <c r="AW6" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AR6" s="9" t="s">
+      <c r="AX6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AS6" s="14" t="s">
+      <c r="AY6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="AT6" s="14" t="s">
+      <c r="AZ6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AV6" s="9" t="s">
+      <c r="BB6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AW6" s="9" t="s">
+      <c r="BC6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AX6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AY6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AZ6" s="9" t="s">
+      <c r="BF6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BG6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BH6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BI6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="BD6" s="9" t="s">
+      <c r="BJ6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BE6" s="9" t="s">
+      <c r="BK6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BF6" s="9" t="s">
+      <c r="BL6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BG6" s="14" t="s">
+      <c r="BM6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BH6" s="2" t="s">
+      <c r="BN6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BI6" s="4" t="s">
+      <c r="BO6" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="AP8" s="17"/>
-      <c r="AQ8" s="17"/>
-    </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="AP9" s="17"/>
-      <c r="AQ9" s="17"/>
-    </row>
-    <row r="1048519" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048575" s="13"/>
+    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AV8" s="17"/>
+      <c r="AW8" s="17"/>
+    </row>
+    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AV9" s="17"/>
+      <c r="AW9" s="17"/>
+    </row>
+    <row r="1048519" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AU5:BG5"/>
+    <mergeCell ref="BA5:BM5"/>
     <mergeCell ref="P5:W5"/>
-    <mergeCell ref="AP5:AS5"/>
+    <mergeCell ref="AV5:AY5"/>
     <mergeCell ref="AB5:AI5"/>
     <mergeCell ref="B5:I5"/>
-    <mergeCell ref="AJ5:AO5"/>
+    <mergeCell ref="AJ5:AU5"/>
     <mergeCell ref="X5:Z5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2502,7 +2616,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y1048573"/>
+  <dimension ref="A1:Z1048573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
@@ -2523,12 +2637,13 @@
     <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="13.75" customWidth="1"/>
     <col min="12" max="12" width="15.625" customWidth="1"/>
-    <col min="13" max="13" width="15.75" customWidth="1"/>
-    <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="11" style="13"/>
+    <col min="13" max="13" width="14.125" customWidth="1"/>
+    <col min="14" max="14" width="15.75" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="32" t="s">
         <v>57</v>
       </c>
@@ -2542,7 +2657,7 @@
       <c r="J1" s="32"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
-      <c r="M1" s="5"/>
+      <c r="M1" s="30"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -2555,8 +2670,9 @@
       <c r="W1" s="5"/>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" s="5"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2564,9 +2680,9 @@
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
-      <c r="P2"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q2"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="48" t="s">
         <v>69</v>
       </c>
@@ -2587,9 +2703,13 @@
       <c r="O3" s="52"/>
       <c r="P3" s="52"/>
       <c r="Q3" s="52"/>
-      <c r="R3" s="56"/>
-    </row>
-    <row r="4" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="R3" s="52"/>
+      <c r="S3" s="56"/>
+    </row>
+    <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>58</v>
       </c>
@@ -2624,201 +2744,204 @@
         <v>91</v>
       </c>
       <c r="M4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="S4" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="1048517" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048517" s="13"/>
-    </row>
-    <row r="1048518" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048518" s="13"/>
-    </row>
-    <row r="1048519" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048573" s="13"/>
+    <row r="1048517" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048517" s="13"/>
+    </row>
+    <row r="1048518" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048518" s="13"/>
+    </row>
+    <row r="1048519" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048573" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H3:R3"/>
+    <mergeCell ref="H3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2827,8 +2950,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
@@ -2845,12 +2968,13 @@
     <col min="7" max="7" width="11.875" customWidth="1"/>
     <col min="9" max="9" width="15.625" customWidth="1"/>
     <col min="10" max="10" width="13.75" customWidth="1"/>
-    <col min="11" max="12" width="15.625" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="15" max="15" width="11.625" customWidth="1"/>
+    <col min="11" max="13" width="15.625" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="16" max="16" width="11.625" customWidth="1"/>
+    <col min="18" max="18" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="32" t="s">
         <v>66</v>
       </c>
@@ -2859,7 +2983,7 @@
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="44" t="s">
         <v>73</v>
       </c>
@@ -2879,9 +3003,12 @@
       <c r="L3" s="52"/>
       <c r="M3" s="52"/>
       <c r="N3" s="52"/>
-      <c r="O3" s="56"/>
-    </row>
-    <row r="4" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="52"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="56"/>
+    </row>
+    <row r="4" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -2915,17 +3042,26 @@
       <c r="K4" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="P4" s="8" t="s">
         <v>36</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2933,9 +3069,10 @@
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="G3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Flesh out characteristics in desk review workbooks (#218)
* Flesh out characteristics in desk review workbooks

* Use more idiomatic R way of summarizing chars in `export` stage

* Better handling of class code when summarizing and displaying char_apts and char_ncu in `export`
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D85A2-4FC0-49EA-AD11-CB31371E6A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED8302D-952E-49F2-A852-F24F8E33C761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <sheet name="Neighborhood Breakout" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BI$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BO$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
+    <pivotCache cacheId="14" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
+    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
+    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
       <text>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{BAC2DDCF-BD81-4E1D-BEBD-2108C20D7DEA}">
       <text>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{CE7918E0-AF03-4CF2-9C96-ECFE90BD81E6}">
       <text>
         <r>
           <rPr>
@@ -130,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{8035D120-422D-440A-8651-B1189F0D5374}">
+    <comment ref="AZ6" authorId="0" shapeId="0" xr:uid="{8035D120-422D-440A-8651-B1189F0D5374}">
       <text>
         <r>
           <rPr>
@@ -143,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{ECF27779-F8CB-4DDB-B47A-434BDB41AF51}">
+    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{ECF27779-F8CB-4DDB-B47A-434BDB41AF51}">
       <text>
         <r>
           <rPr>
@@ -156,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{BC63D4E8-13FE-4190-B049-8F73F08FC6D9}">
+    <comment ref="BB6" authorId="0" shapeId="0" xr:uid="{BC63D4E8-13FE-4190-B049-8F73F08FC6D9}">
       <text>
         <r>
           <rPr>
@@ -169,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{9201257A-E739-4445-9BA2-278E0B79DD9F}">
+    <comment ref="BC6" authorId="0" shapeId="0" xr:uid="{9201257A-E739-4445-9BA2-278E0B79DD9F}">
       <text>
         <r>
           <rPr>
@@ -182,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{617DE059-1ED7-4DF2-ADE1-DA1638E1B1B3}">
+    <comment ref="BD6" authorId="0" shapeId="0" xr:uid="{617DE059-1ED7-4DF2-ADE1-DA1638E1B1B3}">
       <text>
         <r>
           <rPr>
@@ -195,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY6" authorId="0" shapeId="0" xr:uid="{8D952257-05F3-458B-BB51-489A57E1F158}">
+    <comment ref="BE6" authorId="0" shapeId="0" xr:uid="{8D952257-05F3-458B-BB51-489A57E1F158}">
       <text>
         <r>
           <rPr>
@@ -209,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ6" authorId="0" shapeId="0" xr:uid="{C3739962-30FA-49E2-B79F-736E5AEB387B}">
+    <comment ref="BF6" authorId="0" shapeId="0" xr:uid="{C3739962-30FA-49E2-B79F-736E5AEB387B}">
       <text>
         <r>
           <rPr>
@@ -222,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA6" authorId="0" shapeId="0" xr:uid="{E8F31B7F-B8C2-4805-B053-4600780FD7A2}">
+    <comment ref="BG6" authorId="0" shapeId="0" xr:uid="{E8F31B7F-B8C2-4805-B053-4600780FD7A2}">
       <text>
         <r>
           <rPr>
@@ -254,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB6" authorId="0" shapeId="0" xr:uid="{9B95BB78-BBFA-4D08-898D-42D9F801F5C9}">
+    <comment ref="BH6" authorId="0" shapeId="0" xr:uid="{9B95BB78-BBFA-4D08-898D-42D9F801F5C9}">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BC6" authorId="0" shapeId="0" xr:uid="{23361704-B7DC-4593-A117-F2816AD735D7}">
+    <comment ref="BI6" authorId="0" shapeId="0" xr:uid="{23361704-B7DC-4593-A117-F2816AD735D7}">
       <text>
         <r>
           <rPr>
@@ -281,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BD6" authorId="0" shapeId="0" xr:uid="{AE640F8D-C8FE-48E7-A609-B0C718186353}">
+    <comment ref="BJ6" authorId="0" shapeId="0" xr:uid="{AE640F8D-C8FE-48E7-A609-B0C718186353}">
       <text>
         <r>
           <rPr>
@@ -294,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BE6" authorId="0" shapeId="0" xr:uid="{83117FFA-9BB4-4818-B2C6-422A3A943BE2}">
+    <comment ref="BK6" authorId="0" shapeId="0" xr:uid="{83117FFA-9BB4-4818-B2C6-422A3A943BE2}">
       <text>
         <r>
           <rPr>
@@ -307,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BF6" authorId="0" shapeId="0" xr:uid="{66E115B5-8547-42A9-A19E-183D9317F2A3}">
+    <comment ref="BL6" authorId="0" shapeId="0" xr:uid="{66E115B5-8547-42A9-A19E-183D9317F2A3}">
       <text>
         <r>
           <rPr>
@@ -320,7 +320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BG6" authorId="0" shapeId="0" xr:uid="{C26E7A69-3354-428E-BBFF-70904DE96781}">
+    <comment ref="BM6" authorId="0" shapeId="0" xr:uid="{C26E7A69-3354-428E-BBFF-70904DE96781}">
       <text>
         <r>
           <rPr>
@@ -343,7 +343,7 @@
     <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
-    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{03B1BBD3-705D-427B-9A63-A114BEFB7A0C}">
       <text>
         <r>
           <rPr>
@@ -356,7 +356,43 @@
         </r>
       </text>
     </comment>
-    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
+    <comment ref="S4" authorId="0" shapeId="0" xr:uid="{AED861D1-6C64-4E76-9DD1-C8067007C736}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color theme="1"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The number of commercial units in a card. Only present for class 212 parcels.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean Cochrane (Assessor)</author>
+  </authors>
+  <commentList>
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{631EDC07-49FD-49B1-BCE6-37E31B1ACEE7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color theme="1"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The number of apartments in a card. Only present for class 211 and 212 parcels.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{0C3D05B0-7DDF-44DF-B6CD-F791DF4DB5A2}">
       <text>
         <r>
           <rPr>
@@ -374,7 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="93">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -650,6 +686,9 @@
   </si>
   <si>
     <t>Bsmt. Finish</t>
+  </si>
+  <si>
+    <t>Central Air</t>
   </si>
 </sst>
 </file>
@@ -925,7 +964,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1069,6 +1108,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1099,11 +1141,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45343.715909837963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45349.476784375001" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
-  <cacheFields count="61">
+  <cacheFields count="67">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1214,6 +1256,24 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Year Built" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="# Beds" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Ext. Wall" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bsmt. Type" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bsmt. Finish" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Central Air" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Heat" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total        Bld. S. F." numFmtId="0">
@@ -1364,14 +1424,20 @@
     <m/>
     <m/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="61">
+  <pivotFields count="67">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="2">
@@ -1407,6 +1473,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1484,10 +1556,10 @@
   </colItems>
   <dataFields count="6">
     <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
-    <dataField name="Min of Total AV" fld="59" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total AV" fld="59" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total AV" fld="59" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of AV Difference" fld="60" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min of Total AV" fld="65" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="65" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="65" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="66" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1799,10 +1871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI1048575"/>
+  <dimension ref="A1:BO1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
@@ -1840,20 +1912,26 @@
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
     <col min="34" max="34" width="18.625" style="10" customWidth="1"/>
     <col min="35" max="35" width="13" style="16" customWidth="1"/>
-    <col min="39" max="41" width="11" style="13"/>
-    <col min="42" max="42" width="15.625" style="13" customWidth="1"/>
-    <col min="43" max="43" width="11" style="13"/>
-    <col min="44" max="44" width="15.625" style="13" customWidth="1"/>
-    <col min="45" max="46" width="11" style="13"/>
-    <col min="55" max="55" width="14" customWidth="1"/>
-    <col min="56" max="56" width="12.375" customWidth="1"/>
-    <col min="57" max="57" width="11.875" customWidth="1"/>
-    <col min="58" max="58" width="10.875" customWidth="1"/>
-    <col min="59" max="59" width="11.5" customWidth="1"/>
-    <col min="60" max="61" width="11" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="9.25" customWidth="1"/>
+    <col min="38" max="38" width="7.375" customWidth="1"/>
+    <col min="40" max="40" width="15.125" customWidth="1"/>
+    <col min="41" max="41" width="15.625" customWidth="1"/>
+    <col min="42" max="42" width="15.375" customWidth="1"/>
+    <col min="44" max="44" width="8.125" customWidth="1"/>
+    <col min="45" max="47" width="11" style="13"/>
+    <col min="48" max="48" width="15.625" style="13" customWidth="1"/>
+    <col min="49" max="49" width="11" style="13"/>
+    <col min="50" max="50" width="15.625" style="13" customWidth="1"/>
+    <col min="51" max="52" width="11" style="13"/>
+    <col min="61" max="61" width="14" customWidth="1"/>
+    <col min="62" max="62" width="12.375" customWidth="1"/>
+    <col min="63" max="63" width="11.875" customWidth="1"/>
+    <col min="64" max="64" width="10.875" customWidth="1"/>
+    <col min="65" max="65" width="11.5" customWidth="1"/>
+    <col min="66" max="67" width="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:67" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -1913,8 +1991,14 @@
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
       <c r="BG1" s="5"/>
-    </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
+      <c r="BJ1" s="5"/>
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="5"/>
+      <c r="BM1" s="5"/>
+    </row>
+    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1949,16 +2033,16 @@
       <c r="AG2"/>
       <c r="AH2"/>
       <c r="AI2"/>
-      <c r="AM2"/>
-      <c r="AN2"/>
-      <c r="AO2"/>
-      <c r="AP2"/>
-      <c r="AQ2"/>
-      <c r="AR2"/>
       <c r="AS2"/>
       <c r="AT2"/>
-    </row>
-    <row r="3" spans="1:61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+      <c r="AZ2"/>
+    </row>
+    <row r="3" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1994,16 +2078,16 @@
       <c r="AG3"/>
       <c r="AH3"/>
       <c r="AI3"/>
-      <c r="AM3"/>
-      <c r="AN3"/>
-      <c r="AO3"/>
-      <c r="AP3"/>
-      <c r="AQ3"/>
-      <c r="AR3"/>
       <c r="AS3"/>
       <c r="AT3"/>
-    </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AU3"/>
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3"/>
+      <c r="AY3"/>
+      <c r="AZ3"/>
+    </row>
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2037,13 +2121,19 @@
       <c r="AM4" s="19"/>
       <c r="AN4" s="19"/>
       <c r="AO4" s="19"/>
-      <c r="AP4"/>
-      <c r="AQ4"/>
-      <c r="AR4"/>
-      <c r="AS4"/>
-      <c r="AT4"/>
-    </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AP4" s="19"/>
+      <c r="AQ4" s="19"/>
+      <c r="AR4" s="19"/>
+      <c r="AS4" s="19"/>
+      <c r="AT4" s="19"/>
+      <c r="AU4" s="19"/>
+      <c r="AV4"/>
+      <c r="AW4"/>
+      <c r="AX4"/>
+      <c r="AY4"/>
+      <c r="AZ4"/>
+    </row>
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
         <v>67</v>
       </c>
@@ -2094,30 +2184,36 @@
       <c r="AM5" s="52"/>
       <c r="AN5" s="52"/>
       <c r="AO5" s="52"/>
-      <c r="AP5" s="42" t="s">
+      <c r="AP5" s="52"/>
+      <c r="AQ5" s="52"/>
+      <c r="AR5" s="52"/>
+      <c r="AS5" s="52"/>
+      <c r="AT5" s="52"/>
+      <c r="AU5" s="52"/>
+      <c r="AV5" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="AQ5" s="43"/>
-      <c r="AR5" s="43"/>
-      <c r="AS5" s="43"/>
-      <c r="AT5" s="21"/>
-      <c r="AU5" s="36" t="s">
+      <c r="AW5" s="43"/>
+      <c r="AX5" s="43"/>
+      <c r="AY5" s="43"/>
+      <c r="AZ5" s="21"/>
+      <c r="BA5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="AV5" s="37"/>
-      <c r="AW5" s="37"/>
-      <c r="AX5" s="37"/>
-      <c r="AY5" s="37"/>
-      <c r="AZ5" s="37"/>
-      <c r="BA5" s="37"/>
       <c r="BB5" s="37"/>
       <c r="BC5" s="37"/>
       <c r="BD5" s="37"/>
       <c r="BE5" s="37"/>
       <c r="BF5" s="37"/>
-      <c r="BG5" s="38"/>
-    </row>
-    <row r="6" spans="1:61" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="BG5" s="37"/>
+      <c r="BH5" s="37"/>
+      <c r="BI5" s="37"/>
+      <c r="BJ5" s="37"/>
+      <c r="BK5" s="37"/>
+      <c r="BL5" s="37"/>
+      <c r="BM5" s="38"/>
+    </row>
+    <row r="6" spans="1:67" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2227,271 +2323,289 @@
         <v>33</v>
       </c>
       <c r="AK6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO6" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AL6" s="6" t="s">
+      <c r="AR6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AM6" s="6" t="s">
+      <c r="AS6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AN6" s="9" t="s">
+      <c r="AT6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AO6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AP6" s="23" t="s">
+      <c r="AV6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AQ6" s="14" t="s">
+      <c r="AW6" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AR6" s="9" t="s">
+      <c r="AX6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AS6" s="14" t="s">
+      <c r="AY6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="AT6" s="14" t="s">
+      <c r="AZ6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="BA6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AV6" s="9" t="s">
+      <c r="BB6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AW6" s="9" t="s">
+      <c r="BC6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AX6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AY6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AZ6" s="9" t="s">
+      <c r="BF6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BG6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BH6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BI6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="BD6" s="9" t="s">
+      <c r="BJ6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BE6" s="9" t="s">
+      <c r="BK6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BF6" s="9" t="s">
+      <c r="BL6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BG6" s="14" t="s">
+      <c r="BM6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BH6" s="2" t="s">
+      <c r="BN6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BI6" s="4" t="s">
+      <c r="BO6" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="AP8" s="17"/>
-      <c r="AQ8" s="17"/>
-    </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="AP9" s="17"/>
-      <c r="AQ9" s="17"/>
-    </row>
-    <row r="1048519" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048575" s="13"/>
+    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AV8" s="17"/>
+      <c r="AW8" s="17"/>
+    </row>
+    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="AV9" s="17"/>
+      <c r="AW9" s="17"/>
+    </row>
+    <row r="1048519" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="43:43" x14ac:dyDescent="0.25">
+      <c r="AQ1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
-    <mergeCell ref="AU5:BG5"/>
+    <mergeCell ref="BA5:BM5"/>
     <mergeCell ref="P5:W5"/>
-    <mergeCell ref="AP5:AS5"/>
+    <mergeCell ref="AV5:AY5"/>
     <mergeCell ref="AB5:AI5"/>
     <mergeCell ref="B5:I5"/>
-    <mergeCell ref="AJ5:AO5"/>
+    <mergeCell ref="AJ5:AU5"/>
     <mergeCell ref="X5:Z5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2502,7 +2616,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y1048573"/>
+  <dimension ref="A1:Z1048573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
@@ -2523,12 +2637,13 @@
     <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="13.75" customWidth="1"/>
     <col min="12" max="12" width="15.625" customWidth="1"/>
-    <col min="13" max="13" width="15.75" customWidth="1"/>
-    <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="11" style="13"/>
+    <col min="13" max="13" width="14.125" customWidth="1"/>
+    <col min="14" max="14" width="15.75" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="32" t="s">
         <v>57</v>
       </c>
@@ -2542,7 +2657,7 @@
       <c r="J1" s="32"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
-      <c r="M1" s="5"/>
+      <c r="M1" s="30"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -2555,8 +2670,9 @@
       <c r="W1" s="5"/>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" s="5"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2564,9 +2680,9 @@
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
-      <c r="P2"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q2"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="48" t="s">
         <v>69</v>
       </c>
@@ -2587,9 +2703,13 @@
       <c r="O3" s="52"/>
       <c r="P3" s="52"/>
       <c r="Q3" s="52"/>
-      <c r="R3" s="56"/>
-    </row>
-    <row r="4" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="R3" s="52"/>
+      <c r="S3" s="56"/>
+    </row>
+    <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>58</v>
       </c>
@@ -2624,201 +2744,204 @@
         <v>91</v>
       </c>
       <c r="M4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="S4" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="1048517" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048517" s="13"/>
-    </row>
-    <row r="1048518" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048518" s="13"/>
-    </row>
-    <row r="1048519" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N1048573" s="13"/>
+    <row r="1048517" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048517" s="13"/>
+    </row>
+    <row r="1048518" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048518" s="13"/>
+    </row>
+    <row r="1048519" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O1048573" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H3:R3"/>
+    <mergeCell ref="H3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2827,8 +2950,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
@@ -2845,12 +2968,13 @@
     <col min="7" max="7" width="11.875" customWidth="1"/>
     <col min="9" max="9" width="15.625" customWidth="1"/>
     <col min="10" max="10" width="13.75" customWidth="1"/>
-    <col min="11" max="12" width="15.625" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="15" max="15" width="11.625" customWidth="1"/>
+    <col min="11" max="13" width="15.625" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="16" max="16" width="11.625" customWidth="1"/>
+    <col min="18" max="18" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="32" t="s">
         <v>66</v>
       </c>
@@ -2859,7 +2983,7 @@
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="44" t="s">
         <v>73</v>
       </c>
@@ -2879,9 +3003,12 @@
       <c r="L3" s="52"/>
       <c r="M3" s="52"/>
       <c r="N3" s="52"/>
-      <c r="O3" s="56"/>
-    </row>
-    <row r="4" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="52"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="56"/>
+    </row>
+    <row r="4" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -2915,17 +3042,26 @@
       <c r="K4" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="P4" s="8" t="s">
         <v>36</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2933,9 +3069,10 @@
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="G3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Finalize ad-hoc DR sheet with new sales
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED8302D-952E-49F2-A852-F24F8E33C761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B0BEF7-F669-4ED3-A3FA-43E21E7D68A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <sheet name="Neighborhood Breakout" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BO$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BQ$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId5"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -58,7 +58,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>The estimated value for the parcel (Total) divided by the amount of its most recent sale, if one exists (Sale Amount 1). Empty if no recent sales exist. If a recent sale exists but is flagged as a non-arm's-length sale, this ratio will likely not be accurate.</t>
         </r>
@@ -410,7 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -689,6 +689,15 @@
   </si>
   <si>
     <t>Central Air</t>
+  </si>
+  <si>
+    <t>Sale Added Later 1</t>
+  </si>
+  <si>
+    <t>Sale Added Later 2</t>
+  </si>
+  <si>
+    <t>Sales Added Later</t>
   </si>
 </sst>
 </file>
@@ -769,13 +778,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -827,6 +837,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD1D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -964,7 +980,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1031,6 +1047,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1141,11 +1163,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45349.476784375001" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45364.702611458335" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
-  <cacheFields count="67">
+  <cacheFields count="69">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1343,6 +1365,12 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Critical Char. Missing" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Added Later 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Added Later 2" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total AV" numFmtId="0">
@@ -1430,14 +1458,16 @@
     <m/>
     <m/>
     <m/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="67">
+  <pivotFields count="69">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="2">
@@ -1473,6 +1503,8 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1556,10 +1588,10 @@
   </colItems>
   <dataFields count="6">
     <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
-    <dataField name="Min of Total AV" fld="65" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total AV" fld="65" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total AV" fld="65" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of AV Difference" fld="66" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min of Total AV" fld="67" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="67" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="67" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="68" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1871,13 +1903,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BO1048575"/>
+  <dimension ref="A1:BQ1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1927,21 +1959,21 @@
     <col min="62" max="62" width="12.375" customWidth="1"/>
     <col min="63" max="63" width="11.875" customWidth="1"/>
     <col min="64" max="64" width="10.875" customWidth="1"/>
-    <col min="65" max="65" width="11.5" customWidth="1"/>
-    <col min="66" max="67" width="11" hidden="1" customWidth="1"/>
+    <col min="65" max="67" width="11.5" customWidth="1"/>
+    <col min="68" max="69" width="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:69" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1997,8 +2029,10 @@
       <c r="BK1" s="5"/>
       <c r="BL1" s="5"/>
       <c r="BM1" s="5"/>
-    </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BN1" s="5"/>
+      <c r="BO1" s="5"/>
+    </row>
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2042,13 +2076,13 @@
       <c r="AY2"/>
       <c r="AZ2"/>
     </row>
-    <row r="3" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2087,7 +2121,7 @@
       <c r="AY3"/>
       <c r="AZ3"/>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2133,87 +2167,91 @@
       <c r="AY4"/>
       <c r="AZ4"/>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B5" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="40"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="53" t="s">
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="55"/>
+      <c r="Y5" s="56"/>
+      <c r="Z5" s="57"/>
       <c r="AA5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AB5" s="44" t="s">
+      <c r="AB5" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="45"/>
-      <c r="AD5" s="45"/>
-      <c r="AE5" s="46"/>
-      <c r="AF5" s="45"/>
-      <c r="AG5" s="45"/>
-      <c r="AH5" s="46"/>
-      <c r="AI5" s="47"/>
-      <c r="AJ5" s="51" t="s">
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="48"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="48"/>
+      <c r="AI5" s="49"/>
+      <c r="AJ5" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="AK5" s="52"/>
-      <c r="AL5" s="52"/>
-      <c r="AM5" s="52"/>
-      <c r="AN5" s="52"/>
-      <c r="AO5" s="52"/>
-      <c r="AP5" s="52"/>
-      <c r="AQ5" s="52"/>
-      <c r="AR5" s="52"/>
-      <c r="AS5" s="52"/>
-      <c r="AT5" s="52"/>
-      <c r="AU5" s="52"/>
-      <c r="AV5" s="42" t="s">
+      <c r="AK5" s="54"/>
+      <c r="AL5" s="54"/>
+      <c r="AM5" s="54"/>
+      <c r="AN5" s="54"/>
+      <c r="AO5" s="54"/>
+      <c r="AP5" s="54"/>
+      <c r="AQ5" s="54"/>
+      <c r="AR5" s="54"/>
+      <c r="AS5" s="54"/>
+      <c r="AT5" s="54"/>
+      <c r="AU5" s="54"/>
+      <c r="AV5" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="AW5" s="43"/>
-      <c r="AX5" s="43"/>
-      <c r="AY5" s="43"/>
+      <c r="AW5" s="45"/>
+      <c r="AX5" s="45"/>
+      <c r="AY5" s="45"/>
       <c r="AZ5" s="21"/>
-      <c r="BA5" s="36" t="s">
+      <c r="BA5" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="BB5" s="37"/>
-      <c r="BC5" s="37"/>
-      <c r="BD5" s="37"/>
-      <c r="BE5" s="37"/>
-      <c r="BF5" s="37"/>
-      <c r="BG5" s="37"/>
-      <c r="BH5" s="37"/>
-      <c r="BI5" s="37"/>
-      <c r="BJ5" s="37"/>
-      <c r="BK5" s="37"/>
-      <c r="BL5" s="37"/>
-      <c r="BM5" s="38"/>
-    </row>
-    <row r="6" spans="1:67" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="BB5" s="39"/>
+      <c r="BC5" s="39"/>
+      <c r="BD5" s="39"/>
+      <c r="BE5" s="39"/>
+      <c r="BF5" s="39"/>
+      <c r="BG5" s="39"/>
+      <c r="BH5" s="39"/>
+      <c r="BI5" s="39"/>
+      <c r="BJ5" s="39"/>
+      <c r="BK5" s="39"/>
+      <c r="BL5" s="39"/>
+      <c r="BM5" s="40"/>
+      <c r="BN5" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="BO5" s="32"/>
+    </row>
+    <row r="6" spans="1:69" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2409,18 +2447,24 @@
       <c r="BM6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BN6" s="2" t="s">
+      <c r="BN6" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="BO6" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="BP6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BO6" s="4" t="s">
+      <c r="BQ6" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
       <c r="AV8" s="17"/>
       <c r="AW8" s="17"/>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="AV9" s="17"/>
       <c r="AW9" s="17"/>
     </row>
@@ -2596,7 +2640,8 @@
       <c r="AQ1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="BN5:BO5"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
@@ -2644,17 +2689,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
@@ -2683,28 +2728,28 @@
       <c r="Q2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="51" t="s">
+      <c r="C3" s="51"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="56"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="58"/>
     </row>
     <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2975,38 +3020,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="48" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51" t="s">
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="56"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="58"/>
     </row>
     <row r="4" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">

</xml_diff>

<commit_message>
Revert "Finalize ad-hoc DR sheet with new sales"
This reverts commit 47fb94a9f9d81e60ccb449b53fa61ae4ecfe3c37.
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B0BEF7-F669-4ED3-A3FA-43E21E7D68A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED8302D-952E-49F2-A852-F24F8E33C761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <sheet name="Neighborhood Breakout" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BQ$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BO$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
+    <pivotCache cacheId="14" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -58,7 +58,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>The estimated value for the parcel (Total) divided by the amount of its most recent sale, if one exists (Sale Amount 1). Empty if no recent sales exist. If a recent sale exists but is flagged as a non-arm's-length sale, this ratio will likely not be accurate.</t>
         </r>
@@ -410,7 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="93">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -689,15 +689,6 @@
   </si>
   <si>
     <t>Central Air</t>
-  </si>
-  <si>
-    <t>Sale Added Later 1</t>
-  </si>
-  <si>
-    <t>Sale Added Later 2</t>
-  </si>
-  <si>
-    <t>Sales Added Later</t>
   </si>
 </sst>
 </file>
@@ -778,14 +769,13 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -837,12 +827,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD1D1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -980,7 +964,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1047,12 +1031,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1163,11 +1141,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45364.702611458335" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45349.476784375001" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
-  <cacheFields count="69">
+  <cacheFields count="67">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1365,12 +1343,6 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Critical Char. Missing" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Sale Added Later 1" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Sale Added Later 2" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total AV" numFmtId="0">
@@ -1458,16 +1430,14 @@
     <m/>
     <m/>
     <m/>
-    <m/>
-    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="69">
+  <pivotFields count="67">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="2">
@@ -1503,8 +1473,6 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1588,10 +1556,10 @@
   </colItems>
   <dataFields count="6">
     <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
-    <dataField name="Min of Total AV" fld="67" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total AV" fld="67" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total AV" fld="67" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of AV Difference" fld="68" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min of Total AV" fld="65" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="65" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="65" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="66" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1903,13 +1871,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BQ1048575"/>
+  <dimension ref="A1:BO1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1959,21 +1927,21 @@
     <col min="62" max="62" width="12.375" customWidth="1"/>
     <col min="63" max="63" width="11.875" customWidth="1"/>
     <col min="64" max="64" width="10.875" customWidth="1"/>
-    <col min="65" max="67" width="11.5" customWidth="1"/>
-    <col min="68" max="69" width="11" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="11.5" customWidth="1"/>
+    <col min="66" max="67" width="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:67" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -2029,10 +1997,8 @@
       <c r="BK1" s="5"/>
       <c r="BL1" s="5"/>
       <c r="BM1" s="5"/>
-      <c r="BN1" s="5"/>
-      <c r="BO1" s="5"/>
-    </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2076,13 +2042,13 @@
       <c r="AY2"/>
       <c r="AZ2"/>
     </row>
-    <row r="3" spans="1:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2121,7 +2087,7 @@
       <c r="AY3"/>
       <c r="AZ3"/>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2167,91 +2133,87 @@
       <c r="AY4"/>
       <c r="AZ4"/>
     </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="B5" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="42"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="55" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="Y5" s="56"/>
-      <c r="Z5" s="57"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="55"/>
       <c r="AA5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AB5" s="46" t="s">
+      <c r="AB5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="47"/>
-      <c r="AD5" s="47"/>
-      <c r="AE5" s="48"/>
-      <c r="AF5" s="47"/>
-      <c r="AG5" s="47"/>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="49"/>
-      <c r="AJ5" s="53" t="s">
+      <c r="AC5" s="45"/>
+      <c r="AD5" s="45"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="45"/>
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AK5" s="54"/>
-      <c r="AL5" s="54"/>
-      <c r="AM5" s="54"/>
-      <c r="AN5" s="54"/>
-      <c r="AO5" s="54"/>
-      <c r="AP5" s="54"/>
-      <c r="AQ5" s="54"/>
-      <c r="AR5" s="54"/>
-      <c r="AS5" s="54"/>
-      <c r="AT5" s="54"/>
-      <c r="AU5" s="54"/>
-      <c r="AV5" s="44" t="s">
+      <c r="AK5" s="52"/>
+      <c r="AL5" s="52"/>
+      <c r="AM5" s="52"/>
+      <c r="AN5" s="52"/>
+      <c r="AO5" s="52"/>
+      <c r="AP5" s="52"/>
+      <c r="AQ5" s="52"/>
+      <c r="AR5" s="52"/>
+      <c r="AS5" s="52"/>
+      <c r="AT5" s="52"/>
+      <c r="AU5" s="52"/>
+      <c r="AV5" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="AW5" s="45"/>
-      <c r="AX5" s="45"/>
-      <c r="AY5" s="45"/>
+      <c r="AW5" s="43"/>
+      <c r="AX5" s="43"/>
+      <c r="AY5" s="43"/>
       <c r="AZ5" s="21"/>
-      <c r="BA5" s="38" t="s">
+      <c r="BA5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="BB5" s="39"/>
-      <c r="BC5" s="39"/>
-      <c r="BD5" s="39"/>
-      <c r="BE5" s="39"/>
-      <c r="BF5" s="39"/>
-      <c r="BG5" s="39"/>
-      <c r="BH5" s="39"/>
-      <c r="BI5" s="39"/>
-      <c r="BJ5" s="39"/>
-      <c r="BK5" s="39"/>
-      <c r="BL5" s="39"/>
-      <c r="BM5" s="40"/>
-      <c r="BN5" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="BO5" s="32"/>
-    </row>
-    <row r="6" spans="1:69" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="BB5" s="37"/>
+      <c r="BC5" s="37"/>
+      <c r="BD5" s="37"/>
+      <c r="BE5" s="37"/>
+      <c r="BF5" s="37"/>
+      <c r="BG5" s="37"/>
+      <c r="BH5" s="37"/>
+      <c r="BI5" s="37"/>
+      <c r="BJ5" s="37"/>
+      <c r="BK5" s="37"/>
+      <c r="BL5" s="37"/>
+      <c r="BM5" s="38"/>
+    </row>
+    <row r="6" spans="1:67" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2447,24 +2409,18 @@
       <c r="BM6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BN6" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BO6" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="BP6" s="2" t="s">
+      <c r="BN6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BQ6" s="4" t="s">
+      <c r="BO6" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
       <c r="AV8" s="17"/>
       <c r="AW8" s="17"/>
     </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
       <c r="AV9" s="17"/>
       <c r="AW9" s="17"/>
     </row>
@@ -2640,8 +2596,7 @@
       <c r="AQ1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="BN5:BO5"/>
+  <mergeCells count="10">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="J5:O5"/>
@@ -2689,17 +2644,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
@@ -2728,28 +2683,28 @@
       <c r="Q2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="53" t="s">
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="58"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="56"/>
     </row>
     <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -3020,38 +2975,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="50" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="53" t="s">
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="58"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="56"/>
     </row>
     <row r="4" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">

</xml_diff>

<commit_message>
Remove year filter from export code, we don't need it
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F89945F-D3A9-4353-9F7D-DA025522DF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420304A6-F863-4354-90DD-E847C8870184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -342,7 +342,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Flag indicating that the PIN has at least one assessable permit in the past 3 years. Only counts permits that we processed prior to the beginning of desk review.</t>
+          <t>Flag indicating that the PIN has at least one assessable permit in the past 3 years. Only counts permits prior to January 1st of the current assessment year.</t>
         </r>
       </text>
     </comment>
@@ -704,7 +704,7 @@
     <t>Central Air</t>
   </si>
   <si>
-    <t>Assessable Permit in Past 3 Years</t>
+    <t>Recent Assessable Permit</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1157,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45699.660879745374" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45699.667643518522" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>

</xml_diff>

<commit_message>
Add flag to desk review workbook for assessable permit in past 3 years (#345)
* Add flag to desk review workbook for assessable permit in past 3 years

* Remove year filter from export code, we don't need it
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED8302D-952E-49F2-A852-F24F8E33C761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420304A6-F863-4354-90DD-E847C8870184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <sheet name="Neighborhood Breakout" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BO$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BP$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId5"/>
+    <pivotCache cacheId="5" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -333,6 +333,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="BN6" authorId="0" shapeId="0" xr:uid="{ACF72B43-181F-4EDF-AB31-F37EC8467982}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Flag indicating that the PIN has at least one assessable permit in the past 3 years. Only counts permits prior to January 1st of the current assessment year.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -410,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="94">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -689,6 +702,9 @@
   </si>
   <si>
     <t>Central Air</t>
+  </si>
+  <si>
+    <t>Recent Assessable Permit</t>
   </si>
 </sst>
 </file>
@@ -1032,6 +1048,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1051,9 +1070,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1141,11 +1157,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45349.476784375001" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45699.667643518522" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
-  <cacheFields count="67">
+  <cacheFields count="68">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1343,6 +1359,9 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Critical Char. Missing" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Assessable Permit in Past 3 Years" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total AV" numFmtId="0">
@@ -1430,14 +1449,15 @@
     <m/>
     <m/>
     <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="67">
+  <pivotFields count="68">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="2">
@@ -1473,6 +1493,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1556,10 +1577,10 @@
   </colItems>
   <dataFields count="6">
     <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
-    <dataField name="Min of Total AV" fld="65" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total AV" fld="65" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total AV" fld="65" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of AV Difference" fld="66" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min of Total AV" fld="66" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="66" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="66" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="67" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1575,9 +1596,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1615,7 +1636,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1721,7 +1742,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1863,7 +1884,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1871,13 +1892,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BO1048575"/>
+  <dimension ref="A1:BP1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1928,20 +1949,22 @@
     <col min="63" max="63" width="11.875" customWidth="1"/>
     <col min="64" max="64" width="10.875" customWidth="1"/>
     <col min="65" max="65" width="11.5" customWidth="1"/>
-    <col min="66" max="67" width="11" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="13" customWidth="1"/>
+    <col min="67" max="67" width="7.75" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="9.375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:68" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1997,8 +2020,9 @@
       <c r="BK1" s="5"/>
       <c r="BL1" s="5"/>
       <c r="BM1" s="5"/>
-    </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BN1" s="5"/>
+    </row>
+    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2042,13 +2066,13 @@
       <c r="AY2"/>
       <c r="AZ2"/>
     </row>
-    <row r="3" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2087,7 +2111,7 @@
       <c r="AY3"/>
       <c r="AZ3"/>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2133,7 +2157,7 @@
       <c r="AY4"/>
       <c r="AZ4"/>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
         <v>67</v>
       </c>
@@ -2144,12 +2168,12 @@
       <c r="G5" s="49"/>
       <c r="H5" s="49"/>
       <c r="I5" s="50"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="35"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
       <c r="P5" s="39"/>
       <c r="Q5" s="40"/>
       <c r="R5" s="40"/>
@@ -2197,23 +2221,24 @@
       <c r="AX5" s="43"/>
       <c r="AY5" s="43"/>
       <c r="AZ5" s="21"/>
-      <c r="BA5" s="36" t="s">
+      <c r="BA5" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="BB5" s="37"/>
-      <c r="BC5" s="37"/>
-      <c r="BD5" s="37"/>
-      <c r="BE5" s="37"/>
-      <c r="BF5" s="37"/>
-      <c r="BG5" s="37"/>
-      <c r="BH5" s="37"/>
-      <c r="BI5" s="37"/>
-      <c r="BJ5" s="37"/>
-      <c r="BK5" s="37"/>
-      <c r="BL5" s="37"/>
+      <c r="BB5" s="38"/>
+      <c r="BC5" s="38"/>
+      <c r="BD5" s="38"/>
+      <c r="BE5" s="38"/>
+      <c r="BF5" s="38"/>
+      <c r="BG5" s="38"/>
+      <c r="BH5" s="38"/>
+      <c r="BI5" s="38"/>
+      <c r="BJ5" s="38"/>
+      <c r="BK5" s="38"/>
+      <c r="BL5" s="38"/>
       <c r="BM5" s="38"/>
-    </row>
-    <row r="6" spans="1:67" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="BN5" s="31"/>
+    </row>
+    <row r="6" spans="1:68" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2406,21 +2431,24 @@
       <c r="BL6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BM6" s="14" t="s">
+      <c r="BM6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="BN6" s="2" t="s">
+      <c r="BN6" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="BO6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="BO6" s="4" t="s">
+      <c r="BP6" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
       <c r="AV8" s="17"/>
       <c r="AW8" s="17"/>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
       <c r="AV9" s="17"/>
       <c r="AW9" s="17"/>
     </row>
@@ -2644,17 +2672,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
@@ -2975,13 +3003,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="44" t="s">

</xml_diff>

<commit_message>
Edit template and rework solution
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miwagne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED8302D-952E-49F2-A852-F24F8E33C761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9488BA9D-E96B-47B4-BFB0-0F23ACC4E4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29955" yWindow="3090" windowWidth="26595" windowHeight="11775" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId5"/>
+    <pivotCache cacheId="13" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -379,7 +379,7 @@
     <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
-    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{631EDC07-49FD-49B1-BCE6-37E31B1ACEE7}">
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{631EDC07-49FD-49B1-BCE6-37E31B1ACEE7}">
       <text>
         <r>
           <rPr>
@@ -392,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{0C3D05B0-7DDF-44DF-B6CD-F791DF4DB5A2}">
+    <comment ref="S4" authorId="0" shapeId="0" xr:uid="{0C3D05B0-7DDF-44DF-B6CD-F791DF4DB5A2}">
       <text>
         <r>
           <rPr>
@@ -410,7 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="94">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -689,6 +689,9 @@
   </si>
   <si>
     <t>Central Air</t>
+  </si>
+  <si>
+    <t>Doc. No</t>
   </si>
 </sst>
 </file>
@@ -831,7 +834,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -956,6 +959,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -964,7 +982,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1032,6 +1050,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1111,6 +1135,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1141,7 +1168,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45349.476784375001" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Michael Wagner" refreshedDate="45701.617829050927" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1435,7 +1462,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="67">
     <pivotField showAll="0"/>
@@ -1873,75 +1900,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="38.875" customWidth="1"/>
-    <col min="5" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="8.875" customWidth="1"/>
-    <col min="8" max="8" width="15.375" customWidth="1"/>
-    <col min="9" max="9" width="13.875" style="11" customWidth="1"/>
-    <col min="10" max="11" width="11.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.83203125" customWidth="1"/>
+    <col min="5" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="11" customWidth="1"/>
+    <col min="10" max="11" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="10" customWidth="1"/>
-    <col min="13" max="13" width="10.875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="10.625" style="10" customWidth="1"/>
-    <col min="15" max="15" width="9.125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="13.625" style="15" customWidth="1"/>
-    <col min="17" max="18" width="11.625" style="10" customWidth="1"/>
-    <col min="19" max="19" width="13.625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="10.58203125" style="10" customWidth="1"/>
+    <col min="15" max="15" width="9.08203125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="13.58203125" style="15" customWidth="1"/>
+    <col min="17" max="18" width="11.58203125" style="10" customWidth="1"/>
+    <col min="19" max="19" width="13.58203125" style="10" customWidth="1"/>
     <col min="20" max="20" width="11" style="10"/>
-    <col min="21" max="21" width="10.875" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.125" style="10" customWidth="1"/>
-    <col min="23" max="23" width="11.625" style="11" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.08203125" style="10" customWidth="1"/>
+    <col min="23" max="23" width="11.58203125" style="11" customWidth="1"/>
     <col min="24" max="24" width="11" style="12"/>
     <col min="25" max="26" width="11" style="11"/>
-    <col min="27" max="27" width="21.125" style="11" customWidth="1"/>
+    <col min="27" max="27" width="21.08203125" style="11" customWidth="1"/>
     <col min="28" max="28" width="13" customWidth="1"/>
     <col min="29" max="29" width="13" style="10" customWidth="1"/>
-    <col min="30" max="30" width="18.625" style="10" customWidth="1"/>
+    <col min="30" max="30" width="18.58203125" style="10" customWidth="1"/>
     <col min="31" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="34" width="18.625" style="10" customWidth="1"/>
+    <col min="34" max="34" width="18.58203125" style="10" customWidth="1"/>
     <col min="35" max="35" width="13" style="16" customWidth="1"/>
     <col min="37" max="37" width="9.25" customWidth="1"/>
-    <col min="38" max="38" width="7.375" customWidth="1"/>
-    <col min="40" max="40" width="15.125" customWidth="1"/>
-    <col min="41" max="41" width="15.625" customWidth="1"/>
-    <col min="42" max="42" width="15.375" customWidth="1"/>
-    <col min="44" max="44" width="8.125" customWidth="1"/>
+    <col min="38" max="38" width="7.33203125" customWidth="1"/>
+    <col min="40" max="40" width="15.08203125" customWidth="1"/>
+    <col min="41" max="41" width="15.58203125" customWidth="1"/>
+    <col min="42" max="42" width="15.33203125" customWidth="1"/>
+    <col min="44" max="44" width="8.08203125" customWidth="1"/>
     <col min="45" max="47" width="11" style="13"/>
-    <col min="48" max="48" width="15.625" style="13" customWidth="1"/>
+    <col min="48" max="48" width="15.58203125" style="13" customWidth="1"/>
     <col min="49" max="49" width="11" style="13"/>
-    <col min="50" max="50" width="15.625" style="13" customWidth="1"/>
+    <col min="50" max="50" width="15.58203125" style="13" customWidth="1"/>
     <col min="51" max="52" width="11" style="13"/>
     <col min="61" max="61" width="14" customWidth="1"/>
-    <col min="62" max="62" width="12.375" customWidth="1"/>
-    <col min="63" max="63" width="11.875" customWidth="1"/>
-    <col min="64" max="64" width="10.875" customWidth="1"/>
+    <col min="62" max="62" width="12.33203125" customWidth="1"/>
+    <col min="63" max="63" width="11.83203125" customWidth="1"/>
+    <col min="64" max="64" width="10.83203125" customWidth="1"/>
     <col min="65" max="65" width="11.5" customWidth="1"/>
     <col min="66" max="67" width="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:67" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="5"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1998,7 +2025,7 @@
       <c r="BL1" s="5"/>
       <c r="BM1" s="5"/>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2042,13 +2069,13 @@
       <c r="AY2"/>
       <c r="AZ2"/>
     </row>
-    <row r="3" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2087,7 +2114,7 @@
       <c r="AY3"/>
       <c r="AZ3"/>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2133,87 +2160,87 @@
       <c r="AY4"/>
       <c r="AZ4"/>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
+    <row r="5" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="B5" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="40"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="53" t="s">
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="55"/>
+      <c r="Y5" s="56"/>
+      <c r="Z5" s="57"/>
       <c r="AA5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AB5" s="44" t="s">
+      <c r="AB5" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="45"/>
-      <c r="AD5" s="45"/>
-      <c r="AE5" s="46"/>
-      <c r="AF5" s="45"/>
-      <c r="AG5" s="45"/>
-      <c r="AH5" s="46"/>
-      <c r="AI5" s="47"/>
-      <c r="AJ5" s="51" t="s">
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="48"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="48"/>
+      <c r="AI5" s="49"/>
+      <c r="AJ5" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="AK5" s="52"/>
-      <c r="AL5" s="52"/>
-      <c r="AM5" s="52"/>
-      <c r="AN5" s="52"/>
-      <c r="AO5" s="52"/>
-      <c r="AP5" s="52"/>
-      <c r="AQ5" s="52"/>
-      <c r="AR5" s="52"/>
-      <c r="AS5" s="52"/>
-      <c r="AT5" s="52"/>
-      <c r="AU5" s="52"/>
-      <c r="AV5" s="42" t="s">
+      <c r="AK5" s="54"/>
+      <c r="AL5" s="54"/>
+      <c r="AM5" s="54"/>
+      <c r="AN5" s="54"/>
+      <c r="AO5" s="54"/>
+      <c r="AP5" s="54"/>
+      <c r="AQ5" s="54"/>
+      <c r="AR5" s="54"/>
+      <c r="AS5" s="54"/>
+      <c r="AT5" s="54"/>
+      <c r="AU5" s="54"/>
+      <c r="AV5" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="AW5" s="43"/>
-      <c r="AX5" s="43"/>
-      <c r="AY5" s="43"/>
+      <c r="AW5" s="45"/>
+      <c r="AX5" s="45"/>
+      <c r="AY5" s="45"/>
       <c r="AZ5" s="21"/>
-      <c r="BA5" s="36" t="s">
+      <c r="BA5" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="BB5" s="37"/>
-      <c r="BC5" s="37"/>
-      <c r="BD5" s="37"/>
-      <c r="BE5" s="37"/>
-      <c r="BF5" s="37"/>
-      <c r="BG5" s="37"/>
-      <c r="BH5" s="37"/>
-      <c r="BI5" s="37"/>
-      <c r="BJ5" s="37"/>
-      <c r="BK5" s="37"/>
-      <c r="BL5" s="37"/>
-      <c r="BM5" s="38"/>
-    </row>
-    <row r="6" spans="1:67" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="BB5" s="39"/>
+      <c r="BC5" s="39"/>
+      <c r="BD5" s="39"/>
+      <c r="BE5" s="39"/>
+      <c r="BF5" s="39"/>
+      <c r="BG5" s="39"/>
+      <c r="BH5" s="39"/>
+      <c r="BI5" s="39"/>
+      <c r="BJ5" s="39"/>
+      <c r="BK5" s="39"/>
+      <c r="BL5" s="39"/>
+      <c r="BM5" s="40"/>
+    </row>
+    <row r="6" spans="1:67" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2416,183 +2443,183 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" x14ac:dyDescent="0.35">
       <c r="AV8" s="17"/>
       <c r="AW8" s="17"/>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" x14ac:dyDescent="0.35">
       <c r="AV9" s="17"/>
       <c r="AW9" s="17"/>
     </row>
-    <row r="1048519" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048519" s="13"/>
     </row>
-    <row r="1048520" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048520" s="13"/>
     </row>
-    <row r="1048521" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048521" s="13"/>
     </row>
-    <row r="1048522" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048522" s="13"/>
     </row>
-    <row r="1048523" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048523" s="13"/>
     </row>
-    <row r="1048524" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048524" s="13"/>
     </row>
-    <row r="1048525" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048525" s="13"/>
     </row>
-    <row r="1048526" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048526" s="13"/>
     </row>
-    <row r="1048527" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048527" s="13"/>
     </row>
-    <row r="1048528" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048528" s="13"/>
     </row>
-    <row r="1048529" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048529" s="13"/>
     </row>
-    <row r="1048530" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048530" s="13"/>
     </row>
-    <row r="1048531" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048531" s="13"/>
     </row>
-    <row r="1048532" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048532" s="13"/>
     </row>
-    <row r="1048533" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048533" s="13"/>
     </row>
-    <row r="1048534" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048534" s="13"/>
     </row>
-    <row r="1048535" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048535" s="13"/>
     </row>
-    <row r="1048536" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048536" s="13"/>
     </row>
-    <row r="1048537" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048537" s="13"/>
     </row>
-    <row r="1048538" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048538" s="13"/>
     </row>
-    <row r="1048539" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048539" s="13"/>
     </row>
-    <row r="1048540" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048540" s="13"/>
     </row>
-    <row r="1048541" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048541" s="13"/>
     </row>
-    <row r="1048542" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048542" s="13"/>
     </row>
-    <row r="1048543" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048543" s="13"/>
     </row>
-    <row r="1048544" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048544" s="13"/>
     </row>
-    <row r="1048545" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048545" s="13"/>
     </row>
-    <row r="1048546" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048546" s="13"/>
     </row>
-    <row r="1048547" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048547" s="13"/>
     </row>
-    <row r="1048548" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048548" s="13"/>
     </row>
-    <row r="1048549" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048549" s="13"/>
     </row>
-    <row r="1048550" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048550" s="13"/>
     </row>
-    <row r="1048551" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048551" s="13"/>
     </row>
-    <row r="1048552" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048552" s="13"/>
     </row>
-    <row r="1048553" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048553" s="13"/>
     </row>
-    <row r="1048554" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048554" s="13"/>
     </row>
-    <row r="1048555" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048555" s="13"/>
     </row>
-    <row r="1048556" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048556" s="13"/>
     </row>
-    <row r="1048557" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048557" s="13"/>
     </row>
-    <row r="1048558" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048558" s="13"/>
     </row>
-    <row r="1048559" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048559" s="13"/>
     </row>
-    <row r="1048560" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048560" s="13"/>
     </row>
-    <row r="1048561" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048561" s="13"/>
     </row>
-    <row r="1048562" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048562" s="13"/>
     </row>
-    <row r="1048563" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048563" s="13"/>
     </row>
-    <row r="1048564" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048564" s="13"/>
     </row>
-    <row r="1048565" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048565" s="13"/>
     </row>
-    <row r="1048566" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048566" s="13"/>
     </row>
-    <row r="1048567" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048567" s="13"/>
     </row>
-    <row r="1048568" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048568" s="13"/>
     </row>
-    <row r="1048569" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048569" s="13"/>
     </row>
-    <row r="1048570" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048570" s="13"/>
     </row>
-    <row r="1048571" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048571" s="13"/>
     </row>
-    <row r="1048572" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048572" s="13"/>
     </row>
-    <row r="1048573" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048573" s="13"/>
     </row>
-    <row r="1048574" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048574" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048574" s="13"/>
     </row>
-    <row r="1048575" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048575" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048575" s="13"/>
     </row>
   </sheetData>
@@ -2625,36 +2652,36 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.875" style="15" customWidth="1"/>
-    <col min="6" max="7" width="14.625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="15" customWidth="1"/>
+    <col min="6" max="7" width="14.58203125" style="10" customWidth="1"/>
     <col min="9" max="9" width="9.25" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="13.75" customWidth="1"/>
-    <col min="12" max="12" width="15.625" customWidth="1"/>
-    <col min="13" max="13" width="14.125" customWidth="1"/>
+    <col min="12" max="12" width="15.58203125" customWidth="1"/>
+    <col min="13" max="13" width="14.08203125" customWidth="1"/>
     <col min="14" max="14" width="15.75" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
     <col min="17" max="17" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.5">
+      <c r="B1" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
@@ -2672,7 +2699,7 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2682,31 +2709,31 @@
       <c r="G2"/>
       <c r="Q2"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="B3" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="51" t="s">
+      <c r="C3" s="51"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="56"/>
-    </row>
-    <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="58"/>
+    </row>
+    <row r="4" spans="1:26" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -2765,175 +2792,175 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1048517" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048517" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048517" s="13"/>
     </row>
-    <row r="1048518" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048518" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048518" s="13"/>
     </row>
-    <row r="1048519" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048519" s="13"/>
     </row>
-    <row r="1048520" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048520" s="13"/>
     </row>
-    <row r="1048521" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048521" s="13"/>
     </row>
-    <row r="1048522" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048522" s="13"/>
     </row>
-    <row r="1048523" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048523" s="13"/>
     </row>
-    <row r="1048524" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048524" s="13"/>
     </row>
-    <row r="1048525" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048525" s="13"/>
     </row>
-    <row r="1048526" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048526" s="13"/>
     </row>
-    <row r="1048527" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048527" s="13"/>
     </row>
-    <row r="1048528" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048528" s="13"/>
     </row>
-    <row r="1048529" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048529" s="13"/>
     </row>
-    <row r="1048530" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048530" s="13"/>
     </row>
-    <row r="1048531" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048531" s="13"/>
     </row>
-    <row r="1048532" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048532" s="13"/>
     </row>
-    <row r="1048533" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048533" s="13"/>
     </row>
-    <row r="1048534" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048534" s="13"/>
     </row>
-    <row r="1048535" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048535" s="13"/>
     </row>
-    <row r="1048536" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048536" s="13"/>
     </row>
-    <row r="1048537" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048537" s="13"/>
     </row>
-    <row r="1048538" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048538" s="13"/>
     </row>
-    <row r="1048539" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048539" s="13"/>
     </row>
-    <row r="1048540" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048540" s="13"/>
     </row>
-    <row r="1048541" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048541" s="13"/>
     </row>
-    <row r="1048542" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048542" s="13"/>
     </row>
-    <row r="1048543" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048543" s="13"/>
     </row>
-    <row r="1048544" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048544" s="13"/>
     </row>
-    <row r="1048545" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048545" s="13"/>
     </row>
-    <row r="1048546" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048546" s="13"/>
     </row>
-    <row r="1048547" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048547" s="13"/>
     </row>
-    <row r="1048548" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048548" s="13"/>
     </row>
-    <row r="1048549" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048549" s="13"/>
     </row>
-    <row r="1048550" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048550" s="13"/>
     </row>
-    <row r="1048551" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048551" s="13"/>
     </row>
-    <row r="1048552" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048552" s="13"/>
     </row>
-    <row r="1048553" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048553" s="13"/>
     </row>
-    <row r="1048554" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048554" s="13"/>
     </row>
-    <row r="1048555" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048555" s="13"/>
     </row>
-    <row r="1048556" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048556" s="13"/>
     </row>
-    <row r="1048557" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048557" s="13"/>
     </row>
-    <row r="1048558" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048558" s="13"/>
     </row>
-    <row r="1048559" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048559" s="13"/>
     </row>
-    <row r="1048560" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048560" s="13"/>
     </row>
-    <row r="1048561" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048561" s="13"/>
     </row>
-    <row r="1048562" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048562" s="13"/>
     </row>
-    <row r="1048563" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048563" s="13"/>
     </row>
-    <row r="1048564" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048564" s="13"/>
     </row>
-    <row r="1048565" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048565" s="13"/>
     </row>
-    <row r="1048566" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048566" s="13"/>
     </row>
-    <row r="1048567" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048567" s="13"/>
     </row>
-    <row r="1048568" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048568" s="13"/>
     </row>
-    <row r="1048569" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048569" s="13"/>
     </row>
-    <row r="1048570" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048570" s="13"/>
     </row>
-    <row r="1048571" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048571" s="13"/>
     </row>
-    <row r="1048572" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048572" s="13"/>
     </row>
-    <row r="1048573" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048573" s="13"/>
     </row>
   </sheetData>
@@ -2951,125 +2978,129 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="3" width="11.625" customWidth="1"/>
-    <col min="6" max="6" width="26.625" customWidth="1"/>
-    <col min="7" max="7" width="11.875" customWidth="1"/>
-    <col min="9" max="9" width="15.625" customWidth="1"/>
-    <col min="10" max="10" width="13.75" customWidth="1"/>
-    <col min="11" max="13" width="15.625" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="16" max="16" width="11.625" customWidth="1"/>
-    <col min="18" max="18" width="11.625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="4" width="11.58203125" customWidth="1"/>
+    <col min="7" max="7" width="26.58203125" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="10" max="10" width="15.58203125" customWidth="1"/>
+    <col min="11" max="11" width="13.75" customWidth="1"/>
+    <col min="12" max="14" width="15.58203125" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="17" max="17" width="11.58203125" customWidth="1"/>
+    <col min="19" max="19" width="11.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C1" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B3" s="60"/>
+      <c r="C3" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51" t="s">
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="56"/>
-    </row>
-    <row r="4" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="58"/>
+    </row>
+    <row r="4" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="S4" s="20" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:R3"/>
+  <mergeCells count="3">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3084,18 +3115,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.58203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="B1" s="5" t="s">
         <v>80</v>
       </c>
@@ -3104,7 +3135,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>77</v>
       </c>
@@ -3127,7 +3158,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>78</v>
       </c>
@@ -3138,7 +3169,7 @@
       <c r="F4" s="12"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>78</v>
       </c>
@@ -3149,7 +3180,7 @@
       <c r="F5" s="12"/>
       <c r="G5" s="27"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Grab up to date template
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miwagne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9488BA9D-E96B-47B4-BFB0-0F23ACC4E4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDAF5A5-6627-4D03-A243-460CDF98EE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29955" yWindow="3090" windowWidth="26595" windowHeight="11775" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <sheet name="Neighborhood Breakout" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BO$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BP$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId5"/>
+    <pivotCache cacheId="5" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -333,6 +333,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="BN6" authorId="0" shapeId="0" xr:uid="{ACF72B43-181F-4EDF-AB31-F37EC8467982}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Flag indicating that the PIN has at least one assessable permit in the past 3 years. Only counts permits prior to January 1st of the current assessment year.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -410,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="95">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -689,6 +702,9 @@
   </si>
   <si>
     <t>Central Air</t>
+  </si>
+  <si>
+    <t>Recent Assessable Permit</t>
   </si>
   <si>
     <t>Doc. No</t>
@@ -1050,57 +1066,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1137,6 +1150,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1168,11 +1182,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Michael Wagner" refreshedDate="45701.617829050927" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Michael Wagner" refreshedDate="45701.701997916665" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
-  <cacheFields count="67">
+  <cacheFields count="68">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1370,6 +1384,9 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Critical Char. Missing" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Recent Assessable Permit" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total AV" numFmtId="0">
@@ -1457,14 +1474,15 @@
     <m/>
     <m/>
     <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="67">
+  <pivotFields count="68">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="2">
@@ -1500,6 +1518,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1583,10 +1602,10 @@
   </colItems>
   <dataFields count="6">
     <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
-    <dataField name="Min of Total AV" fld="65" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total AV" fld="65" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total AV" fld="65" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of AV Difference" fld="66" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min of Total AV" fld="66" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="66" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="66" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="67" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1898,13 +1917,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BO1048575"/>
+  <dimension ref="A1:BP1048575"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1955,10 +1974,12 @@
     <col min="63" max="63" width="11.83203125" customWidth="1"/>
     <col min="64" max="64" width="10.83203125" customWidth="1"/>
     <col min="65" max="65" width="11.5" customWidth="1"/>
-    <col min="66" max="67" width="11" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="13" customWidth="1"/>
+    <col min="67" max="67" width="7.75" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="9.33203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:68" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="5"/>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -2024,8 +2045,9 @@
       <c r="BK1" s="5"/>
       <c r="BL1" s="5"/>
       <c r="BM1" s="5"/>
-    </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BN1" s="5"/>
+    </row>
+    <row r="2" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2069,7 +2091,7 @@
       <c r="AY2"/>
       <c r="AZ2"/>
     </row>
-    <row r="3" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2114,7 +2136,7 @@
       <c r="AY3"/>
       <c r="AZ3"/>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2160,69 +2182,69 @@
       <c r="AY4"/>
       <c r="AZ4"/>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="B5" s="50" t="s">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="B5" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="52"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="35"/>
       <c r="K5" s="36"/>
       <c r="L5" s="36"/>
       <c r="M5" s="36"/>
       <c r="N5" s="36"/>
       <c r="O5" s="37"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="42"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="55" t="s">
+      <c r="P5" s="40"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="42"/>
+      <c r="X5" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="Y5" s="56"/>
-      <c r="Z5" s="57"/>
+      <c r="Y5" s="55"/>
+      <c r="Z5" s="56"/>
       <c r="AA5" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AB5" s="46" t="s">
+      <c r="AB5" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="47"/>
-      <c r="AD5" s="47"/>
-      <c r="AE5" s="48"/>
-      <c r="AF5" s="47"/>
-      <c r="AG5" s="47"/>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="49"/>
-      <c r="AJ5" s="53" t="s">
+      <c r="AC5" s="46"/>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="46"/>
+      <c r="AG5" s="46"/>
+      <c r="AH5" s="47"/>
+      <c r="AI5" s="48"/>
+      <c r="AJ5" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="AK5" s="54"/>
-      <c r="AL5" s="54"/>
-      <c r="AM5" s="54"/>
-      <c r="AN5" s="54"/>
-      <c r="AO5" s="54"/>
-      <c r="AP5" s="54"/>
-      <c r="AQ5" s="54"/>
-      <c r="AR5" s="54"/>
-      <c r="AS5" s="54"/>
-      <c r="AT5" s="54"/>
-      <c r="AU5" s="54"/>
-      <c r="AV5" s="44" t="s">
+      <c r="AK5" s="53"/>
+      <c r="AL5" s="53"/>
+      <c r="AM5" s="53"/>
+      <c r="AN5" s="53"/>
+      <c r="AO5" s="53"/>
+      <c r="AP5" s="53"/>
+      <c r="AQ5" s="53"/>
+      <c r="AR5" s="53"/>
+      <c r="AS5" s="53"/>
+      <c r="AT5" s="53"/>
+      <c r="AU5" s="53"/>
+      <c r="AV5" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="AW5" s="45"/>
-      <c r="AX5" s="45"/>
-      <c r="AY5" s="45"/>
+      <c r="AW5" s="44"/>
+      <c r="AX5" s="44"/>
+      <c r="AY5" s="44"/>
       <c r="AZ5" s="21"/>
       <c r="BA5" s="38" t="s">
         <v>2</v>
@@ -2238,9 +2260,10 @@
       <c r="BJ5" s="39"/>
       <c r="BK5" s="39"/>
       <c r="BL5" s="39"/>
-      <c r="BM5" s="40"/>
-    </row>
-    <row r="6" spans="1:67" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="BM5" s="39"/>
+      <c r="BN5" s="31"/>
+    </row>
+    <row r="6" spans="1:68" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2433,21 +2456,24 @@
       <c r="BL6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BM6" s="14" t="s">
+      <c r="BM6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="BN6" s="2" t="s">
+      <c r="BN6" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="BO6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="BO6" s="4" t="s">
+      <c r="BP6" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.35">
       <c r="AV8" s="17"/>
       <c r="AW8" s="17"/>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.35">
       <c r="AV9" s="17"/>
       <c r="AW9" s="17"/>
     </row>
@@ -2710,28 +2736,28 @@
       <c r="Q2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="53" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="58"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="57"/>
     </row>
     <row r="4" spans="1:26" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
@@ -2984,13 +3010,12 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="1" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="4" width="11.58203125" customWidth="1"/>
     <col min="7" max="7" width="26.58203125" customWidth="1"/>
     <col min="8" max="8" width="11.83203125" customWidth="1"/>
@@ -3013,36 +3038,36 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B3" s="60"/>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="50" t="s">
+      <c r="D3" s="59"/>
+      <c r="E3" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="53" t="s">
+      <c r="F3" s="50"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="58"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="57"/>
     </row>
     <row r="4" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Update template and doc_no linking
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miwagne\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDAF5A5-6627-4D03-A243-460CDF98EE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C332071-65F2-4E46-A8C4-44A2DF842DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -113,7 +113,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
+          <t>This column shows the sale that the model thinks is most comparable to the target parcel. Click the link to navigate to the corresponding row in the Comparables tab of this sheet.</t>
         </r>
       </text>
     </comment>
@@ -545,15 +545,9 @@
     <t>Overall Comp. Score</t>
   </si>
   <si>
-    <t>Comp. 1 PIN</t>
-  </si>
-  <si>
     <t>Comp. 1 Score</t>
   </si>
   <si>
-    <t>Comp. 2 PIN</t>
-  </si>
-  <si>
     <t>Comp. 2 Score</t>
   </si>
   <si>
@@ -708,6 +702,12 @@
   </si>
   <si>
     <t>Doc. No</t>
+  </si>
+  <si>
+    <t>Comp. 1 Sale</t>
+  </si>
+  <si>
+    <t>Comp. 2 Sale</t>
   </si>
 </sst>
 </file>
@@ -1072,6 +1072,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1148,10 +1152,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1182,7 +1182,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Michael Wagner" refreshedDate="45701.701997916665" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45708.629130439818" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1332,13 +1332,13 @@
     <cacheField name="# Comm. Units" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Comp. 1 PIN" numFmtId="37">
+    <cacheField name="Comp. 1 Sale" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Comp. 1 Score" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Comp. 2 PIN" numFmtId="37">
+    <cacheField name="Comp. 2 Sale" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Comp. 2 Score" numFmtId="37">
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="68">
     <pivotField showAll="0"/>
@@ -1919,77 +1919,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BP1048575"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="38.83203125" customWidth="1"/>
-    <col min="5" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" style="11" customWidth="1"/>
-    <col min="10" max="11" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.875" customWidth="1"/>
+    <col min="5" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="8.875" customWidth="1"/>
+    <col min="8" max="8" width="15.375" customWidth="1"/>
+    <col min="9" max="9" width="13.875" style="11" customWidth="1"/>
+    <col min="10" max="11" width="11.875" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="10" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="10.58203125" style="10" customWidth="1"/>
-    <col min="15" max="15" width="9.08203125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="13.58203125" style="15" customWidth="1"/>
-    <col min="17" max="18" width="11.58203125" style="10" customWidth="1"/>
-    <col min="19" max="19" width="13.58203125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="10.875" style="10" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="9.125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="13.625" style="15" customWidth="1"/>
+    <col min="17" max="18" width="11.625" style="10" customWidth="1"/>
+    <col min="19" max="19" width="13.625" style="10" customWidth="1"/>
     <col min="20" max="20" width="11" style="10"/>
-    <col min="21" max="21" width="10.83203125" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.08203125" style="10" customWidth="1"/>
-    <col min="23" max="23" width="11.58203125" style="11" customWidth="1"/>
+    <col min="21" max="21" width="10.875" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.125" style="10" customWidth="1"/>
+    <col min="23" max="23" width="11.625" style="11" customWidth="1"/>
     <col min="24" max="24" width="11" style="12"/>
     <col min="25" max="26" width="11" style="11"/>
-    <col min="27" max="27" width="21.08203125" style="11" customWidth="1"/>
+    <col min="27" max="27" width="21.125" style="11" customWidth="1"/>
     <col min="28" max="28" width="13" customWidth="1"/>
     <col min="29" max="29" width="13" style="10" customWidth="1"/>
-    <col min="30" max="30" width="18.58203125" style="10" customWidth="1"/>
+    <col min="30" max="30" width="18.625" style="10" customWidth="1"/>
     <col min="31" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="34" width="18.58203125" style="10" customWidth="1"/>
+    <col min="34" max="34" width="18.625" style="10" customWidth="1"/>
     <col min="35" max="35" width="13" style="16" customWidth="1"/>
     <col min="37" max="37" width="9.25" customWidth="1"/>
-    <col min="38" max="38" width="7.33203125" customWidth="1"/>
-    <col min="40" max="40" width="15.08203125" customWidth="1"/>
-    <col min="41" max="41" width="15.58203125" customWidth="1"/>
-    <col min="42" max="42" width="15.33203125" customWidth="1"/>
-    <col min="44" max="44" width="8.08203125" customWidth="1"/>
+    <col min="38" max="38" width="7.375" customWidth="1"/>
+    <col min="40" max="40" width="15.125" customWidth="1"/>
+    <col min="41" max="41" width="15.625" customWidth="1"/>
+    <col min="42" max="42" width="15.375" customWidth="1"/>
+    <col min="44" max="44" width="8.125" customWidth="1"/>
     <col min="45" max="47" width="11" style="13"/>
-    <col min="48" max="48" width="15.58203125" style="13" customWidth="1"/>
+    <col min="48" max="48" width="11" style="13" customWidth="1"/>
     <col min="49" max="49" width="11" style="13"/>
-    <col min="50" max="50" width="15.58203125" style="13" customWidth="1"/>
+    <col min="50" max="50" width="11" style="13" customWidth="1"/>
     <col min="51" max="52" width="11" style="13"/>
     <col min="61" max="61" width="14" customWidth="1"/>
-    <col min="62" max="62" width="12.33203125" customWidth="1"/>
-    <col min="63" max="63" width="11.83203125" customWidth="1"/>
-    <col min="64" max="64" width="10.83203125" customWidth="1"/>
+    <col min="62" max="62" width="12.375" customWidth="1"/>
+    <col min="63" max="63" width="11.875" customWidth="1"/>
+    <col min="64" max="64" width="10.875" customWidth="1"/>
     <col min="65" max="65" width="11.5" customWidth="1"/>
     <col min="66" max="66" width="13" customWidth="1"/>
     <col min="67" max="67" width="7.75" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="9.33203125" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="9.375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:68" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -2047,7 +2047,7 @@
       <c r="BM1" s="5"/>
       <c r="BN1" s="5"/>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2091,13 +2091,13 @@
       <c r="AY2"/>
       <c r="AZ2"/>
     </row>
-    <row r="3" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2136,7 +2136,7 @@
       <c r="AY3"/>
       <c r="AZ3"/>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2182,88 +2182,88 @@
       <c r="AY4"/>
       <c r="AZ4"/>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="B5" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="42"/>
-      <c r="X5" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y5" s="55"/>
-      <c r="Z5" s="56"/>
+    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="B5" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="44"/>
+      <c r="X5" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y5" s="57"/>
+      <c r="Z5" s="58"/>
       <c r="AA5" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB5" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="46"/>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="47"/>
-      <c r="AF5" s="46"/>
-      <c r="AG5" s="46"/>
-      <c r="AH5" s="47"/>
-      <c r="AI5" s="48"/>
-      <c r="AJ5" s="52" t="s">
+      <c r="AB5" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="48"/>
+      <c r="AG5" s="48"/>
+      <c r="AH5" s="49"/>
+      <c r="AI5" s="50"/>
+      <c r="AJ5" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="AK5" s="53"/>
-      <c r="AL5" s="53"/>
-      <c r="AM5" s="53"/>
-      <c r="AN5" s="53"/>
-      <c r="AO5" s="53"/>
-      <c r="AP5" s="53"/>
-      <c r="AQ5" s="53"/>
-      <c r="AR5" s="53"/>
-      <c r="AS5" s="53"/>
-      <c r="AT5" s="53"/>
-      <c r="AU5" s="53"/>
-      <c r="AV5" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW5" s="44"/>
-      <c r="AX5" s="44"/>
-      <c r="AY5" s="44"/>
+      <c r="AK5" s="55"/>
+      <c r="AL5" s="55"/>
+      <c r="AM5" s="55"/>
+      <c r="AN5" s="55"/>
+      <c r="AO5" s="55"/>
+      <c r="AP5" s="55"/>
+      <c r="AQ5" s="55"/>
+      <c r="AR5" s="55"/>
+      <c r="AS5" s="55"/>
+      <c r="AT5" s="55"/>
+      <c r="AU5" s="55"/>
+      <c r="AV5" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW5" s="46"/>
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="46"/>
       <c r="AZ5" s="21"/>
-      <c r="BA5" s="38" t="s">
+      <c r="BA5" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="BB5" s="39"/>
-      <c r="BC5" s="39"/>
-      <c r="BD5" s="39"/>
-      <c r="BE5" s="39"/>
-      <c r="BF5" s="39"/>
-      <c r="BG5" s="39"/>
-      <c r="BH5" s="39"/>
-      <c r="BI5" s="39"/>
-      <c r="BJ5" s="39"/>
-      <c r="BK5" s="39"/>
-      <c r="BL5" s="39"/>
-      <c r="BM5" s="39"/>
+      <c r="BB5" s="41"/>
+      <c r="BC5" s="41"/>
+      <c r="BD5" s="41"/>
+      <c r="BE5" s="41"/>
+      <c r="BF5" s="41"/>
+      <c r="BG5" s="41"/>
+      <c r="BH5" s="41"/>
+      <c r="BI5" s="41"/>
+      <c r="BJ5" s="41"/>
+      <c r="BK5" s="41"/>
+      <c r="BL5" s="41"/>
+      <c r="BM5" s="41"/>
       <c r="BN5" s="31"/>
     </row>
-    <row r="6" spans="1:68" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:68" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2340,10 +2340,10 @@
         <v>24</v>
       </c>
       <c r="Z6" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AB6" s="2" t="s">
         <v>25</v>
@@ -2373,22 +2373,22 @@
         <v>33</v>
       </c>
       <c r="AK6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP6" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="AL6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="AO6" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="AP6" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="AQ6" s="6" t="s">
         <v>34</v>
@@ -2406,246 +2406,246 @@
         <v>38</v>
       </c>
       <c r="AV6" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AW6" s="14" t="s">
+      <c r="AX6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AY6" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="AX6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AY6" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="AZ6" s="14" t="s">
         <v>39</v>
       </c>
       <c r="BA6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="BC6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="BD6" s="9" t="s">
+      <c r="BF6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="BE6" s="9" t="s">
+      <c r="BG6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="BF6" s="9" t="s">
+      <c r="BH6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="BG6" s="9" t="s">
+      <c r="BI6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="BH6" s="9" t="s">
+      <c r="BJ6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="BI6" s="9" t="s">
+      <c r="BK6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="BJ6" s="9" t="s">
+      <c r="BL6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BK6" s="9" t="s">
+      <c r="BM6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="BL6" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="BM6" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="BN6" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="BO6" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="BP6" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
       <c r="AV8" s="17"/>
       <c r="AW8" s="17"/>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
       <c r="AV9" s="17"/>
       <c r="AW9" s="17"/>
     </row>
-    <row r="1048519" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048519" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048519" s="13"/>
     </row>
-    <row r="1048520" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048520" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048520" s="13"/>
     </row>
-    <row r="1048521" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048521" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048521" s="13"/>
     </row>
-    <row r="1048522" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048522" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048522" s="13"/>
     </row>
-    <row r="1048523" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048523" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048523" s="13"/>
     </row>
-    <row r="1048524" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048524" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048524" s="13"/>
     </row>
-    <row r="1048525" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048525" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048525" s="13"/>
     </row>
-    <row r="1048526" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048526" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048526" s="13"/>
     </row>
-    <row r="1048527" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048527" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048527" s="13"/>
     </row>
-    <row r="1048528" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048528" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048528" s="13"/>
     </row>
-    <row r="1048529" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048529" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048529" s="13"/>
     </row>
-    <row r="1048530" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048530" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048530" s="13"/>
     </row>
-    <row r="1048531" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048531" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048531" s="13"/>
     </row>
-    <row r="1048532" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048532" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048532" s="13"/>
     </row>
-    <row r="1048533" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048533" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048533" s="13"/>
     </row>
-    <row r="1048534" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048534" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048534" s="13"/>
     </row>
-    <row r="1048535" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048535" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048535" s="13"/>
     </row>
-    <row r="1048536" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048536" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048536" s="13"/>
     </row>
-    <row r="1048537" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048537" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048537" s="13"/>
     </row>
-    <row r="1048538" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048538" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048538" s="13"/>
     </row>
-    <row r="1048539" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048539" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048539" s="13"/>
     </row>
-    <row r="1048540" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048540" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048540" s="13"/>
     </row>
-    <row r="1048541" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048541" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048541" s="13"/>
     </row>
-    <row r="1048542" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048542" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048542" s="13"/>
     </row>
-    <row r="1048543" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048543" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048543" s="13"/>
     </row>
-    <row r="1048544" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048544" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048544" s="13"/>
     </row>
-    <row r="1048545" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048545" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048545" s="13"/>
     </row>
-    <row r="1048546" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048546" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048546" s="13"/>
     </row>
-    <row r="1048547" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048547" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048547" s="13"/>
     </row>
-    <row r="1048548" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048548" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048548" s="13"/>
     </row>
-    <row r="1048549" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048549" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048549" s="13"/>
     </row>
-    <row r="1048550" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048550" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048550" s="13"/>
     </row>
-    <row r="1048551" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048551" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048551" s="13"/>
     </row>
-    <row r="1048552" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048552" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048552" s="13"/>
     </row>
-    <row r="1048553" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048553" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048553" s="13"/>
     </row>
-    <row r="1048554" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048554" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048554" s="13"/>
     </row>
-    <row r="1048555" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048555" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048555" s="13"/>
     </row>
-    <row r="1048556" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048556" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048556" s="13"/>
     </row>
-    <row r="1048557" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048557" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048557" s="13"/>
     </row>
-    <row r="1048558" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048558" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048558" s="13"/>
     </row>
-    <row r="1048559" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048559" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048559" s="13"/>
     </row>
-    <row r="1048560" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048560" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048560" s="13"/>
     </row>
-    <row r="1048561" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048561" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048561" s="13"/>
     </row>
-    <row r="1048562" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048562" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048562" s="13"/>
     </row>
-    <row r="1048563" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048563" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048563" s="13"/>
     </row>
-    <row r="1048564" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048564" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048564" s="13"/>
     </row>
-    <row r="1048565" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048565" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048565" s="13"/>
     </row>
-    <row r="1048566" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048566" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048566" s="13"/>
     </row>
-    <row r="1048567" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048567" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048567" s="13"/>
     </row>
-    <row r="1048568" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048568" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048568" s="13"/>
     </row>
-    <row r="1048569" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048569" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048569" s="13"/>
     </row>
-    <row r="1048570" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048570" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048570" s="13"/>
     </row>
-    <row r="1048571" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048571" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048571" s="13"/>
     </row>
-    <row r="1048572" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048572" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048572" s="13"/>
     </row>
-    <row r="1048573" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048573" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048573" s="13"/>
     </row>
-    <row r="1048574" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048574" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048574" s="13"/>
     </row>
-    <row r="1048575" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048575" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048575" s="13"/>
     </row>
   </sheetData>
@@ -2675,39 +2675,39 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="15" customWidth="1"/>
-    <col min="6" max="7" width="14.58203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.875" style="15" customWidth="1"/>
+    <col min="6" max="7" width="14.625" style="10" customWidth="1"/>
     <col min="9" max="9" width="9.25" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="13.75" customWidth="1"/>
-    <col min="12" max="12" width="15.58203125" customWidth="1"/>
-    <col min="13" max="13" width="14.08203125" customWidth="1"/>
+    <col min="12" max="12" width="15.625" customWidth="1"/>
+    <col min="13" max="13" width="14.125" customWidth="1"/>
     <col min="14" max="14" width="15.75" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
     <col min="17" max="17" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.5">
-      <c r="B1" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
@@ -2725,7 +2725,7 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2735,36 +2735,36 @@
       <c r="G2"/>
       <c r="Q2"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B3" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="57"/>
-    </row>
-    <row r="4" spans="1:26" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B3" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="59"/>
+    </row>
+    <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>4</v>
@@ -2773,37 +2773,37 @@
         <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>33</v>
       </c>
       <c r="I4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>35</v>
@@ -2818,175 +2818,175 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1048517" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048517" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048517" s="13"/>
     </row>
-    <row r="1048518" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048518" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048518" s="13"/>
     </row>
-    <row r="1048519" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048519" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048519" s="13"/>
     </row>
-    <row r="1048520" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048520" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048520" s="13"/>
     </row>
-    <row r="1048521" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048521" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048521" s="13"/>
     </row>
-    <row r="1048522" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048522" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048522" s="13"/>
     </row>
-    <row r="1048523" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048523" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048523" s="13"/>
     </row>
-    <row r="1048524" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048524" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048524" s="13"/>
     </row>
-    <row r="1048525" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048525" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048525" s="13"/>
     </row>
-    <row r="1048526" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048526" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048526" s="13"/>
     </row>
-    <row r="1048527" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048527" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048527" s="13"/>
     </row>
-    <row r="1048528" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048528" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048528" s="13"/>
     </row>
-    <row r="1048529" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048529" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048529" s="13"/>
     </row>
-    <row r="1048530" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048530" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048530" s="13"/>
     </row>
-    <row r="1048531" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048531" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048531" s="13"/>
     </row>
-    <row r="1048532" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048532" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048532" s="13"/>
     </row>
-    <row r="1048533" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048533" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048533" s="13"/>
     </row>
-    <row r="1048534" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048534" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048534" s="13"/>
     </row>
-    <row r="1048535" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048535" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048535" s="13"/>
     </row>
-    <row r="1048536" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048536" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048536" s="13"/>
     </row>
-    <row r="1048537" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048537" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048537" s="13"/>
     </row>
-    <row r="1048538" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048538" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048538" s="13"/>
     </row>
-    <row r="1048539" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048539" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048539" s="13"/>
     </row>
-    <row r="1048540" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048540" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048540" s="13"/>
     </row>
-    <row r="1048541" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048541" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048541" s="13"/>
     </row>
-    <row r="1048542" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048542" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048542" s="13"/>
     </row>
-    <row r="1048543" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048543" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048543" s="13"/>
     </row>
-    <row r="1048544" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048544" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048544" s="13"/>
     </row>
-    <row r="1048545" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048545" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048545" s="13"/>
     </row>
-    <row r="1048546" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048546" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048546" s="13"/>
     </row>
-    <row r="1048547" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048547" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048547" s="13"/>
     </row>
-    <row r="1048548" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048548" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048548" s="13"/>
     </row>
-    <row r="1048549" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048549" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048549" s="13"/>
     </row>
-    <row r="1048550" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048550" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048550" s="13"/>
     </row>
-    <row r="1048551" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048551" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048551" s="13"/>
     </row>
-    <row r="1048552" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048552" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048552" s="13"/>
     </row>
-    <row r="1048553" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048553" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048553" s="13"/>
     </row>
-    <row r="1048554" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048554" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048554" s="13"/>
     </row>
-    <row r="1048555" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048555" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048555" s="13"/>
     </row>
-    <row r="1048556" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048556" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048556" s="13"/>
     </row>
-    <row r="1048557" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048557" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048557" s="13"/>
     </row>
-    <row r="1048558" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048558" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048558" s="13"/>
     </row>
-    <row r="1048559" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048559" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048559" s="13"/>
     </row>
-    <row r="1048560" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048560" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048560" s="13"/>
     </row>
-    <row r="1048561" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048561" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048561" s="13"/>
     </row>
-    <row r="1048562" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048562" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048562" s="13"/>
     </row>
-    <row r="1048563" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048563" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048563" s="13"/>
     </row>
-    <row r="1048564" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048564" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048564" s="13"/>
     </row>
-    <row r="1048565" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048565" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048565" s="13"/>
     </row>
-    <row r="1048566" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048566" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048566" s="13"/>
     </row>
-    <row r="1048567" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048567" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048567" s="13"/>
     </row>
-    <row r="1048568" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048568" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048568" s="13"/>
     </row>
-    <row r="1048569" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048569" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048569" s="13"/>
     </row>
-    <row r="1048570" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048570" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048570" s="13"/>
     </row>
-    <row r="1048571" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048571" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048571" s="13"/>
     </row>
-    <row r="1048572" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048572" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048572" s="13"/>
     </row>
-    <row r="1048573" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048573" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048573" s="13"/>
     </row>
   </sheetData>
@@ -3006,74 +3006,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="4" width="11.58203125" customWidth="1"/>
-    <col min="7" max="7" width="26.58203125" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
-    <col min="10" max="10" width="15.58203125" customWidth="1"/>
+    <col min="1" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="4" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="26.625" customWidth="1"/>
+    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
     <col min="11" max="11" width="13.75" customWidth="1"/>
-    <col min="12" max="14" width="15.58203125" customWidth="1"/>
+    <col min="12" max="14" width="15.625" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="17" max="17" width="11.58203125" customWidth="1"/>
-    <col min="19" max="19" width="11.58203125" customWidth="1"/>
+    <col min="17" max="17" width="11.625" customWidth="1"/>
+    <col min="19" max="19" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="60"/>
+    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="34"/>
       <c r="C3" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="57"/>
-    </row>
-    <row r="4" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="59"/>
+    </row>
+    <row r="4" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>4</v>
@@ -3088,25 +3088,25 @@
         <v>33</v>
       </c>
       <c r="I4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>35</v>
@@ -3140,52 +3140,52 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.08203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.58203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>85</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>86</v>
       </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="12"/>
@@ -3194,9 +3194,9 @@
       <c r="F4" s="12"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="12"/>
@@ -3205,9 +3205,9 @@
       <c r="F5" s="12"/>
       <c r="G5" s="27"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="12"/>

</xml_diff>

<commit_message>
Update template and doc number linking PR (#354)
* Update template and doc_no linking

* Revert township code source

* Remove unnecessary ungroup
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miwagne\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDAF5A5-6627-4D03-A243-460CDF98EE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C332071-65F2-4E46-A8C4-44A2DF842DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -113,7 +113,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
+          <t>This column shows the sale that the model thinks is most comparable to the target parcel. Click the link to navigate to the corresponding row in the Comparables tab of this sheet.</t>
         </r>
       </text>
     </comment>
@@ -545,15 +545,9 @@
     <t>Overall Comp. Score</t>
   </si>
   <si>
-    <t>Comp. 1 PIN</t>
-  </si>
-  <si>
     <t>Comp. 1 Score</t>
   </si>
   <si>
-    <t>Comp. 2 PIN</t>
-  </si>
-  <si>
     <t>Comp. 2 Score</t>
   </si>
   <si>
@@ -708,6 +702,12 @@
   </si>
   <si>
     <t>Doc. No</t>
+  </si>
+  <si>
+    <t>Comp. 1 Sale</t>
+  </si>
+  <si>
+    <t>Comp. 2 Sale</t>
   </si>
 </sst>
 </file>
@@ -1072,6 +1072,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1148,10 +1152,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1182,7 +1182,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Michael Wagner" refreshedDate="45701.701997916665" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45708.629130439818" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1332,13 +1332,13 @@
     <cacheField name="# Comm. Units" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Comp. 1 PIN" numFmtId="37">
+    <cacheField name="Comp. 1 Sale" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Comp. 1 Score" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Comp. 2 PIN" numFmtId="37">
+    <cacheField name="Comp. 2 Sale" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Comp. 2 Score" numFmtId="37">
@@ -1480,7 +1480,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="68">
     <pivotField showAll="0"/>
@@ -1919,77 +1919,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BP1048575"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="38.83203125" customWidth="1"/>
-    <col min="5" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" style="11" customWidth="1"/>
-    <col min="10" max="11" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.875" customWidth="1"/>
+    <col min="5" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="8.875" customWidth="1"/>
+    <col min="8" max="8" width="15.375" customWidth="1"/>
+    <col min="9" max="9" width="13.875" style="11" customWidth="1"/>
+    <col min="10" max="11" width="11.875" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="10" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="10.58203125" style="10" customWidth="1"/>
-    <col min="15" max="15" width="9.08203125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="13.58203125" style="15" customWidth="1"/>
-    <col min="17" max="18" width="11.58203125" style="10" customWidth="1"/>
-    <col min="19" max="19" width="13.58203125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="10.875" style="10" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="9.125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="13.625" style="15" customWidth="1"/>
+    <col min="17" max="18" width="11.625" style="10" customWidth="1"/>
+    <col min="19" max="19" width="13.625" style="10" customWidth="1"/>
     <col min="20" max="20" width="11" style="10"/>
-    <col min="21" max="21" width="10.83203125" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.08203125" style="10" customWidth="1"/>
-    <col min="23" max="23" width="11.58203125" style="11" customWidth="1"/>
+    <col min="21" max="21" width="10.875" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.125" style="10" customWidth="1"/>
+    <col min="23" max="23" width="11.625" style="11" customWidth="1"/>
     <col min="24" max="24" width="11" style="12"/>
     <col min="25" max="26" width="11" style="11"/>
-    <col min="27" max="27" width="21.08203125" style="11" customWidth="1"/>
+    <col min="27" max="27" width="21.125" style="11" customWidth="1"/>
     <col min="28" max="28" width="13" customWidth="1"/>
     <col min="29" max="29" width="13" style="10" customWidth="1"/>
-    <col min="30" max="30" width="18.58203125" style="10" customWidth="1"/>
+    <col min="30" max="30" width="18.625" style="10" customWidth="1"/>
     <col min="31" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="34" width="18.58203125" style="10" customWidth="1"/>
+    <col min="34" max="34" width="18.625" style="10" customWidth="1"/>
     <col min="35" max="35" width="13" style="16" customWidth="1"/>
     <col min="37" max="37" width="9.25" customWidth="1"/>
-    <col min="38" max="38" width="7.33203125" customWidth="1"/>
-    <col min="40" max="40" width="15.08203125" customWidth="1"/>
-    <col min="41" max="41" width="15.58203125" customWidth="1"/>
-    <col min="42" max="42" width="15.33203125" customWidth="1"/>
-    <col min="44" max="44" width="8.08203125" customWidth="1"/>
+    <col min="38" max="38" width="7.375" customWidth="1"/>
+    <col min="40" max="40" width="15.125" customWidth="1"/>
+    <col min="41" max="41" width="15.625" customWidth="1"/>
+    <col min="42" max="42" width="15.375" customWidth="1"/>
+    <col min="44" max="44" width="8.125" customWidth="1"/>
     <col min="45" max="47" width="11" style="13"/>
-    <col min="48" max="48" width="15.58203125" style="13" customWidth="1"/>
+    <col min="48" max="48" width="11" style="13" customWidth="1"/>
     <col min="49" max="49" width="11" style="13"/>
-    <col min="50" max="50" width="15.58203125" style="13" customWidth="1"/>
+    <col min="50" max="50" width="11" style="13" customWidth="1"/>
     <col min="51" max="52" width="11" style="13"/>
     <col min="61" max="61" width="14" customWidth="1"/>
-    <col min="62" max="62" width="12.33203125" customWidth="1"/>
-    <col min="63" max="63" width="11.83203125" customWidth="1"/>
-    <col min="64" max="64" width="10.83203125" customWidth="1"/>
+    <col min="62" max="62" width="12.375" customWidth="1"/>
+    <col min="63" max="63" width="11.875" customWidth="1"/>
+    <col min="64" max="64" width="10.875" customWidth="1"/>
     <col min="65" max="65" width="11.5" customWidth="1"/>
     <col min="66" max="66" width="13" customWidth="1"/>
     <col min="67" max="67" width="7.75" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="9.33203125" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="9.375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:68" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -2047,7 +2047,7 @@
       <c r="BM1" s="5"/>
       <c r="BN1" s="5"/>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2091,13 +2091,13 @@
       <c r="AY2"/>
       <c r="AZ2"/>
     </row>
-    <row r="3" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2136,7 +2136,7 @@
       <c r="AY3"/>
       <c r="AZ3"/>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2182,88 +2182,88 @@
       <c r="AY4"/>
       <c r="AZ4"/>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="B5" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="42"/>
-      <c r="X5" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y5" s="55"/>
-      <c r="Z5" s="56"/>
+    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="B5" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="44"/>
+      <c r="X5" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y5" s="57"/>
+      <c r="Z5" s="58"/>
       <c r="AA5" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB5" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="46"/>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="47"/>
-      <c r="AF5" s="46"/>
-      <c r="AG5" s="46"/>
-      <c r="AH5" s="47"/>
-      <c r="AI5" s="48"/>
-      <c r="AJ5" s="52" t="s">
+      <c r="AB5" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="48"/>
+      <c r="AG5" s="48"/>
+      <c r="AH5" s="49"/>
+      <c r="AI5" s="50"/>
+      <c r="AJ5" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="AK5" s="53"/>
-      <c r="AL5" s="53"/>
-      <c r="AM5" s="53"/>
-      <c r="AN5" s="53"/>
-      <c r="AO5" s="53"/>
-      <c r="AP5" s="53"/>
-      <c r="AQ5" s="53"/>
-      <c r="AR5" s="53"/>
-      <c r="AS5" s="53"/>
-      <c r="AT5" s="53"/>
-      <c r="AU5" s="53"/>
-      <c r="AV5" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW5" s="44"/>
-      <c r="AX5" s="44"/>
-      <c r="AY5" s="44"/>
+      <c r="AK5" s="55"/>
+      <c r="AL5" s="55"/>
+      <c r="AM5" s="55"/>
+      <c r="AN5" s="55"/>
+      <c r="AO5" s="55"/>
+      <c r="AP5" s="55"/>
+      <c r="AQ5" s="55"/>
+      <c r="AR5" s="55"/>
+      <c r="AS5" s="55"/>
+      <c r="AT5" s="55"/>
+      <c r="AU5" s="55"/>
+      <c r="AV5" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW5" s="46"/>
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="46"/>
       <c r="AZ5" s="21"/>
-      <c r="BA5" s="38" t="s">
+      <c r="BA5" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="BB5" s="39"/>
-      <c r="BC5" s="39"/>
-      <c r="BD5" s="39"/>
-      <c r="BE5" s="39"/>
-      <c r="BF5" s="39"/>
-      <c r="BG5" s="39"/>
-      <c r="BH5" s="39"/>
-      <c r="BI5" s="39"/>
-      <c r="BJ5" s="39"/>
-      <c r="BK5" s="39"/>
-      <c r="BL5" s="39"/>
-      <c r="BM5" s="39"/>
+      <c r="BB5" s="41"/>
+      <c r="BC5" s="41"/>
+      <c r="BD5" s="41"/>
+      <c r="BE5" s="41"/>
+      <c r="BF5" s="41"/>
+      <c r="BG5" s="41"/>
+      <c r="BH5" s="41"/>
+      <c r="BI5" s="41"/>
+      <c r="BJ5" s="41"/>
+      <c r="BK5" s="41"/>
+      <c r="BL5" s="41"/>
+      <c r="BM5" s="41"/>
       <c r="BN5" s="31"/>
     </row>
-    <row r="6" spans="1:68" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:68" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2340,10 +2340,10 @@
         <v>24</v>
       </c>
       <c r="Z6" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AB6" s="2" t="s">
         <v>25</v>
@@ -2373,22 +2373,22 @@
         <v>33</v>
       </c>
       <c r="AK6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP6" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="AL6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="AO6" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="AP6" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="AQ6" s="6" t="s">
         <v>34</v>
@@ -2406,246 +2406,246 @@
         <v>38</v>
       </c>
       <c r="AV6" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AW6" s="14" t="s">
+      <c r="AX6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AY6" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="AX6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AY6" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="AZ6" s="14" t="s">
         <v>39</v>
       </c>
       <c r="BA6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="BC6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="BD6" s="9" t="s">
+      <c r="BF6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="BE6" s="9" t="s">
+      <c r="BG6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="BF6" s="9" t="s">
+      <c r="BH6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="BG6" s="9" t="s">
+      <c r="BI6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="BH6" s="9" t="s">
+      <c r="BJ6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="BI6" s="9" t="s">
+      <c r="BK6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="BJ6" s="9" t="s">
+      <c r="BL6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BK6" s="9" t="s">
+      <c r="BM6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="BL6" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="BM6" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="BN6" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="BO6" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="BP6" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
       <c r="AV8" s="17"/>
       <c r="AW8" s="17"/>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
       <c r="AV9" s="17"/>
       <c r="AW9" s="17"/>
     </row>
-    <row r="1048519" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048519" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048519" s="13"/>
     </row>
-    <row r="1048520" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048520" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048520" s="13"/>
     </row>
-    <row r="1048521" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048521" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048521" s="13"/>
     </row>
-    <row r="1048522" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048522" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048522" s="13"/>
     </row>
-    <row r="1048523" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048523" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048523" s="13"/>
     </row>
-    <row r="1048524" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048524" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048524" s="13"/>
     </row>
-    <row r="1048525" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048525" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048525" s="13"/>
     </row>
-    <row r="1048526" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048526" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048526" s="13"/>
     </row>
-    <row r="1048527" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048527" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048527" s="13"/>
     </row>
-    <row r="1048528" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048528" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048528" s="13"/>
     </row>
-    <row r="1048529" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048529" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048529" s="13"/>
     </row>
-    <row r="1048530" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048530" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048530" s="13"/>
     </row>
-    <row r="1048531" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048531" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048531" s="13"/>
     </row>
-    <row r="1048532" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048532" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048532" s="13"/>
     </row>
-    <row r="1048533" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048533" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048533" s="13"/>
     </row>
-    <row r="1048534" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048534" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048534" s="13"/>
     </row>
-    <row r="1048535" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048535" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048535" s="13"/>
     </row>
-    <row r="1048536" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048536" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048536" s="13"/>
     </row>
-    <row r="1048537" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048537" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048537" s="13"/>
     </row>
-    <row r="1048538" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048538" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048538" s="13"/>
     </row>
-    <row r="1048539" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048539" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048539" s="13"/>
     </row>
-    <row r="1048540" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048540" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048540" s="13"/>
     </row>
-    <row r="1048541" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048541" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048541" s="13"/>
     </row>
-    <row r="1048542" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048542" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048542" s="13"/>
     </row>
-    <row r="1048543" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048543" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048543" s="13"/>
     </row>
-    <row r="1048544" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048544" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048544" s="13"/>
     </row>
-    <row r="1048545" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048545" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048545" s="13"/>
     </row>
-    <row r="1048546" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048546" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048546" s="13"/>
     </row>
-    <row r="1048547" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048547" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048547" s="13"/>
     </row>
-    <row r="1048548" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048548" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048548" s="13"/>
     </row>
-    <row r="1048549" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048549" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048549" s="13"/>
     </row>
-    <row r="1048550" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048550" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048550" s="13"/>
     </row>
-    <row r="1048551" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048551" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048551" s="13"/>
     </row>
-    <row r="1048552" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048552" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048552" s="13"/>
     </row>
-    <row r="1048553" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048553" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048553" s="13"/>
     </row>
-    <row r="1048554" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048554" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048554" s="13"/>
     </row>
-    <row r="1048555" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048555" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048555" s="13"/>
     </row>
-    <row r="1048556" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048556" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048556" s="13"/>
     </row>
-    <row r="1048557" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048557" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048557" s="13"/>
     </row>
-    <row r="1048558" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048558" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048558" s="13"/>
     </row>
-    <row r="1048559" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048559" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048559" s="13"/>
     </row>
-    <row r="1048560" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048560" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048560" s="13"/>
     </row>
-    <row r="1048561" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048561" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048561" s="13"/>
     </row>
-    <row r="1048562" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048562" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048562" s="13"/>
     </row>
-    <row r="1048563" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048563" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048563" s="13"/>
     </row>
-    <row r="1048564" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048564" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048564" s="13"/>
     </row>
-    <row r="1048565" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048565" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048565" s="13"/>
     </row>
-    <row r="1048566" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048566" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048566" s="13"/>
     </row>
-    <row r="1048567" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048567" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048567" s="13"/>
     </row>
-    <row r="1048568" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048568" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048568" s="13"/>
     </row>
-    <row r="1048569" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048569" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048569" s="13"/>
     </row>
-    <row r="1048570" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048570" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048570" s="13"/>
     </row>
-    <row r="1048571" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048571" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048571" s="13"/>
     </row>
-    <row r="1048572" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048572" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048572" s="13"/>
     </row>
-    <row r="1048573" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048573" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048573" s="13"/>
     </row>
-    <row r="1048574" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048574" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048574" s="13"/>
     </row>
-    <row r="1048575" spans="43:43" x14ac:dyDescent="0.35">
+    <row r="1048575" spans="43:43" x14ac:dyDescent="0.25">
       <c r="AQ1048575" s="13"/>
     </row>
   </sheetData>
@@ -2675,39 +2675,39 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="15" customWidth="1"/>
-    <col min="6" max="7" width="14.58203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.875" style="15" customWidth="1"/>
+    <col min="6" max="7" width="14.625" style="10" customWidth="1"/>
     <col min="9" max="9" width="9.25" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="13.75" customWidth="1"/>
-    <col min="12" max="12" width="15.58203125" customWidth="1"/>
-    <col min="13" max="13" width="14.08203125" customWidth="1"/>
+    <col min="12" max="12" width="15.625" customWidth="1"/>
+    <col min="13" max="13" width="14.125" customWidth="1"/>
     <col min="14" max="14" width="15.75" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
     <col min="17" max="17" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.5">
-      <c r="B1" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
@@ -2725,7 +2725,7 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2735,36 +2735,36 @@
       <c r="G2"/>
       <c r="Q2"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B3" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="57"/>
-    </row>
-    <row r="4" spans="1:26" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B3" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="59"/>
+    </row>
+    <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>4</v>
@@ -2773,37 +2773,37 @@
         <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>33</v>
       </c>
       <c r="I4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>35</v>
@@ -2818,175 +2818,175 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1048517" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048517" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048517" s="13"/>
     </row>
-    <row r="1048518" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048518" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048518" s="13"/>
     </row>
-    <row r="1048519" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048519" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048519" s="13"/>
     </row>
-    <row r="1048520" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048520" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048520" s="13"/>
     </row>
-    <row r="1048521" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048521" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048521" s="13"/>
     </row>
-    <row r="1048522" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048522" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048522" s="13"/>
     </row>
-    <row r="1048523" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048523" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048523" s="13"/>
     </row>
-    <row r="1048524" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048524" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048524" s="13"/>
     </row>
-    <row r="1048525" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048525" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048525" s="13"/>
     </row>
-    <row r="1048526" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048526" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048526" s="13"/>
     </row>
-    <row r="1048527" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048527" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048527" s="13"/>
     </row>
-    <row r="1048528" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048528" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048528" s="13"/>
     </row>
-    <row r="1048529" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048529" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048529" s="13"/>
     </row>
-    <row r="1048530" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048530" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048530" s="13"/>
     </row>
-    <row r="1048531" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048531" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048531" s="13"/>
     </row>
-    <row r="1048532" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048532" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048532" s="13"/>
     </row>
-    <row r="1048533" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048533" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048533" s="13"/>
     </row>
-    <row r="1048534" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048534" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048534" s="13"/>
     </row>
-    <row r="1048535" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048535" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048535" s="13"/>
     </row>
-    <row r="1048536" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048536" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048536" s="13"/>
     </row>
-    <row r="1048537" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048537" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048537" s="13"/>
     </row>
-    <row r="1048538" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048538" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048538" s="13"/>
     </row>
-    <row r="1048539" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048539" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048539" s="13"/>
     </row>
-    <row r="1048540" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048540" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048540" s="13"/>
     </row>
-    <row r="1048541" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048541" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048541" s="13"/>
     </row>
-    <row r="1048542" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048542" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048542" s="13"/>
     </row>
-    <row r="1048543" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048543" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048543" s="13"/>
     </row>
-    <row r="1048544" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048544" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048544" s="13"/>
     </row>
-    <row r="1048545" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048545" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048545" s="13"/>
     </row>
-    <row r="1048546" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048546" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048546" s="13"/>
     </row>
-    <row r="1048547" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048547" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048547" s="13"/>
     </row>
-    <row r="1048548" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048548" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048548" s="13"/>
     </row>
-    <row r="1048549" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048549" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048549" s="13"/>
     </row>
-    <row r="1048550" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048550" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048550" s="13"/>
     </row>
-    <row r="1048551" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048551" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048551" s="13"/>
     </row>
-    <row r="1048552" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048552" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048552" s="13"/>
     </row>
-    <row r="1048553" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048553" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048553" s="13"/>
     </row>
-    <row r="1048554" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048554" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048554" s="13"/>
     </row>
-    <row r="1048555" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048555" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048555" s="13"/>
     </row>
-    <row r="1048556" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048556" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048556" s="13"/>
     </row>
-    <row r="1048557" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048557" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048557" s="13"/>
     </row>
-    <row r="1048558" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048558" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048558" s="13"/>
     </row>
-    <row r="1048559" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048559" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048559" s="13"/>
     </row>
-    <row r="1048560" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048560" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048560" s="13"/>
     </row>
-    <row r="1048561" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048561" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048561" s="13"/>
     </row>
-    <row r="1048562" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048562" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048562" s="13"/>
     </row>
-    <row r="1048563" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048563" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048563" s="13"/>
     </row>
-    <row r="1048564" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048564" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048564" s="13"/>
     </row>
-    <row r="1048565" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048565" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048565" s="13"/>
     </row>
-    <row r="1048566" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048566" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048566" s="13"/>
     </row>
-    <row r="1048567" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048567" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048567" s="13"/>
     </row>
-    <row r="1048568" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048568" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048568" s="13"/>
     </row>
-    <row r="1048569" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048569" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048569" s="13"/>
     </row>
-    <row r="1048570" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048570" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048570" s="13"/>
     </row>
-    <row r="1048571" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048571" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048571" s="13"/>
     </row>
-    <row r="1048572" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048572" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048572" s="13"/>
     </row>
-    <row r="1048573" spans="15:15" x14ac:dyDescent="0.35">
+    <row r="1048573" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048573" s="13"/>
     </row>
   </sheetData>
@@ -3006,74 +3006,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="4" width="11.58203125" customWidth="1"/>
-    <col min="7" max="7" width="26.58203125" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
-    <col min="10" max="10" width="15.58203125" customWidth="1"/>
+    <col min="1" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="4" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="26.625" customWidth="1"/>
+    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
     <col min="11" max="11" width="13.75" customWidth="1"/>
-    <col min="12" max="14" width="15.58203125" customWidth="1"/>
+    <col min="12" max="14" width="15.625" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="17" max="17" width="11.58203125" customWidth="1"/>
-    <col min="19" max="19" width="11.58203125" customWidth="1"/>
+    <col min="17" max="17" width="11.625" customWidth="1"/>
+    <col min="19" max="19" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="60"/>
+    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="34"/>
       <c r="C3" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="57"/>
-    </row>
-    <row r="4" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="59"/>
+    </row>
+    <row r="4" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>4</v>
@@ -3088,25 +3088,25 @@
         <v>33</v>
       </c>
       <c r="I4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>35</v>
@@ -3140,52 +3140,52 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.08203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.58203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>85</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>86</v>
       </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="12"/>
@@ -3194,9 +3194,9 @@
       <c r="F4" s="12"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="12"/>
@@ -3205,9 +3205,9 @@
       <c r="F5" s="12"/>
       <c r="G5" s="27"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="12"/>

</xml_diff>

<commit_message>
Update desk review price info to reference doc_no instead of pin (#344)
* First pass

* Update naming

* Switch order

* Edit template and rework solution

* Remove comments

* Linting

* Linting

* Linting

* Fix formatting

* Lint

* Grab up to date template

* Add tentative solution

* Update template and doc number linking PR (#354)

* Update template and doc_no linking

* Revert township code source

* Remove unnecessary ungroup

---------

Co-authored-by: Dan Snow <31494343+dfsnow@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420304A6-F863-4354-90DD-E847C8870184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C332071-65F2-4E46-A8C4-44A2DF842DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -113,7 +113,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column shows the PIN for the sale that the model thinks is most comparablet to the target parcel. Click the link to navigate to the corresponding row in the Sales tab of this sheet.</t>
+          <t>This column shows the sale that the model thinks is most comparable to the target parcel. Click the link to navigate to the corresponding row in the Comparables tab of this sheet.</t>
         </r>
       </text>
     </comment>
@@ -392,7 +392,7 @@
     <author>Jean Cochrane (Assessor)</author>
   </authors>
   <commentList>
-    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{631EDC07-49FD-49B1-BCE6-37E31B1ACEE7}">
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{631EDC07-49FD-49B1-BCE6-37E31B1ACEE7}">
       <text>
         <r>
           <rPr>
@@ -405,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{0C3D05B0-7DDF-44DF-B6CD-F791DF4DB5A2}">
+    <comment ref="S4" authorId="0" shapeId="0" xr:uid="{0C3D05B0-7DDF-44DF-B6CD-F791DF4DB5A2}">
       <text>
         <r>
           <rPr>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="95">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -545,15 +545,9 @@
     <t>Overall Comp. Score</t>
   </si>
   <si>
-    <t>Comp. 1 PIN</t>
-  </si>
-  <si>
     <t>Comp. 1 Score</t>
   </si>
   <si>
-    <t>Comp. 2 PIN</t>
-  </si>
-  <si>
     <t>Comp. 2 Score</t>
   </si>
   <si>
@@ -705,6 +699,15 @@
   </si>
   <si>
     <t>Recent Assessable Permit</t>
+  </si>
+  <si>
+    <t>Doc. No</t>
+  </si>
+  <si>
+    <t>Comp. 1 Sale</t>
+  </si>
+  <si>
+    <t>Comp. 2 Sale</t>
   </si>
 </sst>
 </file>
@@ -847,7 +850,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -972,6 +975,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -980,7 +998,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1049,6 +1067,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1157,7 +1182,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45699.667643518522" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45708.629130439818" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1307,13 +1332,13 @@
     <cacheField name="# Comm. Units" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Comp. 1 PIN" numFmtId="37">
+    <cacheField name="Comp. 1 Sale" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Comp. 1 Score" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Comp. 2 PIN" numFmtId="37">
+    <cacheField name="Comp. 2 Sale" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Comp. 2 Score" numFmtId="37">
@@ -1361,7 +1386,7 @@
     <cacheField name="Critical Char. Missing" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Assessable Permit in Past 3 Years" numFmtId="0">
+    <cacheField name="Recent Assessable Permit" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total AV" numFmtId="0">
@@ -1455,7 +1480,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="68">
     <pivotField showAll="0"/>
@@ -1596,9 +1621,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1636,7 +1661,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1742,7 +1767,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1884,7 +1909,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1898,7 +1923,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1940,9 +1965,9 @@
     <col min="42" max="42" width="15.375" customWidth="1"/>
     <col min="44" max="44" width="8.125" customWidth="1"/>
     <col min="45" max="47" width="11" style="13"/>
-    <col min="48" max="48" width="15.625" style="13" customWidth="1"/>
+    <col min="48" max="48" width="11" style="13" customWidth="1"/>
     <col min="49" max="49" width="11" style="13"/>
-    <col min="50" max="50" width="15.625" style="13" customWidth="1"/>
+    <col min="50" max="50" width="11" style="13" customWidth="1"/>
     <col min="51" max="52" width="11" style="13"/>
     <col min="61" max="61" width="14" customWidth="1"/>
     <col min="62" max="62" width="12.375" customWidth="1"/>
@@ -1956,15 +1981,15 @@
   <sheetData>
     <row r="1" spans="1:68" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -2070,9 +2095,9 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2158,84 +2183,84 @@
       <c r="AZ4"/>
     </row>
     <row r="5" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="40"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="55"/>
+      <c r="B5" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="44"/>
+      <c r="X5" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y5" s="57"/>
+      <c r="Z5" s="58"/>
       <c r="AA5" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="45"/>
-      <c r="AD5" s="45"/>
-      <c r="AE5" s="46"/>
-      <c r="AF5" s="45"/>
-      <c r="AG5" s="45"/>
-      <c r="AH5" s="46"/>
-      <c r="AI5" s="47"/>
-      <c r="AJ5" s="51" t="s">
+      <c r="AB5" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="48"/>
+      <c r="AG5" s="48"/>
+      <c r="AH5" s="49"/>
+      <c r="AI5" s="50"/>
+      <c r="AJ5" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="AK5" s="52"/>
-      <c r="AL5" s="52"/>
-      <c r="AM5" s="52"/>
-      <c r="AN5" s="52"/>
-      <c r="AO5" s="52"/>
-      <c r="AP5" s="52"/>
-      <c r="AQ5" s="52"/>
-      <c r="AR5" s="52"/>
-      <c r="AS5" s="52"/>
-      <c r="AT5" s="52"/>
-      <c r="AU5" s="52"/>
-      <c r="AV5" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW5" s="43"/>
-      <c r="AX5" s="43"/>
-      <c r="AY5" s="43"/>
+      <c r="AK5" s="55"/>
+      <c r="AL5" s="55"/>
+      <c r="AM5" s="55"/>
+      <c r="AN5" s="55"/>
+      <c r="AO5" s="55"/>
+      <c r="AP5" s="55"/>
+      <c r="AQ5" s="55"/>
+      <c r="AR5" s="55"/>
+      <c r="AS5" s="55"/>
+      <c r="AT5" s="55"/>
+      <c r="AU5" s="55"/>
+      <c r="AV5" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW5" s="46"/>
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="46"/>
       <c r="AZ5" s="21"/>
-      <c r="BA5" s="37" t="s">
+      <c r="BA5" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="BB5" s="38"/>
-      <c r="BC5" s="38"/>
-      <c r="BD5" s="38"/>
-      <c r="BE5" s="38"/>
-      <c r="BF5" s="38"/>
-      <c r="BG5" s="38"/>
-      <c r="BH5" s="38"/>
-      <c r="BI5" s="38"/>
-      <c r="BJ5" s="38"/>
-      <c r="BK5" s="38"/>
-      <c r="BL5" s="38"/>
-      <c r="BM5" s="38"/>
+      <c r="BB5" s="41"/>
+      <c r="BC5" s="41"/>
+      <c r="BD5" s="41"/>
+      <c r="BE5" s="41"/>
+      <c r="BF5" s="41"/>
+      <c r="BG5" s="41"/>
+      <c r="BH5" s="41"/>
+      <c r="BI5" s="41"/>
+      <c r="BJ5" s="41"/>
+      <c r="BK5" s="41"/>
+      <c r="BL5" s="41"/>
+      <c r="BM5" s="41"/>
       <c r="BN5" s="31"/>
     </row>
     <row r="6" spans="1:68" ht="47.25" x14ac:dyDescent="0.25">
@@ -2315,10 +2340,10 @@
         <v>24</v>
       </c>
       <c r="Z6" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AB6" s="2" t="s">
         <v>25</v>
@@ -2348,22 +2373,22 @@
         <v>33</v>
       </c>
       <c r="AK6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP6" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="AL6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="AO6" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="AP6" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="AQ6" s="6" t="s">
         <v>34</v>
@@ -2381,67 +2406,67 @@
         <v>38</v>
       </c>
       <c r="AV6" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AW6" s="14" t="s">
+      <c r="AX6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AY6" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="AX6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AY6" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="AZ6" s="14" t="s">
         <v>39</v>
       </c>
       <c r="BA6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="BC6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BD6" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BE6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="BD6" s="9" t="s">
+      <c r="BF6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="BE6" s="9" t="s">
+      <c r="BG6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="BF6" s="9" t="s">
+      <c r="BH6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="BG6" s="9" t="s">
+      <c r="BI6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="BH6" s="9" t="s">
+      <c r="BJ6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="BI6" s="9" t="s">
+      <c r="BK6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="BJ6" s="9" t="s">
+      <c r="BL6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="BK6" s="9" t="s">
+      <c r="BM6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="BL6" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="BM6" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="BN6" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="BO6" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="BP6" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:68" x14ac:dyDescent="0.25">
@@ -2650,7 +2675,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2672,17 +2697,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="B1" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
@@ -2711,35 +2736,35 @@
       <c r="Q2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="56"/>
+      <c r="B3" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="59"/>
     </row>
     <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>4</v>
@@ -2748,37 +2773,37 @@
         <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>33</v>
       </c>
       <c r="I4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>35</v>
@@ -2979,125 +3004,128 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD7EE4-F89B-4035-AD7B-A1EB78B3F665}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="3" width="11.625" customWidth="1"/>
-    <col min="6" max="6" width="26.625" customWidth="1"/>
-    <col min="7" max="7" width="11.875" customWidth="1"/>
-    <col min="9" max="9" width="15.625" customWidth="1"/>
-    <col min="10" max="10" width="13.75" customWidth="1"/>
-    <col min="11" max="13" width="15.625" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="16" max="16" width="11.625" customWidth="1"/>
-    <col min="18" max="18" width="11.625" customWidth="1"/>
+    <col min="1" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="4" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="26.625" customWidth="1"/>
+    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
+    <col min="11" max="11" width="13.75" customWidth="1"/>
+    <col min="12" max="14" width="15.625" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="17" max="17" width="11.625" customWidth="1"/>
+    <col min="19" max="19" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51" t="s">
+    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="34"/>
+      <c r="C3" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="56"/>
-    </row>
-    <row r="4" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="59"/>
+    </row>
+    <row r="4" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="O4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="S4" s="20" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:R3"/>
+  <mergeCells count="3">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3125,7 +3153,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -3134,30 +3162,30 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>85</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>86</v>
-      </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="12"/>
@@ -3168,7 +3196,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="12"/>
@@ -3179,7 +3207,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="12"/>

</xml_diff>

<commit_message>
update to market values rather than assessed values
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8C7427-B209-4D26-ADED-6573D6564EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958634DC-A64C-4579-9015-EDAACD9D8F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5145" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -47,8 +47,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jean Cochrane</author>
+    <author>Damon Major</author>
     <author>Jean Cochrane (Assessor)</author>
-    <author>Damon Major</author>
   </authors>
   <commentList>
     <comment ref="Z6" authorId="0" shapeId="0" xr:uid="{B959BBC6-269B-40A9-8222-4E035C25B553}">
@@ -78,7 +78,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
+    <comment ref="AH6" authorId="1" shapeId="0" xr:uid="{1766D256-2861-4BBA-8780-2C986F60238F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm.
+If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AT6" authorId="2" shapeId="0" xr:uid="{E801C296-DBF0-4A45-8600-56AFE18D9932}">
       <text>
         <r>
           <rPr>
@@ -91,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
+    <comment ref="AU6" authorId="2" shapeId="0" xr:uid="{8499B5E6-DE08-4F49-BEC1-0664F772026C}">
       <text>
         <r>
           <rPr>
@@ -143,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY6" authorId="2" shapeId="0" xr:uid="{0D45338F-140B-44D7-B8C4-BE9610B66C03}">
+    <comment ref="AY6" authorId="1" shapeId="0" xr:uid="{0D45338F-140B-44D7-B8C4-BE9610B66C03}">
       <text>
         <r>
           <rPr>
@@ -602,12 +617,6 @@
     <t>Count of Class</t>
   </si>
   <si>
-    <t>Total AV</t>
-  </si>
-  <si>
-    <t>AV Difference</t>
-  </si>
-  <si>
     <t>Average of YoY ∆ %</t>
   </si>
   <si>
@@ -648,6 +657,12 @@
   </si>
   <si>
     <t>Average of MV Difference</t>
+  </si>
+  <si>
+    <t>MV Difference</t>
+  </si>
+  <si>
+    <t>Total MV</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1106,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46057.712321874998" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46058.584369675926" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1813,11 +1828,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM1048575"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="AQ7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="AX6" sqref="AX6"/>
+      <selection pane="bottomRight" activeCell="BL1" sqref="BL1:BM1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1865,7 +1880,7 @@
     <col min="60" max="60" width="11.875" customWidth="1"/>
     <col min="61" max="61" width="10.875" customWidth="1"/>
     <col min="62" max="62" width="11.5" customWidth="1"/>
-    <col min="63" max="63" width="13" customWidth="1"/>
+    <col min="63" max="63" width="10" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="7.75" hidden="1" customWidth="1"/>
     <col min="65" max="65" width="9.375" hidden="1" customWidth="1"/>
   </cols>
@@ -2116,7 +2131,7 @@
       <c r="AT5" s="50"/>
       <c r="AU5" s="50"/>
       <c r="AV5" s="31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AW5" s="37" t="s">
         <v>2</v>
@@ -2213,7 +2228,7 @@
         <v>24</v>
       </c>
       <c r="Z6" s="28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AA6" s="3" t="s">
         <v>66</v>
@@ -2252,13 +2267,13 @@
         <v>57</v>
       </c>
       <c r="AM6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO6" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AO6" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="AP6" s="6" t="s">
         <v>58</v>
@@ -2279,16 +2294,16 @@
         <v>38</v>
       </c>
       <c r="AV6" s="22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AW6" s="9" t="s">
         <v>39</v>
       </c>
       <c r="AX6" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AY6" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AZ6" s="9" t="s">
         <v>40</v>
@@ -2324,13 +2339,13 @@
         <v>50</v>
       </c>
       <c r="BK6" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="BL6" s="3" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="BM6" s="4" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
@@ -2652,13 +2667,13 @@
         <v>57</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>58</v>
@@ -2867,7 +2882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D773A1D3-FC14-4EA4-B569-35CAE3B3E4FA}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -2899,19 +2914,19 @@
         <v>71</v>
       </c>
       <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>85</v>
       </c>
-      <c r="E3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
small xlsx change, move igraph
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958634DC-A64C-4579-9015-EDAACD9D8F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B887856-3C0B-410A-B536-6035EDBAB426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="11" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -399,7 +399,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -635,9 +635,6 @@
     <t>Recent Assessable Permit</t>
   </si>
   <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>Proration Rates Don't Sum to 100%</t>
   </si>
   <si>
@@ -647,22 +644,13 @@
     <t>HomeVal Report</t>
   </si>
   <si>
-    <t>Min of Total MV</t>
-  </si>
-  <si>
-    <t>Average of Total MV</t>
-  </si>
-  <si>
-    <t>Max of Total MV</t>
-  </si>
-  <si>
-    <t>Average of MV Difference</t>
-  </si>
-  <si>
     <t>MV Difference</t>
   </si>
   <si>
     <t>Total MV</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1094,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46058.584369675926" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46063.592228703703" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1304,10 +1292,10 @@
     <cacheField name="Recent Assessable Permit" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Total AV" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="AV Difference" numFmtId="0">
+    <cacheField name="Total MV" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="MV Difference" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
   </cacheFields>
@@ -1392,8 +1380,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="65">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -1468,8 +1456,8 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="2"/>
@@ -1489,32 +1477,16 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="6">
+  <colItems count="2">
     <i>
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
     </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
   </colItems>
-  <dataFields count="6">
+  <dataFields count="2">
     <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="1"/>
-    <dataField name="Min of Total MV" fld="63" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total MV" fld="63" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total MV" fld="63" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of MV Difference" fld="64" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1832,60 +1804,60 @@
       <pane xSplit="1" ySplit="6" topLeftCell="AQ7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="BL1" sqref="BL1:BM1048576"/>
+      <selection pane="bottomRight" activeCell="AV7" sqref="AV7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="38.875" customWidth="1"/>
-    <col min="5" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="8.875" customWidth="1"/>
-    <col min="8" max="8" width="15.375" customWidth="1"/>
-    <col min="9" max="9" width="13.875" style="11" customWidth="1"/>
-    <col min="10" max="11" width="11.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.83203125" customWidth="1"/>
+    <col min="5" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="11" customWidth="1"/>
+    <col min="10" max="11" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="10" customWidth="1"/>
-    <col min="13" max="13" width="10.875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="10.625" style="10" customWidth="1"/>
-    <col min="15" max="15" width="9.125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="13.625" style="15" customWidth="1"/>
-    <col min="17" max="18" width="11.625" style="10" customWidth="1"/>
-    <col min="19" max="19" width="13.625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="10.58203125" style="10" customWidth="1"/>
+    <col min="15" max="15" width="9.08203125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="13.58203125" style="15" customWidth="1"/>
+    <col min="17" max="18" width="11.58203125" style="10" customWidth="1"/>
+    <col min="19" max="19" width="13.58203125" style="10" customWidth="1"/>
     <col min="20" max="20" width="11" style="10"/>
-    <col min="21" max="21" width="10.875" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.125" style="10" customWidth="1"/>
-    <col min="23" max="23" width="11.625" style="11" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.08203125" style="10" customWidth="1"/>
+    <col min="23" max="23" width="11.58203125" style="11" customWidth="1"/>
     <col min="24" max="24" width="11" style="12"/>
     <col min="25" max="26" width="11" style="11"/>
-    <col min="27" max="27" width="21.125" style="11" customWidth="1"/>
+    <col min="27" max="27" width="21.08203125" style="11" customWidth="1"/>
     <col min="28" max="28" width="13" customWidth="1"/>
     <col min="29" max="29" width="13" style="10" customWidth="1"/>
-    <col min="30" max="30" width="18.625" style="10" customWidth="1"/>
+    <col min="30" max="30" width="18.58203125" style="10" customWidth="1"/>
     <col min="31" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="34" width="18.625" style="10" customWidth="1"/>
+    <col min="34" max="34" width="18.58203125" style="10" customWidth="1"/>
     <col min="35" max="35" width="13" style="16" customWidth="1"/>
     <col min="37" max="37" width="9.25" customWidth="1"/>
-    <col min="38" max="38" width="7.375" customWidth="1"/>
-    <col min="40" max="40" width="15.125" customWidth="1"/>
-    <col min="41" max="41" width="15.625" customWidth="1"/>
-    <col min="42" max="42" width="15.375" customWidth="1"/>
-    <col min="44" max="44" width="8.125" customWidth="1"/>
+    <col min="38" max="38" width="7.33203125" customWidth="1"/>
+    <col min="40" max="40" width="15.08203125" customWidth="1"/>
+    <col min="41" max="41" width="15.58203125" customWidth="1"/>
+    <col min="42" max="42" width="15.33203125" customWidth="1"/>
+    <col min="44" max="44" width="8.08203125" customWidth="1"/>
     <col min="45" max="47" width="11" style="13"/>
     <col min="48" max="48" width="16" style="13" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="14" customWidth="1"/>
-    <col min="59" max="59" width="12.375" customWidth="1"/>
-    <col min="60" max="60" width="11.875" customWidth="1"/>
-    <col min="61" max="61" width="10.875" customWidth="1"/>
+    <col min="59" max="59" width="12.33203125" customWidth="1"/>
+    <col min="60" max="60" width="11.83203125" customWidth="1"/>
+    <col min="61" max="61" width="10.83203125" customWidth="1"/>
     <col min="62" max="62" width="11.5" customWidth="1"/>
     <col min="63" max="63" width="10" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="7.75" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="9.375" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="9.33203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:65" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="5"/>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -1950,7 +1922,7 @@
       <c r="BJ1" s="5"/>
       <c r="BK1" s="5"/>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1990,7 +1962,7 @@
       <c r="AU2"/>
       <c r="AV2"/>
     </row>
-    <row r="3" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2031,7 +2003,7 @@
       <c r="AU3"/>
       <c r="AV3"/>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2073,7 +2045,7 @@
       <c r="AU4" s="19"/>
       <c r="AV4"/>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.35">
       <c r="B5" s="46" t="s">
         <v>60</v>
       </c>
@@ -2131,7 +2103,7 @@
       <c r="AT5" s="50"/>
       <c r="AU5" s="50"/>
       <c r="AV5" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AW5" s="37" t="s">
         <v>2</v>
@@ -2151,7 +2123,7 @@
       <c r="BJ5" s="38"/>
       <c r="BK5" s="30"/>
     </row>
-    <row r="6" spans="1:65" ht="63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2294,16 +2266,16 @@
         <v>38</v>
       </c>
       <c r="AV6" s="22" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="AW6" s="9" t="s">
         <v>39</v>
       </c>
       <c r="AX6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY6" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="AY6" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="AZ6" s="9" t="s">
         <v>40</v>
@@ -2342,187 +2314,187 @@
         <v>77</v>
       </c>
       <c r="BL6" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="BM6" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.35">
       <c r="AV8" s="17"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.35">
       <c r="AV9" s="17"/>
     </row>
-    <row r="1048519" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048519" s="13"/>
     </row>
-    <row r="1048520" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048520" s="13"/>
     </row>
-    <row r="1048521" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048521" s="13"/>
     </row>
-    <row r="1048522" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048522" s="13"/>
     </row>
-    <row r="1048523" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048523" s="13"/>
     </row>
-    <row r="1048524" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048524" s="13"/>
     </row>
-    <row r="1048525" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048525" s="13"/>
     </row>
-    <row r="1048526" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048526" s="13"/>
     </row>
-    <row r="1048527" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048527" s="13"/>
     </row>
-    <row r="1048528" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048528" s="13"/>
     </row>
-    <row r="1048529" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048529" s="13"/>
     </row>
-    <row r="1048530" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048530" s="13"/>
     </row>
-    <row r="1048531" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048531" s="13"/>
     </row>
-    <row r="1048532" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048532" s="13"/>
     </row>
-    <row r="1048533" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048533" s="13"/>
     </row>
-    <row r="1048534" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048534" s="13"/>
     </row>
-    <row r="1048535" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048535" s="13"/>
     </row>
-    <row r="1048536" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048536" s="13"/>
     </row>
-    <row r="1048537" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048537" s="13"/>
     </row>
-    <row r="1048538" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048538" s="13"/>
     </row>
-    <row r="1048539" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048539" s="13"/>
     </row>
-    <row r="1048540" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048540" s="13"/>
     </row>
-    <row r="1048541" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048541" s="13"/>
     </row>
-    <row r="1048542" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048542" s="13"/>
     </row>
-    <row r="1048543" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048543" s="13"/>
     </row>
-    <row r="1048544" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048544" s="13"/>
     </row>
-    <row r="1048545" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048545" s="13"/>
     </row>
-    <row r="1048546" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048546" s="13"/>
     </row>
-    <row r="1048547" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048547" s="13"/>
     </row>
-    <row r="1048548" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048548" s="13"/>
     </row>
-    <row r="1048549" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048549" s="13"/>
     </row>
-    <row r="1048550" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048550" s="13"/>
     </row>
-    <row r="1048551" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048551" s="13"/>
     </row>
-    <row r="1048552" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048552" s="13"/>
     </row>
-    <row r="1048553" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048553" s="13"/>
     </row>
-    <row r="1048554" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048554" s="13"/>
     </row>
-    <row r="1048555" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048555" s="13"/>
     </row>
-    <row r="1048556" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048556" s="13"/>
     </row>
-    <row r="1048557" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048557" s="13"/>
     </row>
-    <row r="1048558" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048558" s="13"/>
     </row>
-    <row r="1048559" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048559" s="13"/>
     </row>
-    <row r="1048560" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048560" s="13"/>
     </row>
-    <row r="1048561" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048561" s="13"/>
     </row>
-    <row r="1048562" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048562" s="13"/>
     </row>
-    <row r="1048563" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048563" s="13"/>
     </row>
-    <row r="1048564" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048564" s="13"/>
     </row>
-    <row r="1048565" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048565" s="13"/>
     </row>
-    <row r="1048566" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048566" s="13"/>
     </row>
-    <row r="1048567" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048567" s="13"/>
     </row>
-    <row r="1048568" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048568" s="13"/>
     </row>
-    <row r="1048569" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048569" s="13"/>
     </row>
-    <row r="1048570" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048570" s="13"/>
     </row>
-    <row r="1048571" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048571" s="13"/>
     </row>
-    <row r="1048572" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048572" s="13"/>
     </row>
-    <row r="1048573" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048573" s="13"/>
     </row>
-    <row r="1048574" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048574" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048574" s="13"/>
     </row>
-    <row r="1048575" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="1048575" spans="43:43" x14ac:dyDescent="0.35">
       <c r="AQ1048575" s="13"/>
     </row>
   </sheetData>
@@ -2554,25 +2526,25 @@
       <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.875" style="15" customWidth="1"/>
-    <col min="6" max="7" width="14.625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="15" customWidth="1"/>
+    <col min="6" max="7" width="14.58203125" style="10" customWidth="1"/>
     <col min="9" max="9" width="9.25" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="13.75" customWidth="1"/>
-    <col min="12" max="12" width="15.625" customWidth="1"/>
-    <col min="13" max="13" width="14.125" customWidth="1"/>
+    <col min="12" max="12" width="15.58203125" customWidth="1"/>
+    <col min="13" max="13" width="14.08203125" customWidth="1"/>
     <col min="14" max="14" width="15.75" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
     <col min="17" max="17" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.5">
       <c r="B1" s="33" t="s">
         <v>51</v>
       </c>
@@ -2601,7 +2573,7 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2611,7 +2583,7 @@
       <c r="G2"/>
       <c r="Q2"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B3" s="46" t="s">
         <v>62</v>
       </c>
@@ -2635,7 +2607,7 @@
       <c r="R3" s="50"/>
       <c r="S3" s="54"/>
     </row>
-    <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -2694,175 +2666,175 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1048517" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048517" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048517" s="13"/>
     </row>
-    <row r="1048518" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048518" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048518" s="13"/>
     </row>
-    <row r="1048519" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048519" s="13"/>
     </row>
-    <row r="1048520" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048520" s="13"/>
     </row>
-    <row r="1048521" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048521" s="13"/>
     </row>
-    <row r="1048522" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048522" s="13"/>
     </row>
-    <row r="1048523" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048523" s="13"/>
     </row>
-    <row r="1048524" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048524" s="13"/>
     </row>
-    <row r="1048525" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048525" s="13"/>
     </row>
-    <row r="1048526" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048526" s="13"/>
     </row>
-    <row r="1048527" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048527" s="13"/>
     </row>
-    <row r="1048528" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048528" s="13"/>
     </row>
-    <row r="1048529" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048529" s="13"/>
     </row>
-    <row r="1048530" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048530" s="13"/>
     </row>
-    <row r="1048531" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048531" s="13"/>
     </row>
-    <row r="1048532" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048532" s="13"/>
     </row>
-    <row r="1048533" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048533" s="13"/>
     </row>
-    <row r="1048534" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048534" s="13"/>
     </row>
-    <row r="1048535" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048535" s="13"/>
     </row>
-    <row r="1048536" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048536" s="13"/>
     </row>
-    <row r="1048537" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048537" s="13"/>
     </row>
-    <row r="1048538" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048538" s="13"/>
     </row>
-    <row r="1048539" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048539" s="13"/>
     </row>
-    <row r="1048540" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048540" s="13"/>
     </row>
-    <row r="1048541" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048541" s="13"/>
     </row>
-    <row r="1048542" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048542" s="13"/>
     </row>
-    <row r="1048543" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048543" s="13"/>
     </row>
-    <row r="1048544" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048544" s="13"/>
     </row>
-    <row r="1048545" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048545" s="13"/>
     </row>
-    <row r="1048546" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048546" s="13"/>
     </row>
-    <row r="1048547" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048547" s="13"/>
     </row>
-    <row r="1048548" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048548" s="13"/>
     </row>
-    <row r="1048549" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048549" s="13"/>
     </row>
-    <row r="1048550" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048550" s="13"/>
     </row>
-    <row r="1048551" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048551" s="13"/>
     </row>
-    <row r="1048552" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048552" s="13"/>
     </row>
-    <row r="1048553" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048553" s="13"/>
     </row>
-    <row r="1048554" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048554" s="13"/>
     </row>
-    <row r="1048555" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048555" s="13"/>
     </row>
-    <row r="1048556" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048556" s="13"/>
     </row>
-    <row r="1048557" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048557" s="13"/>
     </row>
-    <row r="1048558" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048558" s="13"/>
     </row>
-    <row r="1048559" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048559" s="13"/>
     </row>
-    <row r="1048560" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048560" s="13"/>
     </row>
-    <row r="1048561" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048561" s="13"/>
     </row>
-    <row r="1048562" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048562" s="13"/>
     </row>
-    <row r="1048563" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048563" s="13"/>
     </row>
-    <row r="1048564" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048564" s="13"/>
     </row>
-    <row r="1048565" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048565" s="13"/>
     </row>
-    <row r="1048566" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048566" s="13"/>
     </row>
-    <row r="1048567" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048567" s="13"/>
     </row>
-    <row r="1048568" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048568" s="13"/>
     </row>
-    <row r="1048569" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048569" s="13"/>
     </row>
-    <row r="1048570" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048570" s="13"/>
     </row>
-    <row r="1048571" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048571" s="13"/>
     </row>
-    <row r="1048572" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048572" s="13"/>
     </row>
-    <row r="1048573" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O1048573" s="13"/>
     </row>
   </sheetData>
@@ -2880,24 +2852,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D773A1D3-FC14-4EA4-B569-35CAE3B3E4FA}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="B1" s="5" t="s">
         <v>70</v>
       </c>
@@ -2906,7 +2878,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="24" t="s">
         <v>67</v>
       </c>
@@ -2914,53 +2886,29 @@
         <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B4" s="27"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="26"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="26"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>68</v>
       </c>
       <c r="B5" s="27"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="26"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="26"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="27"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
include sorting in template
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B887856-3C0B-410A-B536-6035EDBAB426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD406AB-3267-44BF-888D-C0CD75CF9EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId4"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -399,7 +399,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="84">
   <si>
     <t>Run ID (res):</t>
   </si>
@@ -926,7 +926,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -980,9 +980,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1094,7 +1091,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46063.592228703703" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46063.65912546296" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1244,7 +1241,7 @@
     <cacheField name="# Comm. Units" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="link" numFmtId="37">
+    <cacheField name="Link" numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Is Prorated" numFmtId="0">
@@ -1380,19 +1377,19 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D354C13E-180D-4071-9586-5999D6819012}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="65">
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
+    <pivotField axis="axisRow" dataField="1" showAll="0" sortType="ascending">
       <items count="2">
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="2">
-        <item x="0"/>
+        <item sd="0" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1463,11 +1460,8 @@
     <field x="2"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="2">
     <i>
-      <x/>
-    </i>
-    <i r="1">
       <x/>
     </i>
     <i t="grand">
@@ -1800,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="AQ7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
@@ -1859,15 +1853,15 @@
   <sheetData>
     <row r="1" spans="1:65" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="5"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1966,9 +1960,9 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2046,82 +2040,82 @@
       <c r="AV4"/>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.35">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="40"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="51" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="39"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="39"/>
+      <c r="V5" s="39"/>
+      <c r="W5" s="40"/>
+      <c r="X5" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="Y5" s="52"/>
-      <c r="Z5" s="53"/>
+      <c r="Y5" s="51"/>
+      <c r="Z5" s="52"/>
       <c r="AA5" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="AB5" s="42" t="s">
+      <c r="AB5" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="43"/>
-      <c r="AE5" s="44"/>
-      <c r="AF5" s="43"/>
-      <c r="AG5" s="43"/>
-      <c r="AH5" s="44"/>
-      <c r="AI5" s="45"/>
-      <c r="AJ5" s="49" t="s">
+      <c r="AC5" s="42"/>
+      <c r="AD5" s="42"/>
+      <c r="AE5" s="43"/>
+      <c r="AF5" s="42"/>
+      <c r="AG5" s="42"/>
+      <c r="AH5" s="43"/>
+      <c r="AI5" s="44"/>
+      <c r="AJ5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="AK5" s="50"/>
-      <c r="AL5" s="50"/>
-      <c r="AM5" s="50"/>
-      <c r="AN5" s="50"/>
-      <c r="AO5" s="50"/>
-      <c r="AP5" s="50"/>
-      <c r="AQ5" s="50"/>
-      <c r="AR5" s="50"/>
-      <c r="AS5" s="50"/>
-      <c r="AT5" s="50"/>
-      <c r="AU5" s="50"/>
-      <c r="AV5" s="31" t="s">
+      <c r="AK5" s="49"/>
+      <c r="AL5" s="49"/>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="49"/>
+      <c r="AO5" s="49"/>
+      <c r="AP5" s="49"/>
+      <c r="AQ5" s="49"/>
+      <c r="AR5" s="49"/>
+      <c r="AS5" s="49"/>
+      <c r="AT5" s="49"/>
+      <c r="AU5" s="49"/>
+      <c r="AV5" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="AW5" s="37" t="s">
+      <c r="AW5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="AX5" s="38"/>
-      <c r="AY5" s="38"/>
-      <c r="AZ5" s="38"/>
-      <c r="BA5" s="38"/>
-      <c r="BB5" s="38"/>
-      <c r="BC5" s="38"/>
-      <c r="BD5" s="38"/>
-      <c r="BE5" s="38"/>
-      <c r="BF5" s="38"/>
-      <c r="BG5" s="38"/>
-      <c r="BH5" s="38"/>
-      <c r="BI5" s="38"/>
-      <c r="BJ5" s="38"/>
-      <c r="BK5" s="30"/>
+      <c r="AX5" s="37"/>
+      <c r="AY5" s="37"/>
+      <c r="AZ5" s="37"/>
+      <c r="BA5" s="37"/>
+      <c r="BB5" s="37"/>
+      <c r="BC5" s="37"/>
+      <c r="BD5" s="37"/>
+      <c r="BE5" s="37"/>
+      <c r="BF5" s="37"/>
+      <c r="BG5" s="37"/>
+      <c r="BH5" s="37"/>
+      <c r="BI5" s="37"/>
+      <c r="BJ5" s="37"/>
+      <c r="BK5" s="29"/>
     </row>
     <row r="6" spans="1:65" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -2199,7 +2193,7 @@
       <c r="Y6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z6" s="28" t="s">
+      <c r="Z6" s="27" t="s">
         <v>73</v>
       </c>
       <c r="AA6" s="3" t="s">
@@ -2310,7 +2304,7 @@
       <c r="BJ6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="BK6" s="28" t="s">
+      <c r="BK6" s="27" t="s">
         <v>77</v>
       </c>
       <c r="BL6" s="3" t="s">
@@ -2545,20 +2539,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.5">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -2584,28 +2578,28 @@
       <c r="Q2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="49" t="s">
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="54"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="53"/>
     </row>
     <row r="4" spans="1:26" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
@@ -2852,10 +2846,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D773A1D3-FC14-4EA4-B569-35CAE3B3E4FA}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2893,22 +2887,15 @@
       <c r="A4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="25"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="26"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="A5" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update template with post-modeling changes (#447)
This fixes a few things found during modeling season.
- sets the initial view to cell 1 of the Pinsheet
- corrects the HOMEVAL note
- Remove the extra rows in the template which condenses the output to
the correct length.
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD1B511-B482-4F7B-AC3A-0FF8A485954B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8080567A-2060-4788-A3DF-CE1883463FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -128,7 +128,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column shows the sale that the model thinks is most comparable to the target parcel. Click the link to navigate to the corresponding row in the Comparables tab of this sheet.</t>
+          <t>This column links to the HomeVal website showing the sales that the model thinks are most comparable to the target parcel. Click the link to navigate to the website and see the sales.</t>
         </r>
       </text>
     </comment>
@@ -1006,6 +1006,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1074,15 +1083,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1092,24 +1092,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="12">
     <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <alignment horizontal="right"/>
@@ -1118,16 +1106,16 @@
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right"/>
@@ -1136,46 +1124,10 @@
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1197,7 +1149,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46063.776297916665" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46070.626223148145" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{2A499168-87FA-4E81-AAAC-57B5294536D8}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_Range"/>
   </cacheSource>
@@ -1606,7 +1558,7 @@
     <dataField name="Average of YoY ∆ %" fld="24" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="19">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4" selected="0">
@@ -1618,7 +1570,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4">
@@ -1630,7 +1582,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4" selected="0">
@@ -1642,7 +1594,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4">
@@ -1654,7 +1606,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="7">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4" selected="0">
@@ -1666,7 +1618,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="4">
@@ -1988,13 +1940,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BM1048575"/>
+  <dimension ref="A1:BM9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="AQ7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="AV7" sqref="AV7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2049,15 +2001,15 @@
   <sheetData>
     <row r="1" spans="1:65" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="5"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -2156,9 +2108,9 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2236,81 +2188,81 @@
       <c r="AV4"/>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.35">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="39"/>
-      <c r="V5" s="39"/>
-      <c r="W5" s="40"/>
-      <c r="X5" s="50" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="Y5" s="51"/>
-      <c r="Z5" s="52"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="55"/>
       <c r="AA5" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="AB5" s="41" t="s">
+      <c r="AB5" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="AC5" s="42"/>
-      <c r="AD5" s="42"/>
-      <c r="AE5" s="43"/>
-      <c r="AF5" s="42"/>
-      <c r="AG5" s="42"/>
-      <c r="AH5" s="43"/>
-      <c r="AI5" s="44"/>
-      <c r="AJ5" s="48" t="s">
+      <c r="AC5" s="45"/>
+      <c r="AD5" s="45"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="45"/>
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AK5" s="49"/>
-      <c r="AL5" s="49"/>
-      <c r="AM5" s="49"/>
-      <c r="AN5" s="49"/>
-      <c r="AO5" s="49"/>
-      <c r="AP5" s="49"/>
-      <c r="AQ5" s="49"/>
-      <c r="AR5" s="49"/>
-      <c r="AS5" s="49"/>
-      <c r="AT5" s="49"/>
-      <c r="AU5" s="49"/>
+      <c r="AK5" s="52"/>
+      <c r="AL5" s="52"/>
+      <c r="AM5" s="52"/>
+      <c r="AN5" s="52"/>
+      <c r="AO5" s="52"/>
+      <c r="AP5" s="52"/>
+      <c r="AQ5" s="52"/>
+      <c r="AR5" s="52"/>
+      <c r="AS5" s="52"/>
+      <c r="AT5" s="52"/>
+      <c r="AU5" s="52"/>
       <c r="AV5" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="AW5" s="36" t="s">
+      <c r="AW5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="AX5" s="37"/>
-      <c r="AY5" s="37"/>
-      <c r="AZ5" s="37"/>
-      <c r="BA5" s="37"/>
-      <c r="BB5" s="37"/>
-      <c r="BC5" s="37"/>
-      <c r="BD5" s="37"/>
-      <c r="BE5" s="37"/>
-      <c r="BF5" s="37"/>
-      <c r="BG5" s="37"/>
-      <c r="BH5" s="37"/>
-      <c r="BI5" s="37"/>
-      <c r="BJ5" s="37"/>
+      <c r="AX5" s="40"/>
+      <c r="AY5" s="40"/>
+      <c r="AZ5" s="40"/>
+      <c r="BA5" s="40"/>
+      <c r="BB5" s="40"/>
+      <c r="BC5" s="40"/>
+      <c r="BD5" s="40"/>
+      <c r="BE5" s="40"/>
+      <c r="BF5" s="40"/>
+      <c r="BG5" s="40"/>
+      <c r="BH5" s="40"/>
+      <c r="BI5" s="40"/>
+      <c r="BJ5" s="40"/>
       <c r="BK5" s="29"/>
     </row>
     <row r="6" spans="1:65" ht="62" x14ac:dyDescent="0.35">
@@ -2515,177 +2467,6 @@
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.35">
       <c r="AV9" s="17"/>
-    </row>
-    <row r="1048519" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="43:43" x14ac:dyDescent="0.35">
-      <c r="AQ1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2707,13 +2488,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1048573"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2735,17 +2516,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.5">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="28"/>
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
@@ -2774,28 +2555,28 @@
       <c r="Q2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="48" t="s">
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="53"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="56"/>
     </row>
     <row r="4" spans="1:26" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
@@ -2855,177 +2636,6 @@
       <c r="S4" s="20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="1048517" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048517" s="13"/>
-    </row>
-    <row r="1048518" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048518" s="13"/>
-    </row>
-    <row r="1048519" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="15:15" x14ac:dyDescent="0.35">
-      <c r="O1048573" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3044,18 +2654,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D773A1D3-FC14-4EA4-B569-35CAE3B3E4FA}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.08203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.4140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.9140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.25" style="33" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3063,10 +2671,10 @@
       <c r="B1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="24" t="s">
@@ -3075,16 +2683,16 @@
       <c r="B3" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="32" t="s">
         <v>84</v>
       </c>
       <c r="G3" t="s">
@@ -3096,10 +2704,10 @@
         <v>68</v>
       </c>
       <c r="B4" s="26"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -3107,10 +2715,10 @@
         <v>69</v>
       </c>
       <c r="B5" s="26"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="25"/>
     </row>
   </sheetData>

</xml_diff>